<commit_message>
Actualización de archivos JSON y scripts 31  de octubre
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -10,7 +10,7 @@
     <sheet state="hidden" name="pruebas i" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'EN PROCESO (Colmedica)'!$A$1:$Q$36</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'EN PROCESO (Colmedica)'!$A$1:$Q$38</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'PRUEBAS BOLIVAR'!$A$1:$L$16</definedName>
   </definedNames>
   <calcPr/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="251">
   <si>
     <t>Asignado a</t>
   </si>
@@ -216,7 +216,10 @@
     <t>EN PROCESO</t>
   </si>
   <si>
-    <t>1/10/2025 se prepara el query con el que se debe entregar la información al cliente, y crear una opción por el navegador que permita descargar dicha data</t>
+    <t>1/10/2025 se prepara el query con el que se debe entregar la información al cliente, y crear una opción por el navegador que permita descargar dicha data
+3/10/2025 ya disponible la opción nueva y asignar los permisos al rol necesario y inicio gestion para descargar la información
+6/10/2025 
+7/10/2025</t>
   </si>
   <si>
     <t>WebService Afiliacion PBS - Afiliaciones POS</t>
@@ -607,10 +610,31 @@
 10/10/2025 se pasa a produccion las opciones de subida de los archivos y las de validación para la acreditacipn, junto con la creacion del campo nuevo en la tabla de afiliadospos</t>
   </si>
   <si>
+    <t>OPT_16</t>
+  </si>
+  <si>
     <t>Afiliaciones Pos - Menores Duplicados - RC-CN</t>
   </si>
   <si>
     <t>Control de menores Recien Nacido - Registro Civil duplicados, identificación dentro de contratos diferentes por misma fecha de nacimiento, primer apellido CN es igual al segunto apellido del RC, crear reporte semanal para poder validarlos</t>
+  </si>
+  <si>
+    <t>Afiliaciones Pre - Base datos Inclusiones diarias Cargue</t>
+  </si>
+  <si>
+    <t>sea remitir una base diaria de las solicitudes de inclusiones con los datos de residencia y correspondencia del contratante, para poder actualizarlos en Apolo.</t>
+  </si>
+  <si>
+    <t>31/10/2025 Se inicia creando el query para extraer la información que se necesita reportar, y se envía muestra al cliente para que confirme si así estaria bien la entrega</t>
+  </si>
+  <si>
+    <t>OPT_17</t>
+  </si>
+  <si>
+    <t>Clasificacion Tributaria</t>
+  </si>
+  <si>
+    <t>Captura de información o datos básico de documento Perfil tributario desde la radicación desde el módulo de convenios médicos, y que alimente lo de clasificacion tributaria</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -2438,7 +2462,7 @@
       <c r="AL1" s="4"/>
       <c r="AM1" s="4"/>
     </row>
-    <row r="2" ht="53.25" customHeight="1">
+    <row r="2" ht="53.25" hidden="1" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>17</v>
       </c>
@@ -2512,7 +2536,7 @@
       <c r="AL2" s="27"/>
       <c r="AM2" s="27"/>
     </row>
-    <row r="3" ht="53.25" customHeight="1">
+    <row r="3" ht="53.25" hidden="1" customHeight="1">
       <c r="A3" s="28" t="s">
         <v>17</v>
       </c>
@@ -2586,7 +2610,7 @@
       <c r="AL3" s="42"/>
       <c r="AM3" s="42"/>
     </row>
-    <row r="4" ht="53.25" customHeight="1">
+    <row r="4" ht="53.25" hidden="1" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>17</v>
       </c>
@@ -2660,7 +2684,7 @@
       <c r="AL4" s="27"/>
       <c r="AM4" s="27"/>
     </row>
-    <row r="5" ht="53.25" customHeight="1">
+    <row r="5" ht="53.25" hidden="1" customHeight="1">
       <c r="A5" s="28" t="s">
         <v>17</v>
       </c>
@@ -2732,7 +2756,7 @@
       <c r="AL5" s="42"/>
       <c r="AM5" s="42"/>
     </row>
-    <row r="6" ht="53.25" customHeight="1">
+    <row r="6" ht="53.25" hidden="1" customHeight="1">
       <c r="A6" s="13" t="s">
         <v>17</v>
       </c>
@@ -2835,7 +2859,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f>IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32812</v>
+        <v>32814</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -2899,7 +2923,7 @@
       <c r="L8" s="23"/>
       <c r="M8" s="24">
         <f>IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
@@ -2932,7 +2956,7 @@
       <c r="AL8" s="27"/>
       <c r="AM8" s="27"/>
     </row>
-    <row r="9" ht="53.25" customHeight="1">
+    <row r="9" ht="53.25" hidden="1" customHeight="1">
       <c r="A9" s="28" t="s">
         <v>17</v>
       </c>
@@ -3004,7 +3028,7 @@
       <c r="AL9" s="42"/>
       <c r="AM9" s="42"/>
     </row>
-    <row r="10" ht="53.25" customHeight="1">
+    <row r="10" ht="53.25" hidden="1" customHeight="1">
       <c r="A10" s="13" t="s">
         <v>17</v>
       </c>
@@ -3076,7 +3100,7 @@
       <c r="AL10" s="27"/>
       <c r="AM10" s="27"/>
     </row>
-    <row r="11" ht="53.25" customHeight="1">
+    <row r="11" ht="53.25" hidden="1" customHeight="1">
       <c r="A11" s="28" t="s">
         <v>17</v>
       </c>
@@ -3150,7 +3174,7 @@
       <c r="AL11" s="42"/>
       <c r="AM11" s="42"/>
     </row>
-    <row r="12">
+    <row r="12" hidden="1">
       <c r="A12" s="13" t="s">
         <v>17</v>
       </c>
@@ -3183,7 +3207,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f>IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3218,7 +3242,7 @@
       <c r="AL12" s="27"/>
       <c r="AM12" s="27"/>
     </row>
-    <row r="13">
+    <row r="13" hidden="1">
       <c r="A13" s="28" t="s">
         <v>36</v>
       </c>
@@ -3290,7 +3314,7 @@
       <c r="AL13" s="42"/>
       <c r="AM13" s="42"/>
     </row>
-    <row r="14">
+    <row r="14" hidden="1">
       <c r="A14" s="13" t="s">
         <v>36</v>
       </c>
@@ -3362,7 +3386,7 @@
       <c r="AL14" s="27"/>
       <c r="AM14" s="27"/>
     </row>
-    <row r="15">
+    <row r="15" hidden="1">
       <c r="A15" s="28" t="s">
         <v>36</v>
       </c>
@@ -3434,7 +3458,7 @@
       <c r="AL15" s="42"/>
       <c r="AM15" s="42"/>
     </row>
-    <row r="16">
+    <row r="16" hidden="1">
       <c r="A16" s="13" t="s">
         <v>17</v>
       </c>
@@ -3461,7 +3485,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f>IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32812</v>
+        <v>32814</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -3494,7 +3518,7 @@
       <c r="AL16" s="27"/>
       <c r="AM16" s="27"/>
     </row>
-    <row r="17">
+    <row r="17" hidden="1">
       <c r="A17" s="28" t="s">
         <v>17</v>
       </c>
@@ -3568,7 +3592,7 @@
       <c r="AL17" s="42"/>
       <c r="AM17" s="42"/>
     </row>
-    <row r="18">
+    <row r="18" hidden="1">
       <c r="A18" s="13" t="s">
         <v>17</v>
       </c>
@@ -3642,7 +3666,7 @@
       <c r="AL18" s="27"/>
       <c r="AM18" s="27"/>
     </row>
-    <row r="19">
+    <row r="19" hidden="1">
       <c r="A19" s="28" t="s">
         <v>17</v>
       </c>
@@ -3712,7 +3736,7 @@
       <c r="AL19" s="42"/>
       <c r="AM19" s="42"/>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c r="A20" s="13" t="s">
         <v>17</v>
       </c>
@@ -3784,7 +3808,7 @@
       <c r="AL20" s="27"/>
       <c r="AM20" s="27"/>
     </row>
-    <row r="21" ht="59.25" customHeight="1">
+    <row r="21" ht="59.25" hidden="1" customHeight="1">
       <c r="A21" s="28" t="s">
         <v>36</v>
       </c>
@@ -3887,7 +3911,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f>IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -3920,7 +3944,7 @@
       <c r="AL22" s="27"/>
       <c r="AM22" s="27"/>
     </row>
-    <row r="23">
+    <row r="23" hidden="1">
       <c r="A23" s="28" t="s">
         <v>36</v>
       </c>
@@ -3994,7 +4018,7 @@
       <c r="AL23" s="42"/>
       <c r="AM23" s="42"/>
     </row>
-    <row r="24" ht="49.5" customHeight="1">
+    <row r="24" ht="49.5" hidden="1" customHeight="1">
       <c r="A24" s="13" t="s">
         <v>17</v>
       </c>
@@ -4027,7 +4051,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f>IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4060,7 +4084,7 @@
       <c r="AL24" s="27"/>
       <c r="AM24" s="27"/>
     </row>
-    <row r="25">
+    <row r="25" hidden="1">
       <c r="A25" s="28" t="s">
         <v>17</v>
       </c>
@@ -4134,7 +4158,7 @@
       <c r="AL25" s="42"/>
       <c r="AM25" s="42"/>
     </row>
-    <row r="26">
+    <row r="26" hidden="1">
       <c r="A26" s="13" t="s">
         <v>17</v>
       </c>
@@ -4159,7 +4183,7 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f>IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32812</v>
+        <v>32814</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
@@ -4190,7 +4214,7 @@
       <c r="AL26" s="27"/>
       <c r="AM26" s="27"/>
     </row>
-    <row r="27">
+    <row r="27" hidden="1">
       <c r="A27" s="28" t="s">
         <v>17</v>
       </c>
@@ -4262,7 +4286,7 @@
       <c r="AL27" s="42"/>
       <c r="AM27" s="42"/>
     </row>
-    <row r="28">
+    <row r="28" hidden="1">
       <c r="A28" s="13" t="s">
         <v>17</v>
       </c>
@@ -4297,7 +4321,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f>IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
@@ -4330,7 +4354,7 @@
       <c r="AL28" s="27"/>
       <c r="AM28" s="27"/>
     </row>
-    <row r="29">
+    <row r="29" hidden="1">
       <c r="A29" s="28" t="s">
         <v>17</v>
       </c>
@@ -4404,7 +4428,7 @@
       <c r="AL29" s="42"/>
       <c r="AM29" s="42"/>
     </row>
-    <row r="30">
+    <row r="30" hidden="1">
       <c r="A30" s="13" t="s">
         <v>17</v>
       </c>
@@ -4478,7 +4502,7 @@
       <c r="AL30" s="27"/>
       <c r="AM30" s="27"/>
     </row>
-    <row r="31">
+    <row r="31" hidden="1">
       <c r="A31" s="28" t="s">
         <v>36</v>
       </c>
@@ -4552,7 +4576,7 @@
       <c r="AL31" s="42"/>
       <c r="AM31" s="42"/>
     </row>
-    <row r="32">
+    <row r="32" hidden="1">
       <c r="A32" s="13" t="s">
         <v>36</v>
       </c>
@@ -4626,7 +4650,7 @@
       <c r="AL32" s="27"/>
       <c r="AM32" s="27"/>
     </row>
-    <row r="33">
+    <row r="33" hidden="1">
       <c r="A33" s="28" t="s">
         <v>17</v>
       </c>
@@ -4700,7 +4724,7 @@
       <c r="AL33" s="42"/>
       <c r="AM33" s="42"/>
     </row>
-    <row r="34">
+    <row r="34" hidden="1">
       <c r="A34" s="13" t="s">
         <v>17</v>
       </c>
@@ -4735,7 +4759,7 @@
       <c r="L34" s="23"/>
       <c r="M34" s="24">
         <f>IF(ISBLANK(L34), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L34, Hoja2!$A$1:$A$18))</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
@@ -4768,7 +4792,7 @@
       <c r="AL34" s="27"/>
       <c r="AM34" s="27"/>
     </row>
-    <row r="35">
+    <row r="35" hidden="1">
       <c r="A35" s="28" t="s">
         <v>36</v>
       </c>
@@ -4801,7 +4825,7 @@
       <c r="L35" s="38"/>
       <c r="M35" s="39">
         <f>IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N35" s="38">
         <v>45938.0</v>
@@ -4839,30 +4863,40 @@
       <c r="AM35" s="47"/>
     </row>
     <row r="36">
-      <c r="A36" s="13"/>
-      <c r="B36" s="14"/>
+      <c r="A36" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>143</v>
+      </c>
       <c r="C36" s="15" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E36" s="17"/>
       <c r="F36" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G36" s="19"/>
+      <c r="G36" s="19">
+        <v>0.0</v>
+      </c>
       <c r="H36" s="20"/>
-      <c r="I36" s="21"/>
+      <c r="I36" s="21">
+        <v>45954.0</v>
+      </c>
       <c r="J36" s="22"/>
-      <c r="K36" s="23"/>
+      <c r="K36" s="23">
+        <v>45968.0</v>
+      </c>
       <c r="L36" s="23"/>
       <c r="M36" s="24"/>
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
       <c r="P36" s="25"/>
       <c r="Q36" s="26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R36" s="48"/>
       <c r="S36" s="48"/>
@@ -4888,23 +4922,45 @@
       <c r="AM36" s="49"/>
     </row>
     <row r="37">
-      <c r="A37" s="28"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="31"/>
+      <c r="A37" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>147</v>
+      </c>
       <c r="E37" s="32"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="34"/>
+      <c r="F37" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" s="34">
+        <v>0.0</v>
+      </c>
       <c r="H37" s="35"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="38"/>
+      <c r="I37" s="36">
+        <v>45960.0</v>
+      </c>
+      <c r="J37" s="37">
+        <v>45961.0</v>
+      </c>
+      <c r="K37" s="38">
+        <v>45966.0</v>
+      </c>
       <c r="L37" s="38"/>
       <c r="M37" s="39"/>
       <c r="N37" s="38"/>
       <c r="O37" s="38"/>
-      <c r="P37" s="40"/>
-      <c r="Q37" s="41"/>
+      <c r="P37" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q37" s="41" t="b">
+        <v>1</v>
+      </c>
       <c r="R37" s="46"/>
       <c r="S37" s="46"/>
       <c r="T37" s="46"/>
@@ -4929,15 +4985,29 @@
       <c r="AM37" s="47"/>
     </row>
     <row r="38">
-      <c r="A38" s="13"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="16"/>
+      <c r="A38" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>151</v>
+      </c>
       <c r="E38" s="17"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="19"/>
+      <c r="F38" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="19">
+        <v>0.0</v>
+      </c>
       <c r="H38" s="20"/>
-      <c r="I38" s="21"/>
+      <c r="I38" s="21">
+        <v>45957.0</v>
+      </c>
       <c r="J38" s="22"/>
       <c r="K38" s="23"/>
       <c r="L38" s="23"/>
@@ -4945,7 +5015,9 @@
       <c r="N38" s="23"/>
       <c r="O38" s="23"/>
       <c r="P38" s="25"/>
-      <c r="Q38" s="26"/>
+      <c r="Q38" s="26" t="b">
+        <v>1</v>
+      </c>
       <c r="R38" s="48"/>
       <c r="S38" s="48"/>
       <c r="T38" s="48"/>
@@ -41952,7 +42024,21 @@
       <c r="AM940" s="85"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$Q$36"/>
+  <autoFilter ref="$A$1:$Q$38">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="JENNIFER"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="PENDIENTE"/>
+        <filter val="EN PROCESO"/>
+        <filter val="PRUEBAS CLIENTE"/>
+        <filter val="PAUSADO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="B2:B42">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF(B$2:B$16,B2)&gt;1</formula>
@@ -42001,7 +42087,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="86" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B1" s="86" t="s">
         <v>2</v>
@@ -42028,13 +42114,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="89" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="K1" s="86" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="L1" s="90" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="M1" s="91"/>
       <c r="N1" s="91"/>
@@ -42053,14 +42139,14 @@
     </row>
     <row r="2">
       <c r="A2" s="92" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B2" s="93" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C2" s="94"/>
       <c r="D2" s="95" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E2" s="96">
         <v>45526.0</v>
@@ -42074,7 +42160,7 @@
       <c r="J2" s="94"/>
       <c r="K2" s="94"/>
       <c r="L2" s="94" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="M2" s="97"/>
       <c r="N2" s="97"/>
@@ -42093,13 +42179,13 @@
     </row>
     <row r="3">
       <c r="A3" s="98" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C3" s="100" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="D3" s="100" t="s">
         <v>20</v>
@@ -42123,7 +42209,7 @@
       </c>
       <c r="K3" s="102"/>
       <c r="L3" s="104" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="M3" s="91"/>
       <c r="N3" s="91"/>
@@ -42142,16 +42228,16 @@
     </row>
     <row r="4">
       <c r="A4" s="105" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C4" s="105" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="D4" s="107" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E4" s="108">
         <v>45581.0</v>
@@ -42174,7 +42260,7 @@
       </c>
       <c r="K4" s="108"/>
       <c r="L4" s="105" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="M4" s="111"/>
       <c r="N4" s="111"/>
@@ -42193,16 +42279,16 @@
     </row>
     <row r="5">
       <c r="A5" s="90" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D5" s="112" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E5" s="101">
         <v>45572.0</v>
@@ -42223,7 +42309,7 @@
       </c>
       <c r="K5" s="101"/>
       <c r="L5" s="104" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="M5" s="91"/>
       <c r="N5" s="91"/>
@@ -42242,16 +42328,16 @@
     </row>
     <row r="6">
       <c r="A6" s="113" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B6" s="113" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C6" s="107" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D6" s="113" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E6" s="114">
         <v>45602.0</v>
@@ -42272,7 +42358,7 @@
         <v>45602.0</v>
       </c>
       <c r="L6" s="115" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="M6" s="116"/>
       <c r="N6" s="117"/>
@@ -42291,16 +42377,16 @@
     </row>
     <row r="7">
       <c r="A7" s="90" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C7" s="118" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="112" t="s">
         <v>170</v>
-      </c>
-      <c r="D7" s="112" t="s">
-        <v>163</v>
       </c>
       <c r="E7" s="101">
         <v>45589.0</v>
@@ -42321,7 +42407,7 @@
       </c>
       <c r="K7" s="112"/>
       <c r="L7" s="120" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="M7" s="121"/>
       <c r="N7" s="121"/>
@@ -42340,14 +42426,14 @@
     </row>
     <row r="8">
       <c r="A8" s="122" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B8" s="123" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="C8" s="124"/>
       <c r="D8" s="124" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="E8" s="125">
         <v>45603.0</v>
@@ -42368,7 +42454,7 @@
       </c>
       <c r="K8" s="125"/>
       <c r="L8" s="127" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="M8" s="91"/>
       <c r="N8" s="91"/>
@@ -42387,16 +42473,16 @@
     </row>
     <row r="9">
       <c r="A9" s="128" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B9" s="129" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C9" s="130" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D9" s="131" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E9" s="132">
         <v>45671.0</v>
@@ -42405,7 +42491,7 @@
         <v>45673.0</v>
       </c>
       <c r="G9" s="130" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="H9" s="132">
         <v>45680.0</v>
@@ -42419,7 +42505,7 @@
       </c>
       <c r="K9" s="130"/>
       <c r="L9" s="134" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="M9" s="135"/>
       <c r="N9" s="135"/>
@@ -42438,14 +42524,14 @@
     </row>
     <row r="10">
       <c r="A10" s="128" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B10" s="136"/>
       <c r="C10" s="134" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="D10" s="131" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E10" s="132">
         <v>45671.0</v>
@@ -42464,7 +42550,7 @@
       <c r="J10" s="130"/>
       <c r="K10" s="130"/>
       <c r="L10" s="134" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="M10" s="135"/>
       <c r="N10" s="135"/>
@@ -42483,14 +42569,14 @@
     </row>
     <row r="11">
       <c r="A11" s="128" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B11" s="136"/>
       <c r="C11" s="134" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="D11" s="131" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E11" s="132">
         <v>45671.0</v>
@@ -42509,7 +42595,7 @@
       <c r="J11" s="130"/>
       <c r="K11" s="130"/>
       <c r="L11" s="134" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="M11" s="135"/>
       <c r="N11" s="135"/>
@@ -42528,14 +42614,14 @@
     </row>
     <row r="12">
       <c r="A12" s="128" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B12" s="136"/>
       <c r="C12" s="134" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="D12" s="131" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E12" s="132">
         <v>45671.0</v>
@@ -42554,7 +42640,7 @@
       <c r="J12" s="130"/>
       <c r="K12" s="130"/>
       <c r="L12" s="134" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="M12" s="135"/>
       <c r="N12" s="135"/>
@@ -42573,14 +42659,14 @@
     </row>
     <row r="13">
       <c r="A13" s="128" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B13" s="136"/>
       <c r="C13" s="134" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="131" t="s">
         <v>185</v>
-      </c>
-      <c r="D13" s="131" t="s">
-        <v>178</v>
       </c>
       <c r="E13" s="132">
         <v>45671.0</v>
@@ -42599,7 +42685,7 @@
       <c r="J13" s="130"/>
       <c r="K13" s="130"/>
       <c r="L13" s="134" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="M13" s="135"/>
       <c r="N13" s="135"/>
@@ -42618,14 +42704,14 @@
     </row>
     <row r="14">
       <c r="A14" s="128" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B14" s="136"/>
       <c r="C14" s="134" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="D14" s="131" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E14" s="132">
         <v>45671.0</v>
@@ -42644,7 +42730,7 @@
       <c r="J14" s="130"/>
       <c r="K14" s="130"/>
       <c r="L14" s="130" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="M14" s="135"/>
       <c r="N14" s="135"/>
@@ -42663,14 +42749,14 @@
     </row>
     <row r="15">
       <c r="A15" s="128" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B15" s="136"/>
       <c r="C15" s="134" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="D15" s="131" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E15" s="132">
         <v>45671.0</v>
@@ -42689,7 +42775,7 @@
       <c r="J15" s="130"/>
       <c r="K15" s="130"/>
       <c r="L15" s="130" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="M15" s="135"/>
       <c r="N15" s="135"/>
@@ -42708,14 +42794,14 @@
     </row>
     <row r="16">
       <c r="A16" s="128" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B16" s="137"/>
       <c r="C16" s="138" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="D16" s="131" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E16" s="132">
         <v>45681.0</v>
@@ -42734,7 +42820,7 @@
       <c r="J16" s="130"/>
       <c r="K16" s="130"/>
       <c r="L16" s="134" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="M16" s="135"/>
       <c r="N16" s="135"/>
@@ -49270,7 +49356,7 @@
         <v>45292.0</v>
       </c>
       <c r="B1" s="135" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -49278,7 +49364,7 @@
         <v>45299.0</v>
       </c>
       <c r="B2" s="135" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -49286,7 +49372,7 @@
         <v>45376.0</v>
       </c>
       <c r="B3" s="135" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -49294,7 +49380,7 @@
         <v>45379.0</v>
       </c>
       <c r="B4" s="135" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -49302,7 +49388,7 @@
         <v>45380.0</v>
       </c>
       <c r="B5" s="135" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -49310,7 +49396,7 @@
         <v>45413.0</v>
       </c>
       <c r="B6" s="135" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -49318,7 +49404,7 @@
         <v>45425.0</v>
       </c>
       <c r="B7" s="135" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -49326,7 +49412,7 @@
         <v>45446.0</v>
       </c>
       <c r="B8" s="135" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -49334,7 +49420,7 @@
         <v>45453.0</v>
       </c>
       <c r="B9" s="135" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -49342,7 +49428,7 @@
         <v>45474.0</v>
       </c>
       <c r="B10" s="135" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -49350,7 +49436,7 @@
         <v>45493.0</v>
       </c>
       <c r="B11" s="135" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -49358,7 +49444,7 @@
         <v>45511.0</v>
       </c>
       <c r="B12" s="135" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1">
@@ -49366,7 +49452,7 @@
         <v>45523.0</v>
       </c>
       <c r="B13" s="135" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1">
@@ -49374,7 +49460,7 @@
         <v>45579.0</v>
       </c>
       <c r="B14" s="135" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1">
@@ -49382,7 +49468,7 @@
         <v>45600.0</v>
       </c>
       <c r="B15" s="135" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
@@ -49390,7 +49476,7 @@
         <v>45607.0</v>
       </c>
       <c r="B16" s="135" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
@@ -49398,7 +49484,7 @@
         <v>45634.0</v>
       </c>
       <c r="B17" s="135" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1">
@@ -49406,7 +49492,7 @@
         <v>45651.0</v>
       </c>
       <c r="B18" s="135" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1"/>
@@ -50422,7 +50508,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="140" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="B1" s="135"/>
       <c r="C1" s="135"/>
@@ -50480,7 +50566,7 @@
     </row>
     <row r="3" ht="32.25" customHeight="1">
       <c r="A3" s="141" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="B3" s="142">
         <v>45596.0</v>
@@ -50773,261 +50859,261 @@
     </row>
     <row r="4" ht="30.75" customHeight="1">
       <c r="A4" s="145" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B4" s="146" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C4" s="147" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="H4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="I4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="J4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="K4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="L4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="M4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="N4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="O4" s="148" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="P4" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Q4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="R4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="S4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="T4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="U4" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="V4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="W4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="X4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Y4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Z4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AA4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AB4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AC4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AD4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AE4" s="150" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="AF4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AG4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AH4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AI4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AJ4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AK4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AL4" s="150" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="AM4" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AN4" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AO4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AP4" s="150" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="AQ4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AR4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AS4" s="150" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="AT4" s="151" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AU4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AV4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AW4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AX4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AY4" s="150" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="AZ4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BA4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BB4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BC4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BD4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BE4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BF4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BG4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BH4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BI4" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BJ4" s="150" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="BK4" s="149" t="s">
+        <v>225</v>
+      </c>
+      <c r="BL4" s="149" t="s">
+        <v>225</v>
+      </c>
+      <c r="BM4" s="149" t="s">
+        <v>225</v>
+      </c>
+      <c r="BN4" s="149" t="s">
+        <v>225</v>
+      </c>
+      <c r="BO4" s="149" t="s">
+        <v>225</v>
+      </c>
+      <c r="BP4" s="149" t="s">
+        <v>225</v>
+      </c>
+      <c r="BQ4" s="149" t="s">
+        <v>225</v>
+      </c>
+      <c r="BR4" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="BL4" s="149" t="s">
+      <c r="BS4" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="BM4" s="149" t="s">
+      <c r="BT4" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="BN4" s="149" t="s">
+      <c r="BU4" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="BO4" s="149" t="s">
+      <c r="BV4" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="BP4" s="149" t="s">
+      <c r="BW4" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="BQ4" s="149" t="s">
+      <c r="BX4" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="BR4" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="BS4" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="BT4" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="BU4" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="BV4" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="BW4" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="BX4" s="148" t="s">
-        <v>211</v>
-      </c>
       <c r="BY4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BZ4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CA4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CB4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CC4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CD4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CE4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CF4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CG4" s="148"/>
       <c r="CH4" s="148"/>
       <c r="CI4" s="150" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="CJ4" s="148"/>
       <c r="CK4" s="148"/>
@@ -51039,249 +51125,249 @@
       <c r="CQ4" s="148"/>
       <c r="CR4" s="148"/>
       <c r="CS4" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="145" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B5" s="146" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="H5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="I5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="J5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="K5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="L5" s="148" t="s">
+        <v>225</v>
+      </c>
+      <c r="M5" s="148" t="s">
+        <v>225</v>
+      </c>
+      <c r="N5" s="148" t="s">
+        <v>225</v>
+      </c>
+      <c r="O5" s="148" t="s">
+        <v>225</v>
+      </c>
+      <c r="P5" s="149" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q5" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="M5" s="148" t="s">
+      <c r="R5" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="N5" s="148" t="s">
+      <c r="S5" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="O5" s="148" t="s">
+      <c r="T5" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="P5" s="149" t="s">
+      <c r="U5" s="149" t="s">
         <v>218</v>
       </c>
-      <c r="Q5" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="R5" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="S5" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="T5" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="U5" s="149" t="s">
-        <v>211</v>
-      </c>
       <c r="V5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="W5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="X5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Y5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Z5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AA5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AB5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AC5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AD5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AE5" s="152"/>
       <c r="AF5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AG5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AH5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AI5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AJ5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AK5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AL5" s="152"/>
       <c r="AM5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AN5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AO5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AP5" s="152"/>
       <c r="AQ5" s="148" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="AR5" s="148" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="AS5" s="152"/>
       <c r="AT5" s="148" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="AU5" s="148" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="AV5" s="148" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="AW5" s="148" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="AX5" s="148" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="AY5" s="152"/>
       <c r="AZ5" s="148" t="s">
+        <v>225</v>
+      </c>
+      <c r="BA5" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="BA5" s="148" t="s">
-        <v>211</v>
-      </c>
       <c r="BB5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BC5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BD5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BE5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BF5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BG5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BH5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BI5" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BJ5" s="152"/>
       <c r="BK5" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BL5" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BM5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BN5" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BO5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BP5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BQ5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BR5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BS5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BT5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BU5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BV5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BW5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BX5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BY5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BZ5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CA5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CB5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CC5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CD5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CE5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CF5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CG5" s="148"/>
       <c r="CH5" s="148"/>
@@ -51296,249 +51382,249 @@
       <c r="CQ5" s="148"/>
       <c r="CR5" s="148"/>
       <c r="CS5" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="145" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B6" s="146" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="H6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="I6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="J6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="K6" s="153" t="s">
+        <v>227</v>
+      </c>
+      <c r="L6" s="148" t="s">
+        <v>218</v>
+      </c>
+      <c r="M6" s="148" t="s">
+        <v>218</v>
+      </c>
+      <c r="N6" s="148" t="s">
+        <v>218</v>
+      </c>
+      <c r="O6" s="148" t="s">
         <v>220</v>
       </c>
-      <c r="L6" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="M6" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="N6" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="O6" s="148" t="s">
-        <v>213</v>
-      </c>
       <c r="P6" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Q6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="R6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="S6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="T6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="U6" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="V6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="W6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="X6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Y6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Z6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AA6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AB6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AC6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AD6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AE6" s="152"/>
       <c r="AF6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AG6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AH6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AI6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AJ6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AK6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AL6" s="152"/>
       <c r="AM6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AN6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AO6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AP6" s="152"/>
       <c r="AQ6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AR6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AS6" s="152"/>
       <c r="AT6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AU6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AV6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AW6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AX6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AY6" s="152"/>
       <c r="AZ6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BA6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BB6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BC6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BD6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BE6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BF6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BG6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BH6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BI6" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BJ6" s="152"/>
       <c r="BK6" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BL6" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BM6" s="148" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="BN6" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BO6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BP6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BQ6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BR6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BS6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BT6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BU6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BV6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BW6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BX6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BY6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BZ6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CA6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CB6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CC6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CD6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CE6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CF6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CG6" s="148"/>
       <c r="CH6" s="148"/>
@@ -51553,198 +51639,198 @@
       <c r="CQ6" s="148"/>
       <c r="CR6" s="148"/>
       <c r="CS6" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="145" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="B7" s="146" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="H7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="I7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="J7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="K7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="L7" s="153" t="s">
+        <v>227</v>
+      </c>
+      <c r="M7" s="148" t="s">
+        <v>218</v>
+      </c>
+      <c r="N7" s="148" t="s">
+        <v>218</v>
+      </c>
+      <c r="O7" s="148" t="s">
         <v>220</v>
       </c>
-      <c r="M7" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="N7" s="148" t="s">
-        <v>211</v>
-      </c>
-      <c r="O7" s="148" t="s">
-        <v>213</v>
-      </c>
       <c r="P7" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Q7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="R7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="S7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="T7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="U7" s="149" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="V7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="W7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="X7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Y7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Z7" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AA7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AB7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AC7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AD7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AE7" s="152"/>
       <c r="AF7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AG7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AH7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AI7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AJ7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AK7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AL7" s="152"/>
       <c r="AM7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AN7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AO7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AP7" s="152"/>
       <c r="AQ7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AR7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AS7" s="152"/>
       <c r="AT7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AU7" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AV7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AW7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AX7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AY7" s="152"/>
       <c r="AZ7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BA7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BB7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BC7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BD7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BE7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BF7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BG7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BH7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BI7" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BJ7" s="152"/>
       <c r="BK7" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BL7" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BM7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BN7" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BO7" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BP7" s="148"/>
       <c r="BQ7" s="148"/>
@@ -51752,16 +51838,16 @@
       <c r="BS7" s="148"/>
       <c r="BT7" s="148"/>
       <c r="BU7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BV7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BW7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BX7" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BY7" s="148"/>
       <c r="BZ7" s="148"/>
@@ -51787,220 +51873,220 @@
     </row>
     <row r="8" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="145" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="B8" s="146" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="H8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="I8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="J8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="K8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="L8" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="M8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="N8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="O8" s="148" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="P8" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Q8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="R8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="S8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="T8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="U8" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="V8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="W8" s="148" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="X8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Y8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Z8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AA8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AB8" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AC8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AD8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AE8" s="152"/>
       <c r="AF8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AG8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AH8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AI8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AJ8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AK8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AL8" s="152"/>
       <c r="AM8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AN8" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AO8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AP8" s="152"/>
       <c r="AQ8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AR8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AS8" s="152"/>
       <c r="AT8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AU8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AV8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AW8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AX8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AY8" s="152"/>
       <c r="AZ8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BA8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BB8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BC8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BD8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BE8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BF8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BG8" s="148" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="BH8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BI8" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BJ8" s="152"/>
       <c r="BK8" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BL8" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BM8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BN8" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BO8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BP8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BQ8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BR8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BS8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BT8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BU8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BV8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BW8" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BX8" s="148" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="BY8" s="148"/>
       <c r="BZ8" s="148"/>
@@ -52026,244 +52112,244 @@
     </row>
     <row r="9">
       <c r="A9" s="145" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="B9" s="146" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="H9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="I9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="J9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="K9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="L9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="M9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="N9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="O9" s="153" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="P9" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Q9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="R9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="S9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="T9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="U9" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="V9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="W9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="X9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Y9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Z9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AA9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AB9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AC9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AD9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AE9" s="152"/>
       <c r="AF9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AG9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AH9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AI9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AJ9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AK9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AL9" s="152"/>
       <c r="AM9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AN9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AO9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AP9" s="152"/>
       <c r="AQ9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AR9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AS9" s="152"/>
       <c r="AT9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AU9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AV9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AW9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AX9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AY9" s="152"/>
       <c r="AZ9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BA9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BB9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BC9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BD9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BE9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BF9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BG9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BH9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BI9" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BJ9" s="152"/>
       <c r="BK9" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BL9" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BM9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BN9" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BO9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BP9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BQ9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BR9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BS9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BT9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BU9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BV9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BW9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BX9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BY9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BZ9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CA9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CB9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CC9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CD9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CE9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CF9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CG9" s="148"/>
       <c r="CH9" s="148"/>
@@ -52278,249 +52364,249 @@
       <c r="CQ9" s="148"/>
       <c r="CR9" s="148"/>
       <c r="CS9" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="145" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="B10" s="146" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="H10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="I10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="J10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="K10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="L10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="M10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="N10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="O10" s="148" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="P10" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="Q10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="R10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="S10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="T10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="U10" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="V10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="W10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="X10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Y10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Z10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AA10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AB10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AC10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AD10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AE10" s="152"/>
       <c r="AF10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AG10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AH10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AI10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AJ10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AK10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AL10" s="152"/>
       <c r="AM10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AN10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AO10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AP10" s="152"/>
       <c r="AQ10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AR10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AS10" s="152"/>
       <c r="AT10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AU10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AV10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AW10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AX10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AY10" s="152"/>
       <c r="AZ10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BA10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BB10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BC10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BD10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BE10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BF10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BG10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BH10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BI10" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BJ10" s="152"/>
       <c r="BK10" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BL10" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BM10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BN10" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BO10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BP10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BQ10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BR10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BS10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BT10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BU10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BV10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BW10" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BX10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BY10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BZ10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CA10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CB10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CC10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CD10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CE10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CF10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CG10" s="148"/>
       <c r="CH10" s="148"/>
@@ -52535,249 +52621,249 @@
       <c r="CQ10" s="148"/>
       <c r="CR10" s="148"/>
       <c r="CS10" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="145" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="B11" s="146" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="H11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="I11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="J11" s="148" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="K11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="L11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="M11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="N11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="O11" s="148" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="P11" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Q11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="R11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="S11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="T11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="U11" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="V11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="W11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="X11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Y11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Z11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AA11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AB11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AC11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AD11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AE11" s="152"/>
       <c r="AF11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AG11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AH11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AI11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AJ11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AK11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AL11" s="152"/>
       <c r="AM11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AN11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AO11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AP11" s="152"/>
       <c r="AQ11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AR11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AS11" s="152"/>
       <c r="AT11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AU11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AV11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AW11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AX11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AY11" s="152"/>
       <c r="AZ11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BA11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BB11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BC11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BD11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BE11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BF11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BG11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BH11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BI11" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BJ11" s="152"/>
       <c r="BK11" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BL11" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BM11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BN11" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BO11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BP11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BQ11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BR11" s="148" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="BS11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BT11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BU11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BV11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BW11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BX11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BY11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BZ11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CA11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CB11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="CC11" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="CD11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CE11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CF11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CG11" s="148"/>
       <c r="CH11" s="148"/>
@@ -52792,249 +52878,249 @@
       <c r="CQ11" s="148"/>
       <c r="CR11" s="148"/>
       <c r="CS11" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="145" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="B12" s="146" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="D12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="F12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="G12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="H12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="I12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="J12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="K12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="L12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="M12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="N12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="O12" s="148" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="P12" s="149" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="Q12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="R12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="S12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="T12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="U12" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="V12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="W12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="X12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="Y12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="Z12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AA12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AB12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AC12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AD12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AE12" s="152"/>
       <c r="AF12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AG12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AH12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AI12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AJ12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AK12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AL12" s="152"/>
       <c r="AM12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AN12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AO12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AP12" s="152"/>
       <c r="AQ12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AR12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AS12" s="152"/>
       <c r="AT12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AU12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AV12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AW12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AX12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AY12" s="152"/>
       <c r="AZ12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BA12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BB12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BC12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BD12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BE12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BF12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BG12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BH12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BI12" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BJ12" s="152"/>
       <c r="BK12" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BL12" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BM12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BN12" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BO12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BP12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BQ12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BR12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BS12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BT12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BU12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BV12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BW12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BX12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BY12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="BZ12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="CA12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="CB12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CC12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="CD12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="CE12" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CF12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="CG12" s="148"/>
       <c r="CH12" s="148"/>
@@ -53049,249 +53135,249 @@
       <c r="CQ12" s="148"/>
       <c r="CR12" s="148"/>
       <c r="CS12" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="145" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="B13" s="146" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="D13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="E13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="F13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="G13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="H13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="I13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="J13" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="K13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="L13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="M13" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="N13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="O13" s="148" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="P13" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="Q13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="R13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="S13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="T13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="U13" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="V13" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="W13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="X13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="Y13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="Z13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AA13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AB13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AC13" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AD13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AE13" s="154"/>
       <c r="AF13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AG13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AH13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AI13" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="AJ13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AK13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AL13" s="154"/>
       <c r="AM13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AN13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AO13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AP13" s="154"/>
       <c r="AQ13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AR13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AS13" s="154"/>
       <c r="AT13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AU13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AV13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AW13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AX13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="AY13" s="154"/>
       <c r="AZ13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BA13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BB13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BC13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BD13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BE13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BF13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BG13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BH13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BI13" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BJ13" s="154"/>
       <c r="BK13" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BL13" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BM13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BN13" s="149" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BO13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BP13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BQ13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BR13" s="148" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="BS13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BT13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BU13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BV13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BW13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BX13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BY13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="BZ13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="CA13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="CB13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="CC13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="CD13" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CE13" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CF13" s="148" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="CG13" s="148"/>
       <c r="CH13" s="148"/>
@@ -53306,7 +53392,7 @@
       <c r="CQ13" s="148"/>
       <c r="CR13" s="148"/>
       <c r="CS13" s="148" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54332,7 +54418,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="155" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B1" s="155" t="s">
         <v>2</v>
@@ -54359,13 +54445,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="159" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="K1" s="160" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="L1" s="158" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="M1" s="161"/>
       <c r="N1" s="161"/>
@@ -54384,10 +54470,10 @@
     </row>
     <row r="2">
       <c r="A2" s="162" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B2" s="163" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C2" s="164"/>
       <c r="D2" s="164" t="s">
@@ -54414,7 +54500,7 @@
       </c>
       <c r="K2" s="167"/>
       <c r="L2" s="168" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="M2" s="161"/>
       <c r="N2" s="161"/>
@@ -54433,13 +54519,13 @@
     </row>
     <row r="3">
       <c r="A3" s="162" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="B3" s="169" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C3" s="170" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="D3" s="164" t="s">
         <v>39</v>
@@ -54461,7 +54547,7 @@
       </c>
       <c r="K3" s="165"/>
       <c r="L3" s="168" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="M3" s="171"/>
       <c r="N3" s="161"/>
@@ -54480,11 +54566,11 @@
     </row>
     <row r="4">
       <c r="A4" s="162" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="B4" s="152"/>
       <c r="C4" s="172" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="D4" s="164" t="s">
         <v>39</v>
@@ -54506,7 +54592,7 @@
       </c>
       <c r="K4" s="173"/>
       <c r="L4" s="176" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="M4" s="171"/>
       <c r="N4" s="161"/>
@@ -54525,13 +54611,13 @@
     </row>
     <row r="5">
       <c r="A5" s="162" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="B5" s="158" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="C5" s="164" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="D5" s="164" t="s">
         <v>39</v>
@@ -54553,7 +54639,7 @@
       </c>
       <c r="K5" s="165"/>
       <c r="L5" s="168" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="M5" s="171"/>
       <c r="N5" s="161"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 10 de noviembre
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -627,7 +627,8 @@
     <t>Control de menores Recien Nacido - Registro Civil duplicados, identificación dentro de contratos diferentes por misma fecha de nacimiento, primer apellido CN es igual al segunto apellido del RC, crear reporte semanal para poder validarlos</t>
   </si>
   <si>
-    <t>7/11/2025 Se inica el desarrollo, definiendo el query base con el que se hará la comparación y busqueda de posibles duplicados</t>
+    <t xml:space="preserve">7/11/2025 Se inica el desarrollo, definiendo el query base con el que se hará la comparación y busqueda de posibles duplicados
+</t>
   </si>
   <si>
     <t>OPT_17</t>
@@ -641,7 +642,8 @@
   <si>
     <t>31/10/2025 Se inicia creando el query para extraer la información que se necesita reportar, y se envía muestra al cliente para que confirme si así estaria bien la entrega y continuar con el desarrollo
 4/11/2025 el cliente ya a prueba la estructura, y confirma que se debe hacer el reporte a Diario
-7/11/2025 se crea la pagina que se ejecutará a Diario, y se empieza el desarrollo para la exportación de la data y el envío del correo electrónico</t>
+7/11/2025 se crea la pagina que se ejecutará a Diario, y se empieza el desarrollo para la exportación de la data y el envío del correo electrónico
+10/11/2025 Se termina el desarrollo, se publica la página en pruebas y producción. Se programa tarea para el envío de la información a diario.</t>
   </si>
   <si>
     <t>OPT_18</t>
@@ -2410,9 +2412,9 @@
   </sheetPr>
   <dimension ref="A1:AM940"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2905,7 +2907,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32820</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -3255,7 +3257,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f ca="1">IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3533,7 +3535,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f ca="1">IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32820</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -3959,7 +3961,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f ca="1">IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -4099,7 +4101,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f ca="1">IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4231,7 +4233,7 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f ca="1">IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32819</v>
+        <v>32820</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
@@ -4369,7 +4371,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f ca="1">IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
@@ -4807,7 +4809,7 @@
       <c r="L34" s="23"/>
       <c r="M34" s="24">
         <f ca="1">IF(ISBLANK(L34), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L34, Hoja2!$A$1:$A$18))</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
@@ -4873,7 +4875,7 @@
       <c r="L35" s="38"/>
       <c r="M35" s="39">
         <f ca="1">IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N35" s="38">
         <v>45938</v>
@@ -4928,7 +4930,7 @@
         <v>115</v>
       </c>
       <c r="G36" s="19">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="21">
@@ -4943,7 +4945,7 @@
       <c r="L36" s="23"/>
       <c r="M36" s="24">
         <f ca="1">IF(ISBLANK(L36), NETWORKDAYS(J36, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J36, L36, Hoja2!$A$1:$A$18))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
@@ -4991,10 +4993,10 @@
       </c>
       <c r="E37" s="32"/>
       <c r="F37" s="33" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="G37" s="34">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H37" s="35"/>
       <c r="I37" s="36">
@@ -5009,10 +5011,14 @@
       <c r="L37" s="38"/>
       <c r="M37" s="39">
         <f ca="1">IF(ISBLANK(L37), NETWORKDAYS(J37, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J37, L37, Hoja2!$A$1:$A$18))</f>
-        <v>6</v>
-      </c>
-      <c r="N37" s="38"/>
-      <c r="O37" s="38"/>
+        <v>7</v>
+      </c>
+      <c r="N37" s="38">
+        <v>45971</v>
+      </c>
+      <c r="O37" s="38">
+        <v>45971</v>
+      </c>
       <c r="P37" s="40" t="s">
         <v>150</v>
       </c>
@@ -5073,7 +5079,7 @@
       <c r="L38" s="23"/>
       <c r="M38" s="24">
         <f ca="1">IF(ISBLANK(L38), NETWORKDAYS(J38, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J38, L38, Hoja2!$A$1:$A$18))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N38" s="23"/>
       <c r="O38" s="23"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 11 de noviembre
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -19,7 +19,7 @@
     <sheet name="pruebas i" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EN PROCESO (Colmedica)'!$A$1:$Q$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'EN PROCESO (Colmedica)'!$A$1:$Q$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'PRUEBAS BOLIVAR'!$A$1:$L$16</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="267">
   <si>
     <t>Asignado a</t>
   </si>
@@ -665,6 +665,30 @@
   </si>
   <si>
     <t>Una vez se cargue la base de correos de los colectivos enviados, se debe enviar dicha base de manera automática al equipo de manteniemento de colectivos del área de Fidelización</t>
+  </si>
+  <si>
+    <t>OPT_20</t>
+  </si>
+  <si>
+    <t>Afiliaciones Pre - Base datos usuarios menores sin datos de ubicación</t>
+  </si>
+  <si>
+    <t>envío de una base con la información “si en la solicitud de ingreso los menores de edad vienen con los campos vacíos o en cero en dirección de residencia, teléfono residencia, ciudad, email y celular, se replique la información del contratante y se carguen con los mismos datos. Esto solo para menores de edad y solo si los campos no vienen diligenciados o vienen con dato cero “0”.” De manera semanal , todos los lunes</t>
+  </si>
+  <si>
+    <t>OPT_21</t>
+  </si>
+  <si>
+    <t>Afiliaciones Pre - Base datos usuarios mayores que traen los mismos datos de ubicacion del titular</t>
+  </si>
+  <si>
+    <t>envío de una base con la información “sobre los casos en los que los datos de afiliación de los beneficiarios mayores de edad presenten coincidencias en el correo electrónico y el número de teléfono. Este reporte tiene como objetivo identificar y analizar a los beneficiarios cuya información de contacto sea la misma.”. De manera mensual</t>
+  </si>
+  <si>
+    <t>OPT_22</t>
+  </si>
+  <si>
+    <t>Comercial - Error al guardar observación en el Reingreso</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -2412,9 +2436,9 @@
   </sheetPr>
   <dimension ref="A1:AM940"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2559,7 +2583,7 @@
         <v>21</v>
       </c>
       <c r="Q2" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R2" s="27"/>
       <c r="S2" s="27"/>
@@ -2633,7 +2657,7 @@
         <v>24</v>
       </c>
       <c r="Q3" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R3" s="42"/>
       <c r="S3" s="42"/>
@@ -2707,7 +2731,7 @@
         <v>28</v>
       </c>
       <c r="Q4" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
@@ -2779,7 +2803,7 @@
         <v>32</v>
       </c>
       <c r="Q5" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R5" s="42"/>
       <c r="S5" s="42"/>
@@ -2853,7 +2877,7 @@
         <v>35</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="27"/>
@@ -2907,7 +2931,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32820</v>
+        <v>32821</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -2915,7 +2939,7 @@
         <v>40</v>
       </c>
       <c r="Q7" s="41" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="R7" s="42"/>
       <c r="S7" s="42"/>
@@ -2981,7 +3005,7 @@
         <v>43</v>
       </c>
       <c r="Q8" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
@@ -3053,7 +3077,7 @@
         <v>46</v>
       </c>
       <c r="Q9" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R9" s="42"/>
       <c r="S9" s="42"/>
@@ -3125,7 +3149,7 @@
         <v>49</v>
       </c>
       <c r="Q10" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R10" s="27"/>
       <c r="S10" s="27"/>
@@ -3199,7 +3223,7 @@
         <v>53</v>
       </c>
       <c r="Q11" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R11" s="42"/>
       <c r="S11" s="42"/>
@@ -3257,7 +3281,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f ca="1">IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3267,7 +3291,7 @@
         <v>57</v>
       </c>
       <c r="Q12" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
@@ -3339,7 +3363,7 @@
         <v>61</v>
       </c>
       <c r="Q13" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R13" s="42"/>
       <c r="S13" s="42"/>
@@ -3411,7 +3435,7 @@
         <v>65</v>
       </c>
       <c r="Q14" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R14" s="27"/>
       <c r="S14" s="27"/>
@@ -3483,7 +3507,7 @@
         <v>69</v>
       </c>
       <c r="Q15" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R15" s="42"/>
       <c r="S15" s="42"/>
@@ -3535,7 +3559,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f ca="1">IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32820</v>
+        <v>32821</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -3543,7 +3567,7 @@
         <v>73</v>
       </c>
       <c r="Q16" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R16" s="27"/>
       <c r="S16" s="27"/>
@@ -3617,7 +3641,7 @@
         <v>76</v>
       </c>
       <c r="Q17" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R17" s="42"/>
       <c r="S17" s="42"/>
@@ -3691,7 +3715,7 @@
         <v>80</v>
       </c>
       <c r="Q18" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R18" s="27"/>
       <c r="S18" s="27"/>
@@ -3761,7 +3785,7 @@
         <v>83</v>
       </c>
       <c r="Q19" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R19" s="42"/>
       <c r="S19" s="42"/>
@@ -3833,7 +3857,7 @@
       </c>
       <c r="P20" s="25"/>
       <c r="Q20" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R20" s="27"/>
       <c r="S20" s="27"/>
@@ -3905,7 +3929,7 @@
         <v>89</v>
       </c>
       <c r="Q21" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R21" s="42"/>
       <c r="S21" s="42"/>
@@ -3961,7 +3985,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f ca="1">IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -3969,7 +3993,7 @@
         <v>94</v>
       </c>
       <c r="Q22" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R22" s="27"/>
       <c r="S22" s="27"/>
@@ -4043,7 +4067,7 @@
         <v>98</v>
       </c>
       <c r="Q23" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R23" s="42"/>
       <c r="S23" s="42"/>
@@ -4101,7 +4125,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f ca="1">IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4109,7 +4133,7 @@
         <v>102</v>
       </c>
       <c r="Q24" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R24" s="27"/>
       <c r="S24" s="27"/>
@@ -4183,7 +4207,7 @@
         <v>106</v>
       </c>
       <c r="Q25" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R25" s="42"/>
       <c r="S25" s="42"/>
@@ -4233,13 +4257,13 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f ca="1">IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32820</v>
+        <v>32821</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
       <c r="P26" s="25"/>
       <c r="Q26" s="26" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="R26" s="27"/>
       <c r="S26" s="27"/>
@@ -4311,7 +4335,7 @@
         <v>112</v>
       </c>
       <c r="Q27" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R27" s="42"/>
       <c r="S27" s="42"/>
@@ -4371,7 +4395,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f ca="1">IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
@@ -4379,7 +4403,7 @@
         <v>117</v>
       </c>
       <c r="Q28" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R28" s="27"/>
       <c r="S28" s="27"/>
@@ -4453,7 +4477,7 @@
         <v>120</v>
       </c>
       <c r="Q29" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R29" s="42"/>
       <c r="S29" s="42"/>
@@ -4527,7 +4551,7 @@
         <v>123</v>
       </c>
       <c r="Q30" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R30" s="27"/>
       <c r="S30" s="27"/>
@@ -4601,7 +4625,7 @@
         <v>127</v>
       </c>
       <c r="Q31" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R31" s="42"/>
       <c r="S31" s="42"/>
@@ -4675,7 +4699,7 @@
         <v>131</v>
       </c>
       <c r="Q32" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R32" s="27"/>
       <c r="S32" s="27"/>
@@ -4749,7 +4773,7 @@
         <v>135</v>
       </c>
       <c r="Q33" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R33" s="42"/>
       <c r="S33" s="42"/>
@@ -4809,7 +4833,7 @@
       <c r="L34" s="23"/>
       <c r="M34" s="24">
         <f ca="1">IF(ISBLANK(L34), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L34, Hoja2!$A$1:$A$18))</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
@@ -4817,7 +4841,7 @@
         <v>138</v>
       </c>
       <c r="Q34" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R34" s="27"/>
       <c r="S34" s="27"/>
@@ -4875,7 +4899,7 @@
       <c r="L35" s="38"/>
       <c r="M35" s="39">
         <f ca="1">IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N35" s="38">
         <v>45938</v>
@@ -4887,7 +4911,7 @@
         <v>142</v>
       </c>
       <c r="Q35" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R35" s="46"/>
       <c r="S35" s="46"/>
@@ -4945,7 +4969,7 @@
       <c r="L36" s="23"/>
       <c r="M36" s="24">
         <f ca="1">IF(ISBLANK(L36), NETWORKDAYS(J36, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J36, L36, Hoja2!$A$1:$A$18))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
@@ -4953,7 +4977,7 @@
         <v>146</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R36" s="48"/>
       <c r="S36" s="48"/>
@@ -5011,7 +5035,7 @@
       <c r="L37" s="38"/>
       <c r="M37" s="39">
         <f ca="1">IF(ISBLANK(L37), NETWORKDAYS(J37, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J37, L37, Hoja2!$A$1:$A$18))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N37" s="38">
         <v>45971</v>
@@ -5023,7 +5047,7 @@
         <v>150</v>
       </c>
       <c r="Q37" s="41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R37" s="46"/>
       <c r="S37" s="46"/>
@@ -5079,7 +5103,7 @@
       <c r="L38" s="23"/>
       <c r="M38" s="24">
         <f ca="1">IF(ISBLANK(L38), NETWORKDAYS(J38, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J38, L38, Hoja2!$A$1:$A$18))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N38" s="23"/>
       <c r="O38" s="23"/>
@@ -5087,7 +5111,7 @@
         <v>154</v>
       </c>
       <c r="Q38" s="26" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="R38" s="48"/>
       <c r="S38" s="48"/>
@@ -5146,7 +5170,7 @@
       <c r="O39" s="38"/>
       <c r="P39" s="40"/>
       <c r="Q39" s="41" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="R39" s="46"/>
       <c r="S39" s="46"/>
@@ -5171,24 +5195,42 @@
       <c r="AL39" s="46"/>
       <c r="AM39" s="47"/>
     </row>
-    <row r="40" spans="1:39">
-      <c r="A40" s="13"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="16"/>
+    <row r="40" spans="1:39" ht="63.75">
+      <c r="A40" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>160</v>
+      </c>
       <c r="E40" s="17"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="19"/>
+      <c r="F40" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="G40" s="19">
+        <v>35</v>
+      </c>
       <c r="H40" s="20"/>
-      <c r="I40" s="21"/>
+      <c r="I40" s="21">
+        <v>45968</v>
+      </c>
       <c r="J40" s="22"/>
-      <c r="K40" s="23"/>
+      <c r="K40" s="23">
+        <v>45974</v>
+      </c>
       <c r="L40" s="23"/>
       <c r="M40" s="24"/>
       <c r="N40" s="23"/>
       <c r="O40" s="23"/>
       <c r="P40" s="25"/>
-      <c r="Q40" s="26"/>
+      <c r="Q40" s="26" t="s">
+        <v>265</v>
+      </c>
       <c r="R40" s="48"/>
       <c r="S40" s="48"/>
       <c r="T40" s="48"/>
@@ -5212,24 +5254,42 @@
       <c r="AL40" s="48"/>
       <c r="AM40" s="49"/>
     </row>
-    <row r="41" spans="1:39">
-      <c r="A41" s="28"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="31"/>
+    <row r="41" spans="1:39" ht="71.25">
+      <c r="A41" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>163</v>
+      </c>
       <c r="E41" s="32"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="34"/>
+      <c r="F41" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="G41" s="34">
+        <v>35</v>
+      </c>
       <c r="H41" s="35"/>
-      <c r="I41" s="36"/>
+      <c r="I41" s="36">
+        <v>45968</v>
+      </c>
       <c r="J41" s="37"/>
-      <c r="K41" s="38"/>
+      <c r="K41" s="38">
+        <v>45974</v>
+      </c>
       <c r="L41" s="38"/>
       <c r="M41" s="39"/>
       <c r="N41" s="38"/>
       <c r="O41" s="38"/>
       <c r="P41" s="40"/>
-      <c r="Q41" s="41"/>
+      <c r="Q41" s="41" t="s">
+        <v>265</v>
+      </c>
       <c r="R41" s="46"/>
       <c r="S41" s="46"/>
       <c r="T41" s="46"/>
@@ -5253,16 +5313,28 @@
       <c r="AL41" s="46"/>
       <c r="AM41" s="47"/>
     </row>
-    <row r="42" spans="1:39">
-      <c r="A42" s="13"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="15"/>
+    <row r="42" spans="1:39" ht="42.75">
+      <c r="A42" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>165</v>
+      </c>
       <c r="D42" s="16"/>
       <c r="E42" s="17"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="19"/>
+      <c r="F42" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G42" s="19">
+        <v>0</v>
+      </c>
       <c r="H42" s="20"/>
-      <c r="I42" s="21"/>
+      <c r="I42" s="21">
+        <v>45972</v>
+      </c>
       <c r="J42" s="22"/>
       <c r="K42" s="23"/>
       <c r="L42" s="23"/>
@@ -42113,7 +42185,7 @@
       <c r="AM940" s="85"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q39"/>
+  <autoFilter ref="A1:Q42"/>
   <conditionalFormatting sqref="B2:B42">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF(B$2:B$16,B2)&gt;1</formula>
@@ -42160,7 +42232,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30">
       <c r="A1" s="86" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B1" s="86" t="s">
         <v>2</v>
@@ -42187,13 +42259,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="89" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="K1" s="86" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="L1" s="90" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="M1" s="91"/>
       <c r="N1" s="91"/>
@@ -42212,14 +42284,14 @@
     </row>
     <row r="2" spans="1:26" ht="30">
       <c r="A2" s="92" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B2" s="93" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="C2" s="94"/>
       <c r="D2" s="95" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="E2" s="96">
         <v>45526</v>
@@ -42233,7 +42305,7 @@
       <c r="J2" s="94"/>
       <c r="K2" s="94"/>
       <c r="L2" s="94" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="M2" s="97"/>
       <c r="N2" s="97"/>
@@ -42252,13 +42324,13 @@
     </row>
     <row r="3" spans="1:26" ht="28.5">
       <c r="A3" s="98" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C3" s="100" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D3" s="100" t="s">
         <v>20</v>
@@ -42282,7 +42354,7 @@
       </c>
       <c r="K3" s="102"/>
       <c r="L3" s="104" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="M3" s="91"/>
       <c r="N3" s="91"/>
@@ -42301,16 +42373,16 @@
     </row>
     <row r="4" spans="1:26" ht="186">
       <c r="A4" s="105" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="C4" s="105" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D4" s="107" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E4" s="108">
         <v>45581</v>
@@ -42333,7 +42405,7 @@
       </c>
       <c r="K4" s="108"/>
       <c r="L4" s="105" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="M4" s="111"/>
       <c r="N4" s="111"/>
@@ -42352,16 +42424,16 @@
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" s="90" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D5" s="112" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E5" s="101">
         <v>45572</v>
@@ -42382,7 +42454,7 @@
       </c>
       <c r="K5" s="101"/>
       <c r="L5" s="104" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="M5" s="91"/>
       <c r="N5" s="91"/>
@@ -42401,16 +42473,16 @@
     </row>
     <row r="6" spans="1:26" ht="117">
       <c r="A6" s="113" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B6" s="113" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C6" s="107" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="D6" s="113" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="E6" s="114">
         <v>45602</v>
@@ -42431,7 +42503,7 @@
         <v>45602</v>
       </c>
       <c r="L6" s="115" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="M6" s="116"/>
       <c r="N6" s="117"/>
@@ -42450,16 +42522,16 @@
     </row>
     <row r="7" spans="1:26" ht="99.75">
       <c r="A7" s="90" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C7" s="118" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D7" s="112" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E7" s="101">
         <v>45589</v>
@@ -42480,7 +42552,7 @@
       </c>
       <c r="K7" s="112"/>
       <c r="L7" s="120" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="M7" s="121"/>
       <c r="N7" s="121"/>
@@ -42499,14 +42571,14 @@
     </row>
     <row r="8" spans="1:26" ht="71.25">
       <c r="A8" s="122" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B8" s="123" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C8" s="124"/>
       <c r="D8" s="124" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="E8" s="125">
         <v>45603</v>
@@ -42527,7 +42599,7 @@
       </c>
       <c r="K8" s="125"/>
       <c r="L8" s="127" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="M8" s="91"/>
       <c r="N8" s="91"/>
@@ -42546,16 +42618,16 @@
     </row>
     <row r="9" spans="1:26" ht="42.75">
       <c r="A9" s="128" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B9" s="129" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="C9" s="130" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D9" s="131" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E9" s="132">
         <v>45671</v>
@@ -42564,7 +42636,7 @@
         <v>45673</v>
       </c>
       <c r="G9" s="130" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="H9" s="132">
         <v>45680</v>
@@ -42578,7 +42650,7 @@
       </c>
       <c r="K9" s="130"/>
       <c r="L9" s="134" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="M9" s="135"/>
       <c r="N9" s="135"/>
@@ -42597,14 +42669,14 @@
     </row>
     <row r="10" spans="1:26" ht="57">
       <c r="A10" s="128" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B10" s="136"/>
       <c r="C10" s="134" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D10" s="131" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E10" s="132">
         <v>45671</v>
@@ -42623,7 +42695,7 @@
       <c r="J10" s="130"/>
       <c r="K10" s="130"/>
       <c r="L10" s="134" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="M10" s="135"/>
       <c r="N10" s="135"/>
@@ -42642,14 +42714,14 @@
     </row>
     <row r="11" spans="1:26" ht="42.75">
       <c r="A11" s="128" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B11" s="136"/>
       <c r="C11" s="134" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D11" s="131" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E11" s="132">
         <v>45671</v>
@@ -42668,7 +42740,7 @@
       <c r="J11" s="130"/>
       <c r="K11" s="130"/>
       <c r="L11" s="134" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="M11" s="135"/>
       <c r="N11" s="135"/>
@@ -42687,14 +42759,14 @@
     </row>
     <row r="12" spans="1:26" ht="42.75">
       <c r="A12" s="128" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B12" s="136"/>
       <c r="C12" s="134" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="D12" s="131" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E12" s="132">
         <v>45671</v>
@@ -42713,7 +42785,7 @@
       <c r="J12" s="130"/>
       <c r="K12" s="130"/>
       <c r="L12" s="134" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="M12" s="135"/>
       <c r="N12" s="135"/>
@@ -42732,14 +42804,14 @@
     </row>
     <row r="13" spans="1:26" ht="42.75">
       <c r="A13" s="128" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B13" s="136"/>
       <c r="C13" s="134" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="D13" s="131" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E13" s="132">
         <v>45671</v>
@@ -42758,7 +42830,7 @@
       <c r="J13" s="130"/>
       <c r="K13" s="130"/>
       <c r="L13" s="134" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="M13" s="135"/>
       <c r="N13" s="135"/>
@@ -42777,14 +42849,14 @@
     </row>
     <row r="14" spans="1:26" ht="42.75">
       <c r="A14" s="128" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B14" s="136"/>
       <c r="C14" s="134" t="s">
+        <v>207</v>
+      </c>
+      <c r="D14" s="131" t="s">
         <v>199</v>
-      </c>
-      <c r="D14" s="131" t="s">
-        <v>191</v>
       </c>
       <c r="E14" s="132">
         <v>45671</v>
@@ -42803,7 +42875,7 @@
       <c r="J14" s="130"/>
       <c r="K14" s="130"/>
       <c r="L14" s="130" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="M14" s="135"/>
       <c r="N14" s="135"/>
@@ -42822,14 +42894,14 @@
     </row>
     <row r="15" spans="1:26" ht="42.75">
       <c r="A15" s="128" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B15" s="136"/>
       <c r="C15" s="134" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="D15" s="131" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E15" s="132">
         <v>45671</v>
@@ -42848,7 +42920,7 @@
       <c r="J15" s="130"/>
       <c r="K15" s="130"/>
       <c r="L15" s="130" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="M15" s="135"/>
       <c r="N15" s="135"/>
@@ -42867,14 +42939,14 @@
     </row>
     <row r="16" spans="1:26" ht="71.25">
       <c r="A16" s="128" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B16" s="137"/>
       <c r="C16" s="138" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="D16" s="131" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E16" s="132">
         <v>45681</v>
@@ -42893,7 +42965,7 @@
       <c r="J16" s="130"/>
       <c r="K16" s="130"/>
       <c r="L16" s="134" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="M16" s="135"/>
       <c r="N16" s="135"/>
@@ -49425,7 +49497,7 @@
         <v>45292</v>
       </c>
       <c r="B1" s="135" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
@@ -49433,7 +49505,7 @@
         <v>45299</v>
       </c>
       <c r="B2" s="135" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
@@ -49441,7 +49513,7 @@
         <v>45376</v>
       </c>
       <c r="B3" s="135" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
@@ -49449,7 +49521,7 @@
         <v>45379</v>
       </c>
       <c r="B4" s="135" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
@@ -49457,7 +49529,7 @@
         <v>45380</v>
       </c>
       <c r="B5" s="135" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1">
@@ -49465,7 +49537,7 @@
         <v>45413</v>
       </c>
       <c r="B6" s="135" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
@@ -49473,7 +49545,7 @@
         <v>45425</v>
       </c>
       <c r="B7" s="135" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
@@ -49481,7 +49553,7 @@
         <v>45446</v>
       </c>
       <c r="B8" s="135" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1">
@@ -49489,7 +49561,7 @@
         <v>45453</v>
       </c>
       <c r="B9" s="135" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1">
@@ -49497,7 +49569,7 @@
         <v>45474</v>
       </c>
       <c r="B10" s="135" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1">
@@ -49505,7 +49577,7 @@
         <v>45493</v>
       </c>
       <c r="B11" s="135" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" customHeight="1">
@@ -49513,7 +49585,7 @@
         <v>45511</v>
       </c>
       <c r="B12" s="135" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1">
@@ -49521,7 +49593,7 @@
         <v>45523</v>
       </c>
       <c r="B13" s="135" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" customHeight="1">
@@ -49529,7 +49601,7 @@
         <v>45579</v>
       </c>
       <c r="B14" s="135" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" customHeight="1">
@@ -49537,7 +49609,7 @@
         <v>45600</v>
       </c>
       <c r="B15" s="135" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1">
@@ -49545,7 +49617,7 @@
         <v>45607</v>
       </c>
       <c r="B16" s="135" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
@@ -49553,7 +49625,7 @@
         <v>45634</v>
       </c>
       <c r="B17" s="135" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1">
@@ -49561,7 +49633,7 @@
         <v>45651</v>
       </c>
       <c r="B18" s="135" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1"/>
@@ -50573,7 +50645,7 @@
   <sheetData>
     <row r="1" spans="1:97" ht="15.75">
       <c r="A1" s="140" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B1" s="135"/>
       <c r="C1" s="135"/>
@@ -50631,7 +50703,7 @@
     </row>
     <row r="3" spans="1:97" ht="32.25" customHeight="1">
       <c r="A3" s="141" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="B3" s="142">
         <v>45596</v>
@@ -50924,261 +50996,261 @@
     </row>
     <row r="4" spans="1:97" ht="30.75" customHeight="1">
       <c r="A4" s="145" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B4" s="146" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C4" s="147" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="D4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="G4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="H4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="I4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="K4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="L4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="M4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="N4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="O4" s="148" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="P4" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Q4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="R4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="S4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="T4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="U4" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="V4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="W4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="X4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Y4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Z4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AA4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AB4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AC4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AD4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AE4" s="174" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="AF4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AG4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AH4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AI4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AJ4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AK4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AL4" s="174" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="AM4" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AN4" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AO4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AP4" s="174" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="AQ4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AR4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AS4" s="174" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="AT4" s="150" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AU4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AV4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AW4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AX4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AY4" s="174" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="AZ4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BA4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BB4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BC4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BD4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BE4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BF4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BG4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BH4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BI4" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BJ4" s="174" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="BK4" s="149" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="BL4" s="149" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="BM4" s="149" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="BN4" s="149" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="BO4" s="149" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="BP4" s="149" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="BQ4" s="149" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="BR4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BS4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BT4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BU4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BV4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BW4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BX4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BY4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BZ4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CA4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CB4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CC4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CD4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CE4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CF4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CG4" s="148"/>
       <c r="CH4" s="148"/>
       <c r="CI4" s="174" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="CJ4" s="148"/>
       <c r="CK4" s="148"/>
@@ -51190,249 +51262,249 @@
       <c r="CQ4" s="148"/>
       <c r="CR4" s="148"/>
       <c r="CS4" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:97" ht="15.75" customHeight="1">
       <c r="A5" s="145" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B5" s="146" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="G5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="H5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="I5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="K5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="L5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="M5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="N5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="O5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="P5" s="149" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="Q5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="R5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="S5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="T5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="U5" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="V5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="W5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="X5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Y5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Z5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AA5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AB5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AC5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AD5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AE5" s="175"/>
       <c r="AF5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AG5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AH5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AI5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AJ5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AK5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AL5" s="175"/>
       <c r="AM5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AN5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AO5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AP5" s="175"/>
       <c r="AQ5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="AR5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="AS5" s="175"/>
       <c r="AT5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="AU5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="AV5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="AW5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="AX5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="AY5" s="175"/>
       <c r="AZ5" s="148" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="BA5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BB5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BC5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BD5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BE5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BF5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BG5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BH5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BI5" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BJ5" s="175"/>
       <c r="BK5" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BL5" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BM5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BN5" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BO5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BP5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BQ5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BR5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BS5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BT5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BU5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BV5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BW5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BX5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BY5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BZ5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CA5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CB5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CC5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CD5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CE5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CF5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CG5" s="148"/>
       <c r="CH5" s="148"/>
@@ -51447,249 +51519,249 @@
       <c r="CQ5" s="148"/>
       <c r="CR5" s="148"/>
       <c r="CS5" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:97" ht="15.75">
       <c r="A6" s="145" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B6" s="146" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="G6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="H6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="I6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="K6" s="151" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="L6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="M6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="N6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="O6" s="148" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="P6" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Q6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="R6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="S6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="T6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="U6" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="V6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="W6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="X6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Y6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Z6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AA6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AB6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AC6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AD6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AE6" s="175"/>
       <c r="AF6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AG6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AH6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AI6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AJ6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AK6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AL6" s="175"/>
       <c r="AM6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AN6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AO6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AP6" s="175"/>
       <c r="AQ6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AR6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AS6" s="175"/>
       <c r="AT6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AU6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AV6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AW6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AX6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AY6" s="175"/>
       <c r="AZ6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BA6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BB6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BC6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BD6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BE6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BF6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BG6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BH6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BI6" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BJ6" s="175"/>
       <c r="BK6" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BL6" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BM6" s="148" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="BN6" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BO6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BP6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BQ6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BR6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BS6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BT6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BU6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BV6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BW6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BX6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BY6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BZ6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CA6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CB6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CC6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CD6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CE6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CF6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CG6" s="148"/>
       <c r="CH6" s="148"/>
@@ -51704,198 +51776,198 @@
       <c r="CQ6" s="148"/>
       <c r="CR6" s="148"/>
       <c r="CS6" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="145" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="146" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="D7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="F7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="G7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="H7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="I7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="J7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="K7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="L7" s="151" t="s">
+        <v>241</v>
+      </c>
+      <c r="M7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="N7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="O7" s="148" t="s">
+        <v>234</v>
+      </c>
+      <c r="P7" s="149" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="R7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="S7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="T7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="U7" s="149" t="s">
+        <v>244</v>
+      </c>
+      <c r="V7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="W7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="X7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y7" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="Z7" s="148" t="s">
         <v>235</v>
       </c>
-      <c r="B7" s="146" t="s">
-        <v>224</v>
-      </c>
-      <c r="C7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="D7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="E7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="F7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="G7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="H7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="I7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="J7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="K7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="L7" s="151" t="s">
-        <v>233</v>
-      </c>
-      <c r="M7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="N7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="O7" s="148" t="s">
-        <v>226</v>
-      </c>
-      <c r="P7" s="149" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="R7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="S7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="T7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="U7" s="149" t="s">
-        <v>236</v>
-      </c>
-      <c r="V7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="W7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="X7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="Y7" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="Z7" s="148" t="s">
-        <v>227</v>
-      </c>
       <c r="AA7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AB7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AC7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AD7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AE7" s="175"/>
       <c r="AF7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AG7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AH7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AI7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AJ7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AK7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AL7" s="175"/>
       <c r="AM7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AN7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AO7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AP7" s="175"/>
       <c r="AQ7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AR7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AS7" s="175"/>
       <c r="AT7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AU7" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AV7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AW7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AX7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AY7" s="175"/>
       <c r="AZ7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BA7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BB7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BC7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BD7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BE7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BF7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BG7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BH7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BI7" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BJ7" s="175"/>
       <c r="BK7" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BL7" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BM7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BN7" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BO7" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BP7" s="148"/>
       <c r="BQ7" s="148"/>
@@ -51903,16 +51975,16 @@
       <c r="BS7" s="148"/>
       <c r="BT7" s="148"/>
       <c r="BU7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BV7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BW7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BX7" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BY7" s="148"/>
       <c r="BZ7" s="148"/>
@@ -51938,220 +52010,220 @@
     </row>
     <row r="8" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="145" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B8" s="146" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="G8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="H8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="I8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="K8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="L8" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="M8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="N8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="O8" s="148" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="P8" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Q8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="R8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="S8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="T8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="U8" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="V8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="W8" s="148" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="X8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Y8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Z8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AA8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AB8" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AC8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AD8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AE8" s="175"/>
       <c r="AF8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AG8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AH8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AI8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AJ8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AK8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AL8" s="175"/>
       <c r="AM8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AN8" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AO8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AP8" s="175"/>
       <c r="AQ8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AR8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AS8" s="175"/>
       <c r="AT8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AU8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AV8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AW8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AX8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AY8" s="175"/>
       <c r="AZ8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BA8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BB8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BC8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BD8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BE8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BF8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BG8" s="148" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="BH8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BI8" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BJ8" s="175"/>
       <c r="BK8" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BL8" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BM8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BN8" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BO8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BP8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BQ8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BR8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BS8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BT8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BU8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BV8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BW8" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BX8" s="148" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="BY8" s="148"/>
       <c r="BZ8" s="148"/>
@@ -52177,244 +52249,244 @@
     </row>
     <row r="9" spans="1:97" ht="15.75">
       <c r="A9" s="145" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" s="146" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="D9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="E9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="F9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="G9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="H9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="I9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="J9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="K9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="L9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="M9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="N9" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="O9" s="151" t="s">
         <v>241</v>
       </c>
-      <c r="B9" s="146" t="s">
-        <v>224</v>
-      </c>
-      <c r="C9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="D9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="E9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="F9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="G9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="H9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="I9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="J9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="K9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="L9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="M9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="N9" s="148" t="s">
-        <v>224</v>
-      </c>
-      <c r="O9" s="151" t="s">
-        <v>233</v>
-      </c>
       <c r="P9" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Q9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="R9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="S9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="T9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="U9" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="V9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="W9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="X9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Y9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Z9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AA9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AB9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AC9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AD9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AE9" s="175"/>
       <c r="AF9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AG9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AH9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AI9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AJ9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AK9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AL9" s="175"/>
       <c r="AM9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AN9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AO9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AP9" s="175"/>
       <c r="AQ9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AR9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AS9" s="175"/>
       <c r="AT9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AU9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AV9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AW9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AX9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AY9" s="175"/>
       <c r="AZ9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BA9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BB9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BC9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BD9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BE9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BF9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BG9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BH9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BI9" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BJ9" s="175"/>
       <c r="BK9" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BL9" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BM9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BN9" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BO9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BP9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BQ9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BR9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BS9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BT9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BU9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BV9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BW9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BX9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BY9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BZ9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CA9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CB9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CC9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CD9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CE9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CF9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CG9" s="148"/>
       <c r="CH9" s="148"/>
@@ -52429,249 +52501,249 @@
       <c r="CQ9" s="148"/>
       <c r="CR9" s="148"/>
       <c r="CS9" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:97" ht="15.75">
       <c r="A10" s="145" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="B10" s="146" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="G10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="H10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="I10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="J10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="K10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="L10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="M10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="N10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="O10" s="148" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="P10" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="Q10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="R10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="S10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="T10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="U10" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="V10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="W10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="X10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Y10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Z10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AA10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AB10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AC10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AD10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AE10" s="175"/>
       <c r="AF10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AG10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AH10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AI10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AJ10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AK10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AL10" s="175"/>
       <c r="AM10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AN10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AO10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AP10" s="175"/>
       <c r="AQ10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AR10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AS10" s="175"/>
       <c r="AT10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AU10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AV10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AW10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AX10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AY10" s="175"/>
       <c r="AZ10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BA10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BB10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BC10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BD10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BE10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BF10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BG10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BH10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BI10" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BJ10" s="175"/>
       <c r="BK10" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BL10" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BM10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BN10" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BO10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BP10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BQ10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BR10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BS10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BT10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BU10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BV10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BW10" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BX10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BY10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BZ10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CA10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CB10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CC10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CD10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CE10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CF10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CG10" s="148"/>
       <c r="CH10" s="148"/>
@@ -52686,249 +52758,249 @@
       <c r="CQ10" s="148"/>
       <c r="CR10" s="148"/>
       <c r="CS10" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:97" ht="15.75">
       <c r="A11" s="145" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B11" s="146" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="D11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="G11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="H11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="I11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J11" s="148" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="K11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="L11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="M11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="N11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="O11" s="148" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="P11" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Q11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="R11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="S11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="T11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="U11" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="V11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="W11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="X11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Y11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Z11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AA11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AB11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AC11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AD11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AE11" s="175"/>
       <c r="AF11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AG11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AH11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AI11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AJ11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AK11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AL11" s="175"/>
       <c r="AM11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AN11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AO11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AP11" s="175"/>
       <c r="AQ11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AR11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AS11" s="175"/>
       <c r="AT11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AU11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AV11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AW11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AX11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AY11" s="175"/>
       <c r="AZ11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BA11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BB11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BC11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BD11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BE11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BF11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BG11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BH11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BI11" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BJ11" s="175"/>
       <c r="BK11" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BL11" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BM11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BN11" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BO11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BP11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BQ11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BR11" s="148" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="BS11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BT11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BU11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BV11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BW11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BX11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BY11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BZ11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CA11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CB11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="CC11" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="CD11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CE11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CF11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CG11" s="148"/>
       <c r="CH11" s="148"/>
@@ -52943,249 +53015,249 @@
       <c r="CQ11" s="148"/>
       <c r="CR11" s="148"/>
       <c r="CS11" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:97" ht="15.75">
       <c r="A12" s="145" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B12" s="146" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="D12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="F12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="G12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="H12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="I12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="J12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="K12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="L12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="M12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="N12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="O12" s="148" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="P12" s="149" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="Q12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="R12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="S12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="T12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="U12" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="V12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="W12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="X12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="Y12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="Z12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AA12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AB12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AC12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AD12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AE12" s="175"/>
       <c r="AF12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AG12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AH12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AI12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AJ12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AK12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AL12" s="175"/>
       <c r="AM12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AN12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AO12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AP12" s="175"/>
       <c r="AQ12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AR12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AS12" s="175"/>
       <c r="AT12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AU12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AV12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AW12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AX12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AY12" s="175"/>
       <c r="AZ12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BA12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BB12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BC12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BD12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BE12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BF12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BG12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BH12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BI12" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BJ12" s="175"/>
       <c r="BK12" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BL12" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BM12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BN12" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BO12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BP12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BQ12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BR12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BS12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BT12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BU12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BV12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BW12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BX12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BY12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="BZ12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="CA12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="CB12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CC12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="CD12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="CE12" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CF12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="CG12" s="148"/>
       <c r="CH12" s="148"/>
@@ -53200,249 +53272,249 @@
       <c r="CQ12" s="148"/>
       <c r="CR12" s="148"/>
       <c r="CS12" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:97" ht="15.75">
       <c r="A13" s="145" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="B13" s="146" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="D13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="E13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="F13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="G13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="H13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="I13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="J13" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="K13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="L13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="M13" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="N13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="O13" s="148" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="P13" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="Q13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="R13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="S13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="T13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="U13" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="V13" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="W13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="X13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="Y13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="Z13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AA13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AB13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AC13" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AD13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AE13" s="176"/>
       <c r="AF13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AG13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AH13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AI13" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AJ13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AK13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AL13" s="176"/>
       <c r="AM13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AN13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AO13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AP13" s="176"/>
       <c r="AQ13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AR13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AS13" s="176"/>
       <c r="AT13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AU13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AV13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AW13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AX13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="AY13" s="176"/>
       <c r="AZ13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BA13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BB13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BC13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BD13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BE13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BF13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BG13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BH13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BI13" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BJ13" s="176"/>
       <c r="BK13" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BL13" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BM13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BN13" s="149" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BO13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BP13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BQ13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BR13" s="148" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="BS13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BT13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BU13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BV13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BW13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BX13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BY13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="BZ13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="CA13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="CB13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="CC13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="CD13" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CE13" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CF13" s="148" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="CG13" s="148"/>
       <c r="CH13" s="148"/>
@@ -53457,7 +53529,7 @@
       <c r="CQ13" s="148"/>
       <c r="CR13" s="148"/>
       <c r="CS13" s="148" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54479,7 +54551,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="25.5">
       <c r="A1" s="152" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B1" s="152" t="s">
         <v>2</v>
@@ -54506,13 +54578,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="156" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="K1" s="157" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="L1" s="155" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="M1" s="158"/>
       <c r="N1" s="158"/>
@@ -54531,10 +54603,10 @@
     </row>
     <row r="2" spans="1:26" ht="38.25">
       <c r="A2" s="159" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B2" s="160" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="C2" s="161"/>
       <c r="D2" s="161" t="s">
@@ -54561,7 +54633,7 @@
       </c>
       <c r="K2" s="164"/>
       <c r="L2" s="165" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="M2" s="158"/>
       <c r="N2" s="158"/>
@@ -54580,13 +54652,13 @@
     </row>
     <row r="3" spans="1:26" ht="51">
       <c r="A3" s="159" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B3" s="177" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="C3" s="166" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="D3" s="161" t="s">
         <v>39</v>
@@ -54608,7 +54680,7 @@
       </c>
       <c r="K3" s="162"/>
       <c r="L3" s="165" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="M3" s="167"/>
       <c r="N3" s="158"/>
@@ -54627,11 +54699,11 @@
     </row>
     <row r="4" spans="1:26" ht="51">
       <c r="A4" s="159" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B4" s="175"/>
       <c r="C4" s="168" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="D4" s="161" t="s">
         <v>39</v>
@@ -54653,7 +54725,7 @@
       </c>
       <c r="K4" s="169"/>
       <c r="L4" s="172" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="M4" s="167"/>
       <c r="N4" s="158"/>
@@ -54672,13 +54744,13 @@
     </row>
     <row r="5" spans="1:26" ht="51">
       <c r="A5" s="159" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B5" s="155" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="C5" s="161" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="D5" s="161" t="s">
         <v>39</v>
@@ -54700,7 +54772,7 @@
       </c>
       <c r="K5" s="162"/>
       <c r="L5" s="165" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="M5" s="167"/>
       <c r="N5" s="158"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 21 de noviembre
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="273">
   <si>
     <t>Asignado a</t>
   </si>
@@ -676,6 +676,9 @@
     <t>envío de una base con la información “si en la solicitud de ingreso los menores de edad vienen con los campos vacíos o en cero en dirección de residencia, teléfono residencia, ciudad, email y celular, se replique la información del contratante y se carguen con los mismos datos. Esto solo para menores de edad y solo si los campos no vienen diligenciados o vienen con dato cero “0”.” De manera semanal , todos los lunes</t>
   </si>
   <si>
+    <t>20/11/2025 se envía correo al cliente confirmando el el asunto del correo Menores sin datos en Afiliaciones Prepagadas cargadas y que el envío de la informacion corresponderá a lo cargado la semana inmediatamente anterior lunes a domingo. y se enviará de manera automática todos los lunes</t>
+  </si>
+  <si>
     <t>OPT_21</t>
   </si>
   <si>
@@ -683,6 +686,9 @@
   </si>
   <si>
     <t>envío de una base con la información “sobre los casos en los que los datos de afiliación de los beneficiarios mayores de edad presenten coincidencias en el correo electrónico y el número de teléfono. Este reporte tiene como objetivo identificar y analizar a los beneficiarios cuya información de contacto sea la misma.”. De manera mensual</t>
+  </si>
+  <si>
+    <t>20/11/2025 se envía correo al cliente confirmando el el asunto del correo Mayores con datos igual al Titular en Afiliaciones Prepagadas cargadas y que el envío de la informacion corresponderá a lo cargado el mes inmediatamente anterior, se vniará de manera automática el primer día del mes.</t>
   </si>
   <si>
     <t>OPT_22</t>
@@ -694,7 +700,13 @@
     <t>OPT_23</t>
   </si>
   <si>
-    <t>Afiliaciones Pos - Consulta Afilicion PBS Nuevas cambio la numeración y en la consulta se tiene restringido el largo</t>
+    <t xml:space="preserve">Afiliaciones Pos - Consulta Afilicion PBS Nuevas </t>
+  </si>
+  <si>
+    <t>Afiliaciones nuevas de PBS WEB cambio la numeración y en la consulta se tiene restringido el largo</t>
+  </si>
+  <si>
+    <t>20/11/2025 se ajusta en la página de consulta para seguimiento de las solicitudes de PBS el largo de la numeración, dado los cambios de las nuevas afiliaciones PBS WEB</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -1090,7 +1102,7 @@
     <t>True</t>
   </si>
   <si>
-    <t>false</t>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -2442,9 +2454,9 @@
   </sheetPr>
   <dimension ref="A1:AM940"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P58" sqref="P58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2461,7 +2473,7 @@
     <col min="13" max="13" width="5.109375" customWidth="1"/>
     <col min="14" max="15" width="9.21875" customWidth="1"/>
     <col min="16" max="16" width="33.44140625" customWidth="1"/>
-    <col min="17" max="17" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8" customWidth="1"/>
     <col min="18" max="39" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2589,7 +2601,7 @@
         <v>21</v>
       </c>
       <c r="Q2" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R2" s="27"/>
       <c r="S2" s="27"/>
@@ -2663,7 +2675,7 @@
         <v>24</v>
       </c>
       <c r="Q3" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R3" s="42"/>
       <c r="S3" s="42"/>
@@ -2737,7 +2749,7 @@
         <v>28</v>
       </c>
       <c r="Q4" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
@@ -2809,7 +2821,7 @@
         <v>32</v>
       </c>
       <c r="Q5" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R5" s="42"/>
       <c r="S5" s="42"/>
@@ -2883,7 +2895,7 @@
         <v>35</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="27"/>
@@ -2937,7 +2949,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32824</v>
+        <v>32829</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -2945,7 +2957,7 @@
         <v>40</v>
       </c>
       <c r="Q7" s="41" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="R7" s="42"/>
       <c r="S7" s="42"/>
@@ -3011,7 +3023,7 @@
         <v>43</v>
       </c>
       <c r="Q8" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
@@ -3083,7 +3095,7 @@
         <v>46</v>
       </c>
       <c r="Q9" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R9" s="42"/>
       <c r="S9" s="42"/>
@@ -3155,7 +3167,7 @@
         <v>49</v>
       </c>
       <c r="Q10" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R10" s="27"/>
       <c r="S10" s="27"/>
@@ -3229,7 +3241,7 @@
         <v>53</v>
       </c>
       <c r="Q11" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R11" s="42"/>
       <c r="S11" s="42"/>
@@ -3287,7 +3299,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f ca="1">IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3297,7 +3309,7 @@
         <v>57</v>
       </c>
       <c r="Q12" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
@@ -3369,7 +3381,7 @@
         <v>61</v>
       </c>
       <c r="Q13" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R13" s="42"/>
       <c r="S13" s="42"/>
@@ -3441,7 +3453,7 @@
         <v>65</v>
       </c>
       <c r="Q14" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R14" s="27"/>
       <c r="S14" s="27"/>
@@ -3513,7 +3525,7 @@
         <v>69</v>
       </c>
       <c r="Q15" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R15" s="42"/>
       <c r="S15" s="42"/>
@@ -3565,7 +3577,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f ca="1">IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32824</v>
+        <v>32829</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -3573,7 +3585,7 @@
         <v>73</v>
       </c>
       <c r="Q16" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R16" s="27"/>
       <c r="S16" s="27"/>
@@ -3647,7 +3659,7 @@
         <v>76</v>
       </c>
       <c r="Q17" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R17" s="42"/>
       <c r="S17" s="42"/>
@@ -3721,7 +3733,7 @@
         <v>80</v>
       </c>
       <c r="Q18" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R18" s="27"/>
       <c r="S18" s="27"/>
@@ -3791,7 +3803,7 @@
         <v>83</v>
       </c>
       <c r="Q19" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R19" s="42"/>
       <c r="S19" s="42"/>
@@ -3863,7 +3875,7 @@
       </c>
       <c r="P20" s="25"/>
       <c r="Q20" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R20" s="27"/>
       <c r="S20" s="27"/>
@@ -3935,7 +3947,7 @@
         <v>89</v>
       </c>
       <c r="Q21" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R21" s="42"/>
       <c r="S21" s="42"/>
@@ -3991,7 +4003,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f ca="1">IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -3999,7 +4011,7 @@
         <v>94</v>
       </c>
       <c r="Q22" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R22" s="27"/>
       <c r="S22" s="27"/>
@@ -4073,7 +4085,7 @@
         <v>98</v>
       </c>
       <c r="Q23" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R23" s="42"/>
       <c r="S23" s="42"/>
@@ -4131,7 +4143,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f ca="1">IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4139,7 +4151,7 @@
         <v>102</v>
       </c>
       <c r="Q24" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R24" s="27"/>
       <c r="S24" s="27"/>
@@ -4213,7 +4225,7 @@
         <v>106</v>
       </c>
       <c r="Q25" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R25" s="42"/>
       <c r="S25" s="42"/>
@@ -4263,13 +4275,13 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f ca="1">IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32824</v>
+        <v>32829</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
       <c r="P26" s="25"/>
       <c r="Q26" s="26" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="R26" s="27"/>
       <c r="S26" s="27"/>
@@ -4341,7 +4353,7 @@
         <v>112</v>
       </c>
       <c r="Q27" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R27" s="42"/>
       <c r="S27" s="42"/>
@@ -4401,7 +4413,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f ca="1">IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
@@ -4409,7 +4421,7 @@
         <v>117</v>
       </c>
       <c r="Q28" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R28" s="27"/>
       <c r="S28" s="27"/>
@@ -4483,7 +4495,7 @@
         <v>120</v>
       </c>
       <c r="Q29" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R29" s="42"/>
       <c r="S29" s="42"/>
@@ -4557,7 +4569,7 @@
         <v>123</v>
       </c>
       <c r="Q30" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R30" s="27"/>
       <c r="S30" s="27"/>
@@ -4631,7 +4643,7 @@
         <v>127</v>
       </c>
       <c r="Q31" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R31" s="42"/>
       <c r="S31" s="42"/>
@@ -4705,7 +4717,7 @@
         <v>131</v>
       </c>
       <c r="Q32" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R32" s="27"/>
       <c r="S32" s="27"/>
@@ -4779,7 +4791,7 @@
         <v>135</v>
       </c>
       <c r="Q33" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R33" s="42"/>
       <c r="S33" s="42"/>
@@ -4839,7 +4851,7 @@
       <c r="L34" s="23"/>
       <c r="M34" s="24">
         <f ca="1">IF(ISBLANK(L34), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L34, Hoja2!$A$1:$A$18))</f>
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
@@ -4847,7 +4859,7 @@
         <v>138</v>
       </c>
       <c r="Q34" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R34" s="27"/>
       <c r="S34" s="27"/>
@@ -4905,7 +4917,7 @@
       <c r="L35" s="38"/>
       <c r="M35" s="39">
         <f ca="1">IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="N35" s="38">
         <v>45938</v>
@@ -4917,7 +4929,7 @@
         <v>142</v>
       </c>
       <c r="Q35" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R35" s="46"/>
       <c r="S35" s="46"/>
@@ -4975,7 +4987,7 @@
       <c r="L36" s="23"/>
       <c r="M36" s="24">
         <f ca="1">IF(ISBLANK(L36), NETWORKDAYS(J36, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J36, L36, Hoja2!$A$1:$A$18))</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
@@ -4983,7 +4995,7 @@
         <v>146</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R36" s="48"/>
       <c r="S36" s="48"/>
@@ -5041,7 +5053,7 @@
       <c r="L37" s="38"/>
       <c r="M37" s="39">
         <f ca="1">IF(ISBLANK(L37), NETWORKDAYS(J37, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J37, L37, Hoja2!$A$1:$A$18))</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="N37" s="38">
         <v>45971</v>
@@ -5053,7 +5065,7 @@
         <v>150</v>
       </c>
       <c r="Q37" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R37" s="46"/>
       <c r="S37" s="46"/>
@@ -5109,7 +5121,7 @@
       <c r="L38" s="23"/>
       <c r="M38" s="24">
         <f ca="1">IF(ISBLANK(L38), NETWORKDAYS(J38, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J38, L38, Hoja2!$A$1:$A$18))</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="N38" s="23"/>
       <c r="O38" s="23"/>
@@ -5117,7 +5129,7 @@
         <v>154</v>
       </c>
       <c r="Q38" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R38" s="48"/>
       <c r="S38" s="48"/>
@@ -5176,7 +5188,7 @@
       <c r="O39" s="38"/>
       <c r="P39" s="40"/>
       <c r="Q39" s="41" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="R39" s="46"/>
       <c r="S39" s="46"/>
@@ -5216,26 +5228,34 @@
       </c>
       <c r="E40" s="17"/>
       <c r="F40" s="18" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="G40" s="19">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="H40" s="20"/>
       <c r="I40" s="21">
         <v>45968</v>
       </c>
-      <c r="J40" s="22"/>
+      <c r="J40" s="22">
+        <v>45968</v>
+      </c>
       <c r="K40" s="23">
         <v>45975</v>
       </c>
       <c r="L40" s="23"/>
       <c r="M40" s="24"/>
-      <c r="N40" s="23"/>
-      <c r="O40" s="23"/>
-      <c r="P40" s="25"/>
+      <c r="N40" s="23">
+        <v>45981</v>
+      </c>
+      <c r="O40" s="23">
+        <v>45981</v>
+      </c>
+      <c r="P40" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="Q40" s="26" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R40" s="48"/>
       <c r="S40" s="48"/>
@@ -5265,36 +5285,44 @@
         <v>36</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E41" s="32"/>
       <c r="F41" s="33" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="G41" s="34">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="H41" s="35"/>
       <c r="I41" s="36">
         <v>45968</v>
       </c>
-      <c r="J41" s="37"/>
+      <c r="J41" s="37">
+        <v>45968</v>
+      </c>
       <c r="K41" s="38">
         <v>45975</v>
       </c>
       <c r="L41" s="38"/>
       <c r="M41" s="39"/>
-      <c r="N41" s="38"/>
-      <c r="O41" s="38"/>
-      <c r="P41" s="40"/>
+      <c r="N41" s="38">
+        <v>45981</v>
+      </c>
+      <c r="O41" s="38">
+        <v>45981</v>
+      </c>
+      <c r="P41" s="40" t="s">
+        <v>165</v>
+      </c>
       <c r="Q41" s="41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="R41" s="46"/>
       <c r="S41" s="46"/>
@@ -5324,10 +5352,10 @@
         <v>36</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="17"/>
@@ -5372,34 +5400,50 @@
       <c r="AL42" s="48"/>
       <c r="AM42" s="49"/>
     </row>
-    <row r="43" spans="1:39" ht="71.25">
+    <row r="43" spans="1:39" ht="28.5">
       <c r="A43" s="28" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="D43" s="31"/>
+        <v>169</v>
+      </c>
+      <c r="D43" s="31" t="s">
+        <v>170</v>
+      </c>
       <c r="E43" s="32"/>
       <c r="F43" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="G43" s="34"/>
+        <v>20</v>
+      </c>
+      <c r="G43" s="34">
+        <v>100</v>
+      </c>
       <c r="H43" s="35"/>
       <c r="I43" s="36">
         <v>45973</v>
       </c>
-      <c r="J43" s="37"/>
-      <c r="K43" s="38"/>
+      <c r="J43" s="37">
+        <v>45981</v>
+      </c>
+      <c r="K43" s="38">
+        <v>45981</v>
+      </c>
       <c r="L43" s="38"/>
       <c r="M43" s="39"/>
-      <c r="N43" s="38"/>
-      <c r="O43" s="38"/>
-      <c r="P43" s="40"/>
-      <c r="Q43" s="41"/>
+      <c r="N43" s="38">
+        <v>45981</v>
+      </c>
+      <c r="O43" s="38">
+        <v>45981</v>
+      </c>
+      <c r="P43" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q43" s="41" t="s">
+        <v>271</v>
+      </c>
       <c r="R43" s="46"/>
       <c r="S43" s="46"/>
       <c r="T43" s="46"/>
@@ -42248,7 +42292,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30">
       <c r="A1" s="86" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B1" s="86" t="s">
         <v>2</v>
@@ -42275,13 +42319,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="89" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="K1" s="86" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="L1" s="90" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="M1" s="91"/>
       <c r="N1" s="91"/>
@@ -42300,14 +42344,14 @@
     </row>
     <row r="2" spans="1:26" ht="30">
       <c r="A2" s="92" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B2" s="93" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C2" s="94"/>
       <c r="D2" s="95" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E2" s="96">
         <v>45526</v>
@@ -42321,7 +42365,7 @@
       <c r="J2" s="94"/>
       <c r="K2" s="94"/>
       <c r="L2" s="94" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M2" s="97"/>
       <c r="N2" s="97"/>
@@ -42340,13 +42384,13 @@
     </row>
     <row r="3" spans="1:26" ht="28.5">
       <c r="A3" s="98" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C3" s="100" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D3" s="100" t="s">
         <v>20</v>
@@ -42370,7 +42414,7 @@
       </c>
       <c r="K3" s="102"/>
       <c r="L3" s="104" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="M3" s="91"/>
       <c r="N3" s="91"/>
@@ -42389,16 +42433,16 @@
     </row>
     <row r="4" spans="1:26" ht="186">
       <c r="A4" s="105" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C4" s="105" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D4" s="107" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E4" s="108">
         <v>45581</v>
@@ -42421,7 +42465,7 @@
       </c>
       <c r="K4" s="108"/>
       <c r="L4" s="105" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="M4" s="111"/>
       <c r="N4" s="111"/>
@@ -42440,16 +42484,16 @@
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" s="90" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D5" s="112" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E5" s="101">
         <v>45572</v>
@@ -42470,7 +42514,7 @@
       </c>
       <c r="K5" s="101"/>
       <c r="L5" s="104" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M5" s="91"/>
       <c r="N5" s="91"/>
@@ -42489,16 +42533,16 @@
     </row>
     <row r="6" spans="1:26" ht="117">
       <c r="A6" s="113" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B6" s="113" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C6" s="107" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D6" s="113" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E6" s="114">
         <v>45602</v>
@@ -42519,7 +42563,7 @@
         <v>45602</v>
       </c>
       <c r="L6" s="115" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M6" s="116"/>
       <c r="N6" s="117"/>
@@ -42538,16 +42582,16 @@
     </row>
     <row r="7" spans="1:26" ht="99.75">
       <c r="A7" s="90" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C7" s="118" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D7" s="112" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E7" s="101">
         <v>45589</v>
@@ -42568,7 +42612,7 @@
       </c>
       <c r="K7" s="112"/>
       <c r="L7" s="120" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="M7" s="121"/>
       <c r="N7" s="121"/>
@@ -42587,14 +42631,14 @@
     </row>
     <row r="8" spans="1:26" ht="71.25">
       <c r="A8" s="122" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B8" s="123" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C8" s="124"/>
       <c r="D8" s="124" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="E8" s="125">
         <v>45603</v>
@@ -42615,7 +42659,7 @@
       </c>
       <c r="K8" s="125"/>
       <c r="L8" s="127" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M8" s="91"/>
       <c r="N8" s="91"/>
@@ -42634,16 +42678,16 @@
     </row>
     <row r="9" spans="1:26" ht="42.75">
       <c r="A9" s="128" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B9" s="129" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C9" s="130" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D9" s="131" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E9" s="132">
         <v>45671</v>
@@ -42652,7 +42696,7 @@
         <v>45673</v>
       </c>
       <c r="G9" s="130" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="H9" s="132">
         <v>45680</v>
@@ -42666,7 +42710,7 @@
       </c>
       <c r="K9" s="130"/>
       <c r="L9" s="134" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="M9" s="135"/>
       <c r="N9" s="135"/>
@@ -42685,14 +42729,14 @@
     </row>
     <row r="10" spans="1:26" ht="57">
       <c r="A10" s="128" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B10" s="136"/>
       <c r="C10" s="134" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D10" s="131" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E10" s="132">
         <v>45671</v>
@@ -42711,7 +42755,7 @@
       <c r="J10" s="130"/>
       <c r="K10" s="130"/>
       <c r="L10" s="134" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="M10" s="135"/>
       <c r="N10" s="135"/>
@@ -42730,14 +42774,14 @@
     </row>
     <row r="11" spans="1:26" ht="42.75">
       <c r="A11" s="128" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B11" s="136"/>
       <c r="C11" s="134" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D11" s="131" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E11" s="132">
         <v>45671</v>
@@ -42756,7 +42800,7 @@
       <c r="J11" s="130"/>
       <c r="K11" s="130"/>
       <c r="L11" s="134" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="M11" s="135"/>
       <c r="N11" s="135"/>
@@ -42775,14 +42819,14 @@
     </row>
     <row r="12" spans="1:26" ht="42.75">
       <c r="A12" s="128" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B12" s="136"/>
       <c r="C12" s="134" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D12" s="131" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E12" s="132">
         <v>45671</v>
@@ -42801,7 +42845,7 @@
       <c r="J12" s="130"/>
       <c r="K12" s="130"/>
       <c r="L12" s="134" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="M12" s="135"/>
       <c r="N12" s="135"/>
@@ -42820,14 +42864,14 @@
     </row>
     <row r="13" spans="1:26" ht="42.75">
       <c r="A13" s="128" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B13" s="136"/>
       <c r="C13" s="134" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="D13" s="131" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E13" s="132">
         <v>45671</v>
@@ -42846,7 +42890,7 @@
       <c r="J13" s="130"/>
       <c r="K13" s="130"/>
       <c r="L13" s="134" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="M13" s="135"/>
       <c r="N13" s="135"/>
@@ -42865,14 +42909,14 @@
     </row>
     <row r="14" spans="1:26" ht="42.75">
       <c r="A14" s="128" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B14" s="136"/>
       <c r="C14" s="134" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D14" s="131" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E14" s="132">
         <v>45671</v>
@@ -42891,7 +42935,7 @@
       <c r="J14" s="130"/>
       <c r="K14" s="130"/>
       <c r="L14" s="130" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="M14" s="135"/>
       <c r="N14" s="135"/>
@@ -42910,14 +42954,14 @@
     </row>
     <row r="15" spans="1:26" ht="42.75">
       <c r="A15" s="128" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B15" s="136"/>
       <c r="C15" s="134" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D15" s="131" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E15" s="132">
         <v>45671</v>
@@ -42936,7 +42980,7 @@
       <c r="J15" s="130"/>
       <c r="K15" s="130"/>
       <c r="L15" s="130" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="M15" s="135"/>
       <c r="N15" s="135"/>
@@ -42955,14 +42999,14 @@
     </row>
     <row r="16" spans="1:26" ht="71.25">
       <c r="A16" s="128" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B16" s="137"/>
       <c r="C16" s="138" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D16" s="131" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E16" s="132">
         <v>45681</v>
@@ -42981,7 +43025,7 @@
       <c r="J16" s="130"/>
       <c r="K16" s="130"/>
       <c r="L16" s="134" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M16" s="135"/>
       <c r="N16" s="135"/>
@@ -49513,7 +49557,7 @@
         <v>45292</v>
       </c>
       <c r="B1" s="135" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
@@ -49521,7 +49565,7 @@
         <v>45299</v>
       </c>
       <c r="B2" s="135" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
@@ -49529,7 +49573,7 @@
         <v>45376</v>
       </c>
       <c r="B3" s="135" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
@@ -49537,7 +49581,7 @@
         <v>45379</v>
       </c>
       <c r="B4" s="135" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
@@ -49545,7 +49589,7 @@
         <v>45380</v>
       </c>
       <c r="B5" s="135" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1">
@@ -49553,7 +49597,7 @@
         <v>45413</v>
       </c>
       <c r="B6" s="135" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
@@ -49561,7 +49605,7 @@
         <v>45425</v>
       </c>
       <c r="B7" s="135" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
@@ -49569,7 +49613,7 @@
         <v>45446</v>
       </c>
       <c r="B8" s="135" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1">
@@ -49577,7 +49621,7 @@
         <v>45453</v>
       </c>
       <c r="B9" s="135" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1">
@@ -49585,7 +49629,7 @@
         <v>45474</v>
       </c>
       <c r="B10" s="135" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1">
@@ -49593,7 +49637,7 @@
         <v>45493</v>
       </c>
       <c r="B11" s="135" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" customHeight="1">
@@ -49601,7 +49645,7 @@
         <v>45511</v>
       </c>
       <c r="B12" s="135" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1">
@@ -49609,7 +49653,7 @@
         <v>45523</v>
       </c>
       <c r="B13" s="135" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" customHeight="1">
@@ -49617,7 +49661,7 @@
         <v>45579</v>
       </c>
       <c r="B14" s="135" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" customHeight="1">
@@ -49625,7 +49669,7 @@
         <v>45600</v>
       </c>
       <c r="B15" s="135" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1">
@@ -49633,7 +49677,7 @@
         <v>45607</v>
       </c>
       <c r="B16" s="135" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
@@ -49641,7 +49685,7 @@
         <v>45634</v>
       </c>
       <c r="B17" s="135" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1">
@@ -49649,7 +49693,7 @@
         <v>45651</v>
       </c>
       <c r="B18" s="135" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1"/>
@@ -50661,7 +50705,7 @@
   <sheetData>
     <row r="1" spans="1:97" ht="15.75">
       <c r="A1" s="140" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B1" s="135"/>
       <c r="C1" s="135"/>
@@ -50719,7 +50763,7 @@
     </row>
     <row r="3" spans="1:97" ht="32.25" customHeight="1">
       <c r="A3" s="141" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B3" s="142">
         <v>45596</v>
@@ -51012,261 +51056,261 @@
     </row>
     <row r="4" spans="1:97" ht="30.75" customHeight="1">
       <c r="A4" s="145" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B4" s="146" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C4" s="147" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="G4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="J4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="L4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="M4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="N4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="O4" s="148" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="P4" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Q4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="R4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="S4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="T4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="U4" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="V4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="W4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="X4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Y4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Z4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AA4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AB4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AC4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AD4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AE4" s="174" t="s">
+        <v>242</v>
+      </c>
+      <c r="AF4" s="148" t="s">
         <v>238</v>
       </c>
-      <c r="AF4" s="148" t="s">
-        <v>234</v>
-      </c>
       <c r="AG4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AH4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AI4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AJ4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AK4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AL4" s="174" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="AM4" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AN4" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AO4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AP4" s="174" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="AQ4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AR4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AS4" s="174" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="AT4" s="150" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AU4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AV4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AW4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AX4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AY4" s="174" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="AZ4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BA4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BB4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BC4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BD4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BE4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BF4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BG4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BH4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BI4" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BJ4" s="174" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="BK4" s="149" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="BL4" s="149" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="BM4" s="149" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="BN4" s="149" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="BO4" s="149" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="BP4" s="149" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="BQ4" s="149" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="BR4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BS4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BT4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BU4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BV4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BW4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BX4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BY4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BZ4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CA4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CB4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CC4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CD4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CE4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CF4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CG4" s="148"/>
       <c r="CH4" s="148"/>
       <c r="CI4" s="174" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="CJ4" s="148"/>
       <c r="CK4" s="148"/>
@@ -51278,249 +51322,249 @@
       <c r="CQ4" s="148"/>
       <c r="CR4" s="148"/>
       <c r="CS4" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:97" ht="15.75" customHeight="1">
       <c r="A5" s="145" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B5" s="146" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="G5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="J5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="L5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="M5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="N5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="O5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="P5" s="149" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="Q5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="R5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="S5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="T5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="U5" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="V5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="W5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="X5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Y5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Z5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AA5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AB5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AC5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AD5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AE5" s="175"/>
       <c r="AF5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AG5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AH5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AI5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AJ5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AK5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AL5" s="175"/>
       <c r="AM5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AN5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AO5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AP5" s="175"/>
       <c r="AQ5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="AR5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="AS5" s="175"/>
       <c r="AT5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="AU5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="AV5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="AW5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="AX5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="AY5" s="175"/>
       <c r="AZ5" s="148" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="BA5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BB5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BC5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BD5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BE5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BF5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BG5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BH5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BI5" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BJ5" s="175"/>
       <c r="BK5" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BL5" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BM5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BN5" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BO5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BP5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BQ5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BR5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BS5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BT5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BU5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BV5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BW5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BX5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BY5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BZ5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CA5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CB5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CC5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CD5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CE5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CF5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CG5" s="148"/>
       <c r="CH5" s="148"/>
@@ -51535,249 +51579,249 @@
       <c r="CQ5" s="148"/>
       <c r="CR5" s="148"/>
       <c r="CS5" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:97" ht="15.75">
       <c r="A6" s="145" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B6" s="146" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="G6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="J6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K6" s="151" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="L6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="M6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="N6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="O6" s="148" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="P6" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Q6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="R6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="S6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="T6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="U6" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="V6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="W6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="X6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Y6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Z6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AA6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AB6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AC6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AD6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AE6" s="175"/>
       <c r="AF6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AG6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AH6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AI6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AJ6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AK6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AL6" s="175"/>
       <c r="AM6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AN6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AO6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AP6" s="175"/>
       <c r="AQ6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AR6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AS6" s="175"/>
       <c r="AT6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AU6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AV6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AW6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AX6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AY6" s="175"/>
       <c r="AZ6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BA6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BB6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BC6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BD6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BE6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BF6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BG6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BH6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BI6" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BJ6" s="175"/>
       <c r="BK6" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BL6" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BM6" s="148" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="BN6" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BO6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BP6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BQ6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BR6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BS6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BT6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BU6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BV6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BW6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BX6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BY6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BZ6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CA6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CB6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CC6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CD6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CE6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CF6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CG6" s="148"/>
       <c r="CH6" s="148"/>
@@ -51792,198 +51836,198 @@
       <c r="CQ6" s="148"/>
       <c r="CR6" s="148"/>
       <c r="CS6" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="145" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B7" s="146" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="G7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="J7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="L7" s="151" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="M7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="N7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="O7" s="148" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="P7" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Q7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="R7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="S7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="T7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="U7" s="149" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="V7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="W7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="X7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Y7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Z7" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AA7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AB7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AC7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AD7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AE7" s="175"/>
       <c r="AF7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AG7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AH7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AI7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AJ7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AK7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AL7" s="175"/>
       <c r="AM7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AN7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AO7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AP7" s="175"/>
       <c r="AQ7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AR7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AS7" s="175"/>
       <c r="AT7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AU7" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AV7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AW7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AX7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AY7" s="175"/>
       <c r="AZ7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BA7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BB7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BC7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BD7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BE7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BF7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BG7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BH7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BI7" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BJ7" s="175"/>
       <c r="BK7" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BL7" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BM7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BN7" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BO7" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BP7" s="148"/>
       <c r="BQ7" s="148"/>
@@ -51991,16 +52035,16 @@
       <c r="BS7" s="148"/>
       <c r="BT7" s="148"/>
       <c r="BU7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BV7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BW7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BX7" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BY7" s="148"/>
       <c r="BZ7" s="148"/>
@@ -52026,220 +52070,220 @@
     </row>
     <row r="8" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="145" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B8" s="146" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="G8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="J8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="L8" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="M8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="N8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="O8" s="148" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="P8" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Q8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="R8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="S8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="T8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="U8" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="V8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="W8" s="148" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="X8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Y8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Z8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AA8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AB8" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AC8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AD8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AE8" s="175"/>
       <c r="AF8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AG8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AH8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AI8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AJ8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AK8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AL8" s="175"/>
       <c r="AM8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AN8" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AO8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AP8" s="175"/>
       <c r="AQ8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AR8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AS8" s="175"/>
       <c r="AT8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AU8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AV8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AW8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AX8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AY8" s="175"/>
       <c r="AZ8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BA8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BB8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BC8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BD8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BE8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BF8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BG8" s="148" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="BH8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BI8" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BJ8" s="175"/>
       <c r="BK8" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BL8" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BM8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BN8" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BO8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BP8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BQ8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BR8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BS8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BT8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BU8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BV8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BW8" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BX8" s="148" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="BY8" s="148"/>
       <c r="BZ8" s="148"/>
@@ -52265,244 +52309,244 @@
     </row>
     <row r="9" spans="1:97" ht="15.75">
       <c r="A9" s="145" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B9" s="146" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="G9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="J9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="L9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="M9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="N9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="O9" s="151" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="P9" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Q9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="R9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="S9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="T9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="U9" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="V9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="W9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="X9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Y9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Z9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AA9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AB9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AC9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AD9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AE9" s="175"/>
       <c r="AF9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AG9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AH9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AI9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AJ9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AK9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AL9" s="175"/>
       <c r="AM9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AN9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AO9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AP9" s="175"/>
       <c r="AQ9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AR9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AS9" s="175"/>
       <c r="AT9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AU9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AV9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AW9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AX9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AY9" s="175"/>
       <c r="AZ9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BA9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BB9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BC9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BD9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BE9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BF9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BG9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BH9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BI9" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BJ9" s="175"/>
       <c r="BK9" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BL9" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BM9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BN9" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BO9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BP9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BQ9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BR9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BS9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BT9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BU9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BV9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BW9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BX9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BY9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BZ9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CA9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CB9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CC9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CD9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CE9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CF9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CG9" s="148"/>
       <c r="CH9" s="148"/>
@@ -52517,249 +52561,249 @@
       <c r="CQ9" s="148"/>
       <c r="CR9" s="148"/>
       <c r="CS9" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:97" ht="15.75">
       <c r="A10" s="145" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B10" s="146" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="G10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="J10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="L10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="M10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="N10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="O10" s="148" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="P10" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="Q10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="R10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="S10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="T10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="U10" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="V10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="W10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="X10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Y10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Z10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AA10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AB10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AC10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AD10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AE10" s="175"/>
       <c r="AF10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AG10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AH10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AI10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AJ10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AK10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AL10" s="175"/>
       <c r="AM10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AN10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AO10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AP10" s="175"/>
       <c r="AQ10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AR10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AS10" s="175"/>
       <c r="AT10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AU10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AV10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AW10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AX10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AY10" s="175"/>
       <c r="AZ10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BA10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BB10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BC10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BD10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BE10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BF10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BG10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BH10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BI10" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BJ10" s="175"/>
       <c r="BK10" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BL10" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BM10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BN10" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BO10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BP10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BQ10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BR10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BS10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BT10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BU10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BV10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BW10" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BX10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BY10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BZ10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CA10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CB10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CC10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CD10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CE10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CF10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CG10" s="148"/>
       <c r="CH10" s="148"/>
@@ -52774,249 +52818,249 @@
       <c r="CQ10" s="148"/>
       <c r="CR10" s="148"/>
       <c r="CS10" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:97" ht="15.75">
       <c r="A11" s="145" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B11" s="146" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="G11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="J11" s="148" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="K11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="L11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="M11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="N11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="O11" s="148" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="P11" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Q11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="R11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="S11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="T11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="U11" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="V11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="W11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="X11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Y11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Z11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AA11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AB11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AC11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AD11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AE11" s="175"/>
       <c r="AF11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AG11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AH11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AI11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AJ11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AK11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AL11" s="175"/>
       <c r="AM11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AN11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AO11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AP11" s="175"/>
       <c r="AQ11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AR11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AS11" s="175"/>
       <c r="AT11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AU11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AV11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AW11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AX11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AY11" s="175"/>
       <c r="AZ11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BA11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BB11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BC11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BD11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BE11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BF11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BG11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BH11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BI11" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BJ11" s="175"/>
       <c r="BK11" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BL11" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BM11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BN11" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BO11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BP11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BQ11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BR11" s="148" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="BS11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BT11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BU11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BV11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BW11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BX11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BY11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BZ11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CA11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CB11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="CC11" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="CD11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CE11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CF11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CG11" s="148"/>
       <c r="CH11" s="148"/>
@@ -53031,249 +53075,249 @@
       <c r="CQ11" s="148"/>
       <c r="CR11" s="148"/>
       <c r="CS11" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:97" ht="15.75">
       <c r="A12" s="145" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B12" s="146" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="G12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="H12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="I12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="J12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="L12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="M12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="N12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="O12" s="148" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="P12" s="149" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="Q12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="R12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="S12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="T12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="U12" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="V12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="W12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="X12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="Y12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="Z12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AA12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AB12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AC12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AD12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AE12" s="175"/>
       <c r="AF12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AG12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AH12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AI12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AJ12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AK12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AL12" s="175"/>
       <c r="AM12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AN12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AO12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AP12" s="175"/>
       <c r="AQ12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AR12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AS12" s="175"/>
       <c r="AT12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AU12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AV12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AW12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AX12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AY12" s="175"/>
       <c r="AZ12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BA12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BB12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BC12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BD12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BE12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BF12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BG12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BH12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BI12" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BJ12" s="175"/>
       <c r="BK12" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BL12" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BM12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BN12" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BO12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BP12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BQ12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BR12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BS12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BT12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BU12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BV12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BW12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BX12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BY12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="BZ12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="CA12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="CB12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CC12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="CD12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="CE12" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CF12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="CG12" s="148"/>
       <c r="CH12" s="148"/>
@@ -53288,249 +53332,249 @@
       <c r="CQ12" s="148"/>
       <c r="CR12" s="148"/>
       <c r="CS12" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:97" ht="15.75">
       <c r="A13" s="145" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B13" s="146" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="G13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="H13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="I13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="J13" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="K13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="L13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="M13" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="N13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="O13" s="148" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="P13" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="Q13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="R13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="S13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="T13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="U13" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="V13" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="W13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="X13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="Y13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="Z13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AA13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AB13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AC13" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AD13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AE13" s="176"/>
       <c r="AF13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AG13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AH13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AI13" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="AJ13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AK13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AL13" s="176"/>
       <c r="AM13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AN13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AO13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AP13" s="176"/>
       <c r="AQ13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AR13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AS13" s="176"/>
       <c r="AT13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AU13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AV13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AW13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AX13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AY13" s="176"/>
       <c r="AZ13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BA13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BB13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BC13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BD13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BE13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BF13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BG13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BH13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BI13" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BJ13" s="176"/>
       <c r="BK13" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BL13" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BM13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BN13" s="149" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BO13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BP13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BQ13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BR13" s="148" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="BS13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BT13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BU13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BV13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BW13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BX13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BY13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="BZ13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="CA13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="CB13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="CC13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="CD13" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CE13" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CF13" s="148" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="CG13" s="148"/>
       <c r="CH13" s="148"/>
@@ -53545,7 +53589,7 @@
       <c r="CQ13" s="148"/>
       <c r="CR13" s="148"/>
       <c r="CS13" s="148" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54567,7 +54611,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="25.5">
       <c r="A1" s="152" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B1" s="152" t="s">
         <v>2</v>
@@ -54594,13 +54638,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="156" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="K1" s="157" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="L1" s="155" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="M1" s="158"/>
       <c r="N1" s="158"/>
@@ -54619,10 +54663,10 @@
     </row>
     <row r="2" spans="1:26" ht="38.25">
       <c r="A2" s="159" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B2" s="160" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C2" s="161"/>
       <c r="D2" s="161" t="s">
@@ -54649,7 +54693,7 @@
       </c>
       <c r="K2" s="164"/>
       <c r="L2" s="165" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="M2" s="158"/>
       <c r="N2" s="158"/>
@@ -54668,13 +54712,13 @@
     </row>
     <row r="3" spans="1:26" ht="51">
       <c r="A3" s="159" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B3" s="177" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C3" s="166" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D3" s="161" t="s">
         <v>39</v>
@@ -54696,7 +54740,7 @@
       </c>
       <c r="K3" s="162"/>
       <c r="L3" s="165" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="M3" s="167"/>
       <c r="N3" s="158"/>
@@ -54715,11 +54759,11 @@
     </row>
     <row r="4" spans="1:26" ht="51">
       <c r="A4" s="159" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B4" s="175"/>
       <c r="C4" s="168" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D4" s="161" t="s">
         <v>39</v>
@@ -54741,7 +54785,7 @@
       </c>
       <c r="K4" s="169"/>
       <c r="L4" s="172" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="M4" s="167"/>
       <c r="N4" s="158"/>
@@ -54760,13 +54804,13 @@
     </row>
     <row r="5" spans="1:26" ht="51">
       <c r="A5" s="159" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B5" s="155" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C5" s="161" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="D5" s="161" t="s">
         <v>39</v>
@@ -54788,7 +54832,7 @@
       </c>
       <c r="K5" s="162"/>
       <c r="L5" s="165" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="M5" s="167"/>
       <c r="N5" s="158"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 10 Diciembre
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9555"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="EN PROCESO (Colmedica)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="288">
   <si>
     <t>Asignado a</t>
   </si>
@@ -709,6 +709,52 @@
     <t>20/11/2025 se ajusta en la página de consulta para seguimiento de las solicitudes de PBS el largo de la numeración, dado los cambios de las nuevas afiliaciones PBS WEB</t>
   </si>
   <si>
+    <t>OPT_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afiliaciones Pos - Proceso nuevas afiliaciones </t>
+  </si>
+  <si>
+    <t>inconsistencia en la generación de los lotes por imágenes de más y que son informativas, Adicionar al proceso la eliminación de estos archivos para que el sistema no las tenga en cuenta al momento del loteo</t>
+  </si>
+  <si>
+    <t>OPT_25</t>
+  </si>
+  <si>
+    <t>Afiliaciones Pre - Parentescos XML</t>
+  </si>
+  <si>
+    <t>Ajustar un parentesco que no se estaba cargando desde el xml por cambio en su escritura</t>
+  </si>
+  <si>
+    <t>OPT_26</t>
+  </si>
+  <si>
+    <t>Afiliaciones Pos - Documentos con extension errada</t>
+  </si>
+  <si>
+    <t>Seguimiento nuevas afiliaciones en la marcación de soportes hay imágenes que no se pueden visualizar, y se detecta que llegan con una extensión que no corresponde al tipo de archivo real</t>
+  </si>
+  <si>
+    <t>13/11/2025 se detecta que las imagenes no se pueden visualizar y es por un error de la extensión, asi que se hace desarrollo para que el sistema identifique si llega jpg y es pdf, le cambia la extención, para que cuando se arme el lote, el documento ya tenga la extensión correcta. 
+14/11/2025 Reporte de la inconsistencia para que corrigan desde el origen(otro proveedor)</t>
+  </si>
+  <si>
+    <t>OPT_27</t>
+  </si>
+  <si>
+    <t>Afiliaciones Pre - Llegan casos con imágenes repetidas en el xml, generando imágenes incompletas en el proceso</t>
+  </si>
+  <si>
+    <t>Opción para eliminar imágenes duplicadas dentro de la ya actual de reproceso de Afiliaciones Pre</t>
+  </si>
+  <si>
+    <t>Afiliaciones Pos - Más imágenes de las reportadas en el XML</t>
+  </si>
+  <si>
+    <t>Opción para adicionar documentos, algunas solicitudes quedan pendiente de proceso por que llegan más imágenes de las reportadas en el xml, generando inconsistencia</t>
+  </si>
+  <si>
     <t>Asignado</t>
   </si>
   <si>
@@ -1102,7 +1148,7 @@
     <t>True</t>
   </si>
   <si>
-    <t>False</t>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -2455,8 +2501,8 @@
   <dimension ref="A1:AM940"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P58" sqref="P58"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2601,7 +2647,7 @@
         <v>21</v>
       </c>
       <c r="Q2" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R2" s="27"/>
       <c r="S2" s="27"/>
@@ -2675,7 +2721,7 @@
         <v>24</v>
       </c>
       <c r="Q3" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R3" s="42"/>
       <c r="S3" s="42"/>
@@ -2749,7 +2795,7 @@
         <v>28</v>
       </c>
       <c r="Q4" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
@@ -2821,7 +2867,7 @@
         <v>32</v>
       </c>
       <c r="Q5" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R5" s="42"/>
       <c r="S5" s="42"/>
@@ -2895,7 +2941,7 @@
         <v>35</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="27"/>
@@ -2949,7 +2995,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32829</v>
+        <v>32842</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -2957,7 +3003,7 @@
         <v>40</v>
       </c>
       <c r="Q7" s="41" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="R7" s="42"/>
       <c r="S7" s="42"/>
@@ -3023,7 +3069,7 @@
         <v>43</v>
       </c>
       <c r="Q8" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
@@ -3095,7 +3141,7 @@
         <v>46</v>
       </c>
       <c r="Q9" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R9" s="42"/>
       <c r="S9" s="42"/>
@@ -3167,7 +3213,7 @@
         <v>49</v>
       </c>
       <c r="Q10" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R10" s="27"/>
       <c r="S10" s="27"/>
@@ -3241,7 +3287,7 @@
         <v>53</v>
       </c>
       <c r="Q11" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R11" s="42"/>
       <c r="S11" s="42"/>
@@ -3299,7 +3345,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f ca="1">IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3309,7 +3355,7 @@
         <v>57</v>
       </c>
       <c r="Q12" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
@@ -3381,7 +3427,7 @@
         <v>61</v>
       </c>
       <c r="Q13" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R13" s="42"/>
       <c r="S13" s="42"/>
@@ -3453,7 +3499,7 @@
         <v>65</v>
       </c>
       <c r="Q14" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R14" s="27"/>
       <c r="S14" s="27"/>
@@ -3525,7 +3571,7 @@
         <v>69</v>
       </c>
       <c r="Q15" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R15" s="42"/>
       <c r="S15" s="42"/>
@@ -3577,7 +3623,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f ca="1">IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32829</v>
+        <v>32842</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -3585,7 +3631,7 @@
         <v>73</v>
       </c>
       <c r="Q16" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R16" s="27"/>
       <c r="S16" s="27"/>
@@ -3659,7 +3705,7 @@
         <v>76</v>
       </c>
       <c r="Q17" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R17" s="42"/>
       <c r="S17" s="42"/>
@@ -3733,7 +3779,7 @@
         <v>80</v>
       </c>
       <c r="Q18" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R18" s="27"/>
       <c r="S18" s="27"/>
@@ -3803,7 +3849,7 @@
         <v>83</v>
       </c>
       <c r="Q19" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R19" s="42"/>
       <c r="S19" s="42"/>
@@ -3875,7 +3921,7 @@
       </c>
       <c r="P20" s="25"/>
       <c r="Q20" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R20" s="27"/>
       <c r="S20" s="27"/>
@@ -3947,7 +3993,7 @@
         <v>89</v>
       </c>
       <c r="Q21" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R21" s="42"/>
       <c r="S21" s="42"/>
@@ -4003,7 +4049,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f ca="1">IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -4011,7 +4057,7 @@
         <v>94</v>
       </c>
       <c r="Q22" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R22" s="27"/>
       <c r="S22" s="27"/>
@@ -4085,7 +4131,7 @@
         <v>98</v>
       </c>
       <c r="Q23" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R23" s="42"/>
       <c r="S23" s="42"/>
@@ -4143,7 +4189,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f ca="1">IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4151,7 +4197,7 @@
         <v>102</v>
       </c>
       <c r="Q24" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R24" s="27"/>
       <c r="S24" s="27"/>
@@ -4225,7 +4271,7 @@
         <v>106</v>
       </c>
       <c r="Q25" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R25" s="42"/>
       <c r="S25" s="42"/>
@@ -4275,13 +4321,13 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f ca="1">IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32829</v>
+        <v>32842</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
       <c r="P26" s="25"/>
       <c r="Q26" s="26" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="R26" s="27"/>
       <c r="S26" s="27"/>
@@ -4353,7 +4399,7 @@
         <v>112</v>
       </c>
       <c r="Q27" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R27" s="42"/>
       <c r="S27" s="42"/>
@@ -4413,7 +4459,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f ca="1">IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
@@ -4421,7 +4467,7 @@
         <v>117</v>
       </c>
       <c r="Q28" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R28" s="27"/>
       <c r="S28" s="27"/>
@@ -4495,7 +4541,7 @@
         <v>120</v>
       </c>
       <c r="Q29" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R29" s="42"/>
       <c r="S29" s="42"/>
@@ -4569,7 +4615,7 @@
         <v>123</v>
       </c>
       <c r="Q30" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R30" s="27"/>
       <c r="S30" s="27"/>
@@ -4643,7 +4689,7 @@
         <v>127</v>
       </c>
       <c r="Q31" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R31" s="42"/>
       <c r="S31" s="42"/>
@@ -4717,7 +4763,7 @@
         <v>131</v>
       </c>
       <c r="Q32" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R32" s="27"/>
       <c r="S32" s="27"/>
@@ -4791,7 +4837,7 @@
         <v>135</v>
       </c>
       <c r="Q33" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R33" s="42"/>
       <c r="S33" s="42"/>
@@ -4851,7 +4897,7 @@
       <c r="L34" s="23"/>
       <c r="M34" s="24">
         <f ca="1">IF(ISBLANK(L34), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L34, Hoja2!$A$1:$A$18))</f>
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
@@ -4859,7 +4905,7 @@
         <v>138</v>
       </c>
       <c r="Q34" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R34" s="27"/>
       <c r="S34" s="27"/>
@@ -4917,7 +4963,7 @@
       <c r="L35" s="38"/>
       <c r="M35" s="39">
         <f ca="1">IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="N35" s="38">
         <v>45938</v>
@@ -4929,7 +4975,7 @@
         <v>142</v>
       </c>
       <c r="Q35" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R35" s="46"/>
       <c r="S35" s="46"/>
@@ -4987,7 +5033,7 @@
       <c r="L36" s="23"/>
       <c r="M36" s="24">
         <f ca="1">IF(ISBLANK(L36), NETWORKDAYS(J36, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J36, L36, Hoja2!$A$1:$A$18))</f>
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
@@ -4995,7 +5041,7 @@
         <v>146</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R36" s="48"/>
       <c r="S36" s="48"/>
@@ -5053,7 +5099,7 @@
       <c r="L37" s="38"/>
       <c r="M37" s="39">
         <f ca="1">IF(ISBLANK(L37), NETWORKDAYS(J37, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J37, L37, Hoja2!$A$1:$A$18))</f>
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="N37" s="38">
         <v>45971</v>
@@ -5065,7 +5111,7 @@
         <v>150</v>
       </c>
       <c r="Q37" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R37" s="46"/>
       <c r="S37" s="46"/>
@@ -5121,7 +5167,7 @@
       <c r="L38" s="23"/>
       <c r="M38" s="24">
         <f ca="1">IF(ISBLANK(L38), NETWORKDAYS(J38, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J38, L38, Hoja2!$A$1:$A$18))</f>
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="N38" s="23"/>
       <c r="O38" s="23"/>
@@ -5129,7 +5175,7 @@
         <v>154</v>
       </c>
       <c r="Q38" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R38" s="48"/>
       <c r="S38" s="48"/>
@@ -5188,7 +5234,7 @@
       <c r="O39" s="38"/>
       <c r="P39" s="40"/>
       <c r="Q39" s="41" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="R39" s="46"/>
       <c r="S39" s="46"/>
@@ -5255,7 +5301,7 @@
         <v>161</v>
       </c>
       <c r="Q40" s="26" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R40" s="48"/>
       <c r="S40" s="48"/>
@@ -5322,7 +5368,7 @@
         <v>165</v>
       </c>
       <c r="Q41" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R41" s="46"/>
       <c r="S41" s="46"/>
@@ -5376,7 +5422,9 @@
       <c r="N42" s="23"/>
       <c r="O42" s="23"/>
       <c r="P42" s="25"/>
-      <c r="Q42" s="26"/>
+      <c r="Q42" s="26" t="s">
+        <v>287</v>
+      </c>
       <c r="R42" s="48"/>
       <c r="S42" s="48"/>
       <c r="T42" s="48"/>
@@ -5442,7 +5490,7 @@
         <v>171</v>
       </c>
       <c r="Q43" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="R43" s="46"/>
       <c r="S43" s="46"/>
@@ -5467,24 +5515,44 @@
       <c r="AL43" s="46"/>
       <c r="AM43" s="47"/>
     </row>
-    <row r="44" spans="1:39">
-      <c r="A44" s="13"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="16"/>
+    <row r="44" spans="1:39" ht="38.25">
+      <c r="A44" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>174</v>
+      </c>
       <c r="E44" s="17"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="19"/>
+      <c r="F44" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" s="19">
+        <v>100</v>
+      </c>
       <c r="H44" s="20"/>
-      <c r="I44" s="21"/>
+      <c r="I44" s="21">
+        <v>45973</v>
+      </c>
       <c r="J44" s="22"/>
       <c r="K44" s="23"/>
       <c r="L44" s="23"/>
       <c r="M44" s="24"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
+      <c r="N44" s="21">
+        <v>45973</v>
+      </c>
+      <c r="O44" s="21">
+        <v>45973</v>
+      </c>
       <c r="P44" s="25"/>
-      <c r="Q44" s="26"/>
+      <c r="Q44" s="26" t="s">
+        <v>286</v>
+      </c>
       <c r="R44" s="48"/>
       <c r="S44" s="48"/>
       <c r="T44" s="48"/>
@@ -5508,24 +5576,44 @@
       <c r="AL44" s="48"/>
       <c r="AM44" s="49"/>
     </row>
-    <row r="45" spans="1:39">
-      <c r="A45" s="28"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="31"/>
+    <row r="45" spans="1:39" ht="28.5">
+      <c r="A45" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>177</v>
+      </c>
       <c r="E45" s="32"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="34"/>
+      <c r="F45" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="34">
+        <v>100</v>
+      </c>
       <c r="H45" s="35"/>
-      <c r="I45" s="36"/>
+      <c r="I45" s="36">
+        <v>45973</v>
+      </c>
       <c r="J45" s="37"/>
       <c r="K45" s="38"/>
       <c r="L45" s="38"/>
       <c r="M45" s="39"/>
-      <c r="N45" s="38"/>
-      <c r="O45" s="38"/>
+      <c r="N45" s="36">
+        <v>45973</v>
+      </c>
+      <c r="O45" s="36">
+        <v>45973</v>
+      </c>
       <c r="P45" s="40"/>
-      <c r="Q45" s="41"/>
+      <c r="Q45" s="41" t="s">
+        <v>286</v>
+      </c>
       <c r="R45" s="46"/>
       <c r="S45" s="46"/>
       <c r="T45" s="46"/>
@@ -5549,24 +5637,42 @@
       <c r="AL45" s="46"/>
       <c r="AM45" s="47"/>
     </row>
-    <row r="46" spans="1:39">
-      <c r="A46" s="13"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="16"/>
+    <row r="46" spans="1:39" ht="42.75">
+      <c r="A46" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>180</v>
+      </c>
       <c r="E46" s="17"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="19"/>
+      <c r="F46" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" s="19">
+        <v>100</v>
+      </c>
       <c r="H46" s="20"/>
-      <c r="I46" s="21"/>
+      <c r="I46" s="21">
+        <v>45974</v>
+      </c>
       <c r="J46" s="22"/>
       <c r="K46" s="23"/>
       <c r="L46" s="23"/>
       <c r="M46" s="24"/>
       <c r="N46" s="23"/>
       <c r="O46" s="23"/>
-      <c r="P46" s="25"/>
-      <c r="Q46" s="26"/>
+      <c r="P46" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q46" s="26" t="s">
+        <v>286</v>
+      </c>
       <c r="R46" s="48"/>
       <c r="S46" s="48"/>
       <c r="T46" s="48"/>
@@ -5590,16 +5696,28 @@
       <c r="AL46" s="48"/>
       <c r="AM46" s="49"/>
     </row>
-    <row r="47" spans="1:39">
-      <c r="A47" s="28"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="31"/>
+    <row r="47" spans="1:39" ht="71.25">
+      <c r="A47" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>184</v>
+      </c>
       <c r="E47" s="32"/>
-      <c r="F47" s="33"/>
+      <c r="F47" s="33" t="s">
+        <v>39</v>
+      </c>
       <c r="G47" s="34"/>
       <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
+      <c r="I47" s="36">
+        <v>45980</v>
+      </c>
       <c r="J47" s="37"/>
       <c r="K47" s="38"/>
       <c r="L47" s="38"/>
@@ -5607,7 +5725,9 @@
       <c r="N47" s="38"/>
       <c r="O47" s="38"/>
       <c r="P47" s="40"/>
-      <c r="Q47" s="41"/>
+      <c r="Q47" s="41" t="s">
+        <v>287</v>
+      </c>
       <c r="R47" s="46"/>
       <c r="S47" s="46"/>
       <c r="T47" s="46"/>
@@ -5631,16 +5751,24 @@
       <c r="AL47" s="46"/>
       <c r="AM47" s="47"/>
     </row>
-    <row r="48" spans="1:39">
+    <row r="48" spans="1:39" ht="42.75">
       <c r="A48" s="13"/>
       <c r="B48" s="14"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="16"/>
+      <c r="C48" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>186</v>
+      </c>
       <c r="E48" s="17"/>
-      <c r="F48" s="18"/>
+      <c r="F48" s="18" t="s">
+        <v>39</v>
+      </c>
       <c r="G48" s="19"/>
       <c r="H48" s="20"/>
-      <c r="I48" s="21"/>
+      <c r="I48" s="21">
+        <v>45981</v>
+      </c>
       <c r="J48" s="22"/>
       <c r="K48" s="23"/>
       <c r="L48" s="23"/>
@@ -5648,7 +5776,9 @@
       <c r="N48" s="23"/>
       <c r="O48" s="23"/>
       <c r="P48" s="25"/>
-      <c r="Q48" s="26"/>
+      <c r="Q48" s="26" t="s">
+        <v>287</v>
+      </c>
       <c r="R48" s="48"/>
       <c r="S48" s="48"/>
       <c r="T48" s="48"/>
@@ -42292,7 +42422,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30">
       <c r="A1" s="86" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="B1" s="86" t="s">
         <v>2</v>
@@ -42319,13 +42449,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="89" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="K1" s="86" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="L1" s="90" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="M1" s="91"/>
       <c r="N1" s="91"/>
@@ -42344,14 +42474,14 @@
     </row>
     <row r="2" spans="1:26" ht="30">
       <c r="A2" s="92" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="B2" s="93" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="C2" s="94"/>
       <c r="D2" s="95" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="E2" s="96">
         <v>45526</v>
@@ -42365,7 +42495,7 @@
       <c r="J2" s="94"/>
       <c r="K2" s="94"/>
       <c r="L2" s="94" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="M2" s="97"/>
       <c r="N2" s="97"/>
@@ -42384,13 +42514,13 @@
     </row>
     <row r="3" spans="1:26" ht="28.5">
       <c r="A3" s="98" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="C3" s="100" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="D3" s="100" t="s">
         <v>20</v>
@@ -42414,7 +42544,7 @@
       </c>
       <c r="K3" s="102"/>
       <c r="L3" s="104" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="M3" s="91"/>
       <c r="N3" s="91"/>
@@ -42433,16 +42563,16 @@
     </row>
     <row r="4" spans="1:26" ht="186">
       <c r="A4" s="105" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="C4" s="105" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="D4" s="107" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="E4" s="108">
         <v>45581</v>
@@ -42465,7 +42595,7 @@
       </c>
       <c r="K4" s="108"/>
       <c r="L4" s="105" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="M4" s="111"/>
       <c r="N4" s="111"/>
@@ -42484,16 +42614,16 @@
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" s="90" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="D5" s="112" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="E5" s="101">
         <v>45572</v>
@@ -42514,7 +42644,7 @@
       </c>
       <c r="K5" s="101"/>
       <c r="L5" s="104" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="M5" s="91"/>
       <c r="N5" s="91"/>
@@ -42533,16 +42663,16 @@
     </row>
     <row r="6" spans="1:26" ht="117">
       <c r="A6" s="113" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="B6" s="113" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="C6" s="107" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="D6" s="113" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="E6" s="114">
         <v>45602</v>
@@ -42563,7 +42693,7 @@
         <v>45602</v>
       </c>
       <c r="L6" s="115" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="M6" s="116"/>
       <c r="N6" s="117"/>
@@ -42582,16 +42712,16 @@
     </row>
     <row r="7" spans="1:26" ht="99.75">
       <c r="A7" s="90" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="C7" s="118" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="D7" s="112" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="E7" s="101">
         <v>45589</v>
@@ -42612,7 +42742,7 @@
       </c>
       <c r="K7" s="112"/>
       <c r="L7" s="120" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="M7" s="121"/>
       <c r="N7" s="121"/>
@@ -42631,14 +42761,14 @@
     </row>
     <row r="8" spans="1:26" ht="71.25">
       <c r="A8" s="122" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="B8" s="123" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="C8" s="124"/>
       <c r="D8" s="124" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="E8" s="125">
         <v>45603</v>
@@ -42659,7 +42789,7 @@
       </c>
       <c r="K8" s="125"/>
       <c r="L8" s="127" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="M8" s="91"/>
       <c r="N8" s="91"/>
@@ -42678,16 +42808,16 @@
     </row>
     <row r="9" spans="1:26" ht="42.75">
       <c r="A9" s="128" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="B9" s="129" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="C9" s="130" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="D9" s="131" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="E9" s="132">
         <v>45671</v>
@@ -42696,7 +42826,7 @@
         <v>45673</v>
       </c>
       <c r="G9" s="130" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="H9" s="132">
         <v>45680</v>
@@ -42710,7 +42840,7 @@
       </c>
       <c r="K9" s="130"/>
       <c r="L9" s="134" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="M9" s="135"/>
       <c r="N9" s="135"/>
@@ -42729,14 +42859,14 @@
     </row>
     <row r="10" spans="1:26" ht="57">
       <c r="A10" s="128" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="B10" s="136"/>
       <c r="C10" s="134" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="D10" s="131" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="E10" s="132">
         <v>45671</v>
@@ -42755,7 +42885,7 @@
       <c r="J10" s="130"/>
       <c r="K10" s="130"/>
       <c r="L10" s="134" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="M10" s="135"/>
       <c r="N10" s="135"/>
@@ -42774,14 +42904,14 @@
     </row>
     <row r="11" spans="1:26" ht="42.75">
       <c r="A11" s="128" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="B11" s="136"/>
       <c r="C11" s="134" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="D11" s="131" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="E11" s="132">
         <v>45671</v>
@@ -42800,7 +42930,7 @@
       <c r="J11" s="130"/>
       <c r="K11" s="130"/>
       <c r="L11" s="134" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="M11" s="135"/>
       <c r="N11" s="135"/>
@@ -42819,14 +42949,14 @@
     </row>
     <row r="12" spans="1:26" ht="42.75">
       <c r="A12" s="128" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="B12" s="136"/>
       <c r="C12" s="134" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="D12" s="131" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="E12" s="132">
         <v>45671</v>
@@ -42845,7 +42975,7 @@
       <c r="J12" s="130"/>
       <c r="K12" s="130"/>
       <c r="L12" s="134" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="M12" s="135"/>
       <c r="N12" s="135"/>
@@ -42864,14 +42994,14 @@
     </row>
     <row r="13" spans="1:26" ht="42.75">
       <c r="A13" s="128" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="B13" s="136"/>
       <c r="C13" s="134" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="D13" s="131" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="E13" s="132">
         <v>45671</v>
@@ -42890,7 +43020,7 @@
       <c r="J13" s="130"/>
       <c r="K13" s="130"/>
       <c r="L13" s="134" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="M13" s="135"/>
       <c r="N13" s="135"/>
@@ -42909,14 +43039,14 @@
     </row>
     <row r="14" spans="1:26" ht="42.75">
       <c r="A14" s="128" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="B14" s="136"/>
       <c r="C14" s="134" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="D14" s="131" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="E14" s="132">
         <v>45671</v>
@@ -42935,7 +43065,7 @@
       <c r="J14" s="130"/>
       <c r="K14" s="130"/>
       <c r="L14" s="130" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="M14" s="135"/>
       <c r="N14" s="135"/>
@@ -42954,14 +43084,14 @@
     </row>
     <row r="15" spans="1:26" ht="42.75">
       <c r="A15" s="128" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="B15" s="136"/>
       <c r="C15" s="134" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="D15" s="131" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="E15" s="132">
         <v>45671</v>
@@ -42980,7 +43110,7 @@
       <c r="J15" s="130"/>
       <c r="K15" s="130"/>
       <c r="L15" s="130" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="M15" s="135"/>
       <c r="N15" s="135"/>
@@ -42999,14 +43129,14 @@
     </row>
     <row r="16" spans="1:26" ht="71.25">
       <c r="A16" s="128" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="B16" s="137"/>
       <c r="C16" s="138" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="D16" s="131" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="E16" s="132">
         <v>45681</v>
@@ -43025,7 +43155,7 @@
       <c r="J16" s="130"/>
       <c r="K16" s="130"/>
       <c r="L16" s="134" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="M16" s="135"/>
       <c r="N16" s="135"/>
@@ -49557,7 +49687,7 @@
         <v>45292</v>
       </c>
       <c r="B1" s="135" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
@@ -49565,7 +49695,7 @@
         <v>45299</v>
       </c>
       <c r="B2" s="135" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
@@ -49573,7 +49703,7 @@
         <v>45376</v>
       </c>
       <c r="B3" s="135" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
@@ -49581,7 +49711,7 @@
         <v>45379</v>
       </c>
       <c r="B4" s="135" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
@@ -49589,7 +49719,7 @@
         <v>45380</v>
       </c>
       <c r="B5" s="135" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1">
@@ -49597,7 +49727,7 @@
         <v>45413</v>
       </c>
       <c r="B6" s="135" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
@@ -49605,7 +49735,7 @@
         <v>45425</v>
       </c>
       <c r="B7" s="135" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
@@ -49613,7 +49743,7 @@
         <v>45446</v>
       </c>
       <c r="B8" s="135" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1">
@@ -49621,7 +49751,7 @@
         <v>45453</v>
       </c>
       <c r="B9" s="135" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1">
@@ -49629,7 +49759,7 @@
         <v>45474</v>
       </c>
       <c r="B10" s="135" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1">
@@ -49637,7 +49767,7 @@
         <v>45493</v>
       </c>
       <c r="B11" s="135" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" customHeight="1">
@@ -49645,7 +49775,7 @@
         <v>45511</v>
       </c>
       <c r="B12" s="135" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1">
@@ -49653,7 +49783,7 @@
         <v>45523</v>
       </c>
       <c r="B13" s="135" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" customHeight="1">
@@ -49661,7 +49791,7 @@
         <v>45579</v>
       </c>
       <c r="B14" s="135" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" customHeight="1">
@@ -49669,7 +49799,7 @@
         <v>45600</v>
       </c>
       <c r="B15" s="135" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1">
@@ -49677,7 +49807,7 @@
         <v>45607</v>
       </c>
       <c r="B16" s="135" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
@@ -49685,7 +49815,7 @@
         <v>45634</v>
       </c>
       <c r="B17" s="135" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1">
@@ -49693,7 +49823,7 @@
         <v>45651</v>
       </c>
       <c r="B18" s="135" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1"/>
@@ -50705,7 +50835,7 @@
   <sheetData>
     <row r="1" spans="1:97" ht="15.75">
       <c r="A1" s="140" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="B1" s="135"/>
       <c r="C1" s="135"/>
@@ -50763,7 +50893,7 @@
     </row>
     <row r="3" spans="1:97" ht="32.25" customHeight="1">
       <c r="A3" s="141" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="B3" s="142">
         <v>45596</v>
@@ -51056,261 +51186,261 @@
     </row>
     <row r="4" spans="1:97" ht="30.75" customHeight="1">
       <c r="A4" s="145" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="B4" s="146" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C4" s="147" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="D4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="E4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="F4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="G4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="H4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="J4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="K4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="L4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="M4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="N4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="O4" s="148" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="P4" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Q4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="R4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="S4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="T4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="U4" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="V4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="W4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="X4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Y4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Z4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AA4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AB4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AC4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AD4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AE4" s="174" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="AF4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AG4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AH4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AI4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AJ4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AK4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AL4" s="174" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="AM4" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AN4" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AO4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AP4" s="174" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="AQ4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AR4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AS4" s="174" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="AT4" s="150" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AU4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AV4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AW4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AX4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AY4" s="174" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="AZ4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BA4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BB4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BC4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BD4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BE4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BF4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BG4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BH4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BI4" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BJ4" s="174" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="BK4" s="149" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="BL4" s="149" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="BM4" s="149" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="BN4" s="149" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="BO4" s="149" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="BP4" s="149" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="BQ4" s="149" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="BR4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BS4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BT4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BU4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BV4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BW4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BX4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BY4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BZ4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CA4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CB4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CC4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CD4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CE4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CF4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CG4" s="148"/>
       <c r="CH4" s="148"/>
       <c r="CI4" s="174" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="CJ4" s="148"/>
       <c r="CK4" s="148"/>
@@ -51322,249 +51452,249 @@
       <c r="CQ4" s="148"/>
       <c r="CR4" s="148"/>
       <c r="CS4" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:97" ht="15.75" customHeight="1">
       <c r="A5" s="145" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="B5" s="146" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="D5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="E5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="F5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="G5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="H5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="J5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="K5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="L5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="M5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="N5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="O5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="P5" s="149" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="Q5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="R5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="S5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="T5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="U5" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="V5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="W5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="X5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Y5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Z5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AA5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AB5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AC5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AD5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AE5" s="175"/>
       <c r="AF5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AG5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AH5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AI5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AJ5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AK5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AL5" s="175"/>
       <c r="AM5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AN5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AO5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AP5" s="175"/>
       <c r="AQ5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="AR5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="AS5" s="175"/>
       <c r="AT5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="AU5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="AV5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="AW5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="AX5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="AY5" s="175"/>
       <c r="AZ5" s="148" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="BA5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BB5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BC5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BD5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BE5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BF5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BG5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BH5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BI5" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BJ5" s="175"/>
       <c r="BK5" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BL5" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BM5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BN5" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BO5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BP5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BQ5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BR5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BS5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BT5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BU5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BV5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BW5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BX5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BY5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BZ5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CA5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CB5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CC5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CD5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CE5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CF5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CG5" s="148"/>
       <c r="CH5" s="148"/>
@@ -51579,249 +51709,249 @@
       <c r="CQ5" s="148"/>
       <c r="CR5" s="148"/>
       <c r="CS5" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:97" ht="15.75">
       <c r="A6" s="145" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="B6" s="146" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="D6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="E6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="F6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="G6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="H6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="J6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="K6" s="151" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="L6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="M6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="N6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="O6" s="148" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="P6" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Q6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="R6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="S6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="T6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="U6" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="V6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="W6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="X6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Y6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Z6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AA6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AB6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AC6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AD6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AE6" s="175"/>
       <c r="AF6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AG6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AH6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AI6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AJ6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AK6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AL6" s="175"/>
       <c r="AM6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AN6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AO6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AP6" s="175"/>
       <c r="AQ6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AR6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AS6" s="175"/>
       <c r="AT6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AU6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AV6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AW6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AX6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AY6" s="175"/>
       <c r="AZ6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BA6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BB6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BC6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BD6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BE6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BF6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BG6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BH6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BI6" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BJ6" s="175"/>
       <c r="BK6" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BL6" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BM6" s="148" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="BN6" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BO6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BP6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BQ6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BR6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BS6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BT6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BU6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BV6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BW6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BX6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BY6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BZ6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CA6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CB6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CC6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CD6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CE6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CF6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CG6" s="148"/>
       <c r="CH6" s="148"/>
@@ -51836,198 +51966,198 @@
       <c r="CQ6" s="148"/>
       <c r="CR6" s="148"/>
       <c r="CS6" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="145" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="B7" s="146" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="D7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="E7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="F7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="G7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="H7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="J7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="K7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="L7" s="151" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="M7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="N7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="O7" s="148" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="P7" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Q7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="R7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="S7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="T7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="U7" s="149" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="V7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="W7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="X7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Y7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Z7" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AA7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AB7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AC7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AD7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AE7" s="175"/>
       <c r="AF7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AG7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AH7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AI7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AJ7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AK7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AL7" s="175"/>
       <c r="AM7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AN7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AO7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AP7" s="175"/>
       <c r="AQ7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AR7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AS7" s="175"/>
       <c r="AT7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AU7" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AV7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AW7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AX7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AY7" s="175"/>
       <c r="AZ7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BA7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BB7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BC7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BD7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BE7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BF7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BG7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BH7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BI7" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BJ7" s="175"/>
       <c r="BK7" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BL7" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BM7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BN7" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BO7" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BP7" s="148"/>
       <c r="BQ7" s="148"/>
@@ -52035,16 +52165,16 @@
       <c r="BS7" s="148"/>
       <c r="BT7" s="148"/>
       <c r="BU7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BV7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BW7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BX7" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BY7" s="148"/>
       <c r="BZ7" s="148"/>
@@ -52070,220 +52200,220 @@
     </row>
     <row r="8" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="145" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="B8" s="146" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="D8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="E8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="F8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="G8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="H8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="J8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="K8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="L8" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="M8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="N8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="O8" s="148" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="P8" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Q8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="R8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="S8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="T8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="U8" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="V8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="W8" s="148" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="X8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Y8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Z8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AA8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AB8" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AC8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AD8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AE8" s="175"/>
       <c r="AF8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AG8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AH8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AI8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AJ8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AK8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AL8" s="175"/>
       <c r="AM8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AN8" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AO8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AP8" s="175"/>
       <c r="AQ8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AR8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AS8" s="175"/>
       <c r="AT8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AU8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AV8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AW8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AX8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AY8" s="175"/>
       <c r="AZ8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BA8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BB8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BC8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BD8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BE8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BF8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BG8" s="148" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH8" s="148" t="s">
         <v>253</v>
       </c>
-      <c r="BH8" s="148" t="s">
-        <v>238</v>
-      </c>
       <c r="BI8" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BJ8" s="175"/>
       <c r="BK8" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BL8" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BM8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BN8" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BO8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BP8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BQ8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BR8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BS8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BT8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BU8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BV8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BW8" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BX8" s="148" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="BY8" s="148"/>
       <c r="BZ8" s="148"/>
@@ -52309,244 +52439,244 @@
     </row>
     <row r="9" spans="1:97" ht="15.75">
       <c r="A9" s="145" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="B9" s="146" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="D9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="E9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="F9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="G9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="H9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="J9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="K9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="L9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="M9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="N9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="O9" s="151" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="P9" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Q9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="R9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="S9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="T9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="U9" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="V9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="W9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="X9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Y9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Z9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AA9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AB9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AC9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AD9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AE9" s="175"/>
       <c r="AF9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AG9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AH9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AI9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AJ9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AK9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AL9" s="175"/>
       <c r="AM9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AN9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AO9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AP9" s="175"/>
       <c r="AQ9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AR9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AS9" s="175"/>
       <c r="AT9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AU9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AV9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AW9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AX9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AY9" s="175"/>
       <c r="AZ9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BA9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BB9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BC9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BD9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BE9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BF9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BG9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BH9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BI9" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BJ9" s="175"/>
       <c r="BK9" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BL9" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BM9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BN9" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BO9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BP9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BQ9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BR9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BS9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BT9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BU9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BV9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BW9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BX9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BY9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BZ9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CA9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CB9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CC9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CD9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CE9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CF9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CG9" s="148"/>
       <c r="CH9" s="148"/>
@@ -52561,249 +52691,249 @@
       <c r="CQ9" s="148"/>
       <c r="CR9" s="148"/>
       <c r="CS9" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:97" ht="15.75">
       <c r="A10" s="145" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10" s="146" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10" s="148" t="s">
+        <v>253</v>
+      </c>
+      <c r="D10" s="148" t="s">
+        <v>253</v>
+      </c>
+      <c r="E10" s="148" t="s">
+        <v>253</v>
+      </c>
+      <c r="F10" s="148" t="s">
+        <v>253</v>
+      </c>
+      <c r="G10" s="148" t="s">
+        <v>253</v>
+      </c>
+      <c r="H10" s="148" t="s">
+        <v>253</v>
+      </c>
+      <c r="I10" s="148" t="s">
         <v>256</v>
       </c>
-      <c r="B10" s="146" t="s">
-        <v>238</v>
-      </c>
-      <c r="C10" s="148" t="s">
-        <v>238</v>
-      </c>
-      <c r="D10" s="148" t="s">
-        <v>238</v>
-      </c>
-      <c r="E10" s="148" t="s">
-        <v>238</v>
-      </c>
-      <c r="F10" s="148" t="s">
-        <v>238</v>
-      </c>
-      <c r="G10" s="148" t="s">
-        <v>238</v>
-      </c>
-      <c r="H10" s="148" t="s">
-        <v>238</v>
-      </c>
-      <c r="I10" s="148" t="s">
-        <v>241</v>
-      </c>
       <c r="J10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="K10" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="L10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="M10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="N10" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="O10" s="148" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="P10" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="Q10" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="R10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="S10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="T10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="U10" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="V10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="W10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="X10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Y10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Z10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AA10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AB10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AC10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AD10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AE10" s="175"/>
       <c r="AF10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AG10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AH10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AI10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AJ10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AK10" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AL10" s="175"/>
       <c r="AM10" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AN10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AO10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AP10" s="175"/>
       <c r="AQ10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AR10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AS10" s="175"/>
       <c r="AT10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AU10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AV10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AW10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AX10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AY10" s="175"/>
       <c r="AZ10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BA10" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BB10" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BC10" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BD10" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BE10" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BF10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BG10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BH10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BI10" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BJ10" s="175"/>
       <c r="BK10" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BL10" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BM10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BN10" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BO10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BP10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BQ10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BR10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BS10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BT10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BU10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BV10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BW10" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BX10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BY10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BZ10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CA10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CB10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CC10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CD10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CE10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CF10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CG10" s="148"/>
       <c r="CH10" s="148"/>
@@ -52818,249 +52948,249 @@
       <c r="CQ10" s="148"/>
       <c r="CR10" s="148"/>
       <c r="CS10" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:97" ht="15.75">
       <c r="A11" s="145" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="B11" s="146" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="D11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="E11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="F11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="G11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="H11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="J11" s="148" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="K11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="L11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="M11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="N11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="O11" s="148" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="P11" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Q11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="R11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="S11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="T11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="U11" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="V11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="W11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="X11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Y11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Z11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AA11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AB11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AC11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AD11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AE11" s="175"/>
       <c r="AF11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AG11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AH11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AI11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AJ11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AK11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AL11" s="175"/>
       <c r="AM11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AN11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AO11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AP11" s="175"/>
       <c r="AQ11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AR11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AS11" s="175"/>
       <c r="AT11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AU11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AV11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AW11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AX11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AY11" s="175"/>
       <c r="AZ11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BA11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BB11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BC11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BD11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BE11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BF11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BG11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BH11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BI11" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BJ11" s="175"/>
       <c r="BK11" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BL11" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BM11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BN11" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BO11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BP11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BQ11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BR11" s="148" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="BS11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BT11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BU11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BV11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BW11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BX11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BY11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BZ11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CA11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CB11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="CC11" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="CD11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CE11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CF11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CG11" s="148"/>
       <c r="CH11" s="148"/>
@@ -53075,249 +53205,249 @@
       <c r="CQ11" s="148"/>
       <c r="CR11" s="148"/>
       <c r="CS11" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:97" ht="15.75">
       <c r="A12" s="145" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="B12" s="146" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="D12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="E12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="F12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="G12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="H12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="J12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="K12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="L12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="M12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="N12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="O12" s="148" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="P12" s="149" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="Q12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="R12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="S12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="T12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="U12" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="V12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="W12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="X12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="Y12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="Z12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AA12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AB12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AC12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AD12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AE12" s="175"/>
       <c r="AF12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AG12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AH12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AI12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AJ12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AK12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AL12" s="175"/>
       <c r="AM12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AN12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AO12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AP12" s="175"/>
       <c r="AQ12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AR12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AS12" s="175"/>
       <c r="AT12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AU12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AV12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AW12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AX12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AY12" s="175"/>
       <c r="AZ12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BA12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BB12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BC12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BD12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BE12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BF12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BG12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BH12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BI12" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BJ12" s="175"/>
       <c r="BK12" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BL12" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BM12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BN12" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BO12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BP12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BQ12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BR12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BS12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BT12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BU12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BV12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BW12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BX12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BY12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="BZ12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="CA12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="CB12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CC12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="CD12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="CE12" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CF12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="CG12" s="148"/>
       <c r="CH12" s="148"/>
@@ -53332,249 +53462,249 @@
       <c r="CQ12" s="148"/>
       <c r="CR12" s="148"/>
       <c r="CS12" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:97" ht="15.75">
       <c r="A13" s="145" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="B13" s="146" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="D13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="E13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="F13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="G13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="H13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="I13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="J13" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="K13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="L13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="M13" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="N13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="O13" s="148" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="P13" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="Q13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="R13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="S13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="T13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="U13" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="V13" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="W13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="X13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="Y13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="Z13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AA13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AB13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AC13" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AD13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AE13" s="176"/>
       <c r="AF13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AG13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AH13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AI13" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="AJ13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AK13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AL13" s="176"/>
       <c r="AM13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AN13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AO13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AP13" s="176"/>
       <c r="AQ13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AR13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AS13" s="176"/>
       <c r="AT13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AU13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AV13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AW13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AX13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="AY13" s="176"/>
       <c r="AZ13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BA13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BB13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BC13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BD13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BE13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BF13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BG13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BH13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BI13" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BJ13" s="176"/>
       <c r="BK13" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BL13" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BM13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BN13" s="149" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BO13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BP13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BQ13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BR13" s="148" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="BS13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BT13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BU13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BV13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BW13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BX13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BY13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="BZ13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="CA13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="CB13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="CC13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="CD13" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CE13" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CF13" s="148" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="CG13" s="148"/>
       <c r="CH13" s="148"/>
@@ -53589,7 +53719,7 @@
       <c r="CQ13" s="148"/>
       <c r="CR13" s="148"/>
       <c r="CS13" s="148" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54611,7 +54741,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="25.5">
       <c r="A1" s="152" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="B1" s="152" t="s">
         <v>2</v>
@@ -54638,13 +54768,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="156" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="K1" s="157" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="L1" s="155" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="M1" s="158"/>
       <c r="N1" s="158"/>
@@ -54663,10 +54793,10 @@
     </row>
     <row r="2" spans="1:26" ht="38.25">
       <c r="A2" s="159" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="B2" s="160" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="C2" s="161"/>
       <c r="D2" s="161" t="s">
@@ -54693,7 +54823,7 @@
       </c>
       <c r="K2" s="164"/>
       <c r="L2" s="165" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="M2" s="158"/>
       <c r="N2" s="158"/>
@@ -54712,13 +54842,13 @@
     </row>
     <row r="3" spans="1:26" ht="51">
       <c r="A3" s="159" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="B3" s="177" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
       <c r="C3" s="166" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="D3" s="161" t="s">
         <v>39</v>
@@ -54740,7 +54870,7 @@
       </c>
       <c r="K3" s="162"/>
       <c r="L3" s="165" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="M3" s="167"/>
       <c r="N3" s="158"/>
@@ -54759,11 +54889,11 @@
     </row>
     <row r="4" spans="1:26" ht="51">
       <c r="A4" s="159" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="B4" s="175"/>
       <c r="C4" s="168" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="D4" s="161" t="s">
         <v>39</v>
@@ -54785,7 +54915,7 @@
       </c>
       <c r="K4" s="169"/>
       <c r="L4" s="172" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="M4" s="167"/>
       <c r="N4" s="158"/>
@@ -54804,13 +54934,13 @@
     </row>
     <row r="5" spans="1:26" ht="51">
       <c r="A5" s="159" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="B5" s="155" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="C5" s="161" t="s">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="D5" s="161" t="s">
         <v>39</v>
@@ -54832,7 +54962,7 @@
       </c>
       <c r="K5" s="162"/>
       <c r="L5" s="165" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="M5" s="167"/>
       <c r="N5" s="158"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 18 Diciembre
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="303">
   <si>
     <t>Asignado a</t>
   </si>
@@ -789,7 +789,9 @@
 </t>
   </si>
   <si>
-    <t>28/11/2025 Creacion de botón que permita la ajecución del proceso de busqueda documental</t>
+    <t>28/11/2025 Creacion de opcion por Administración que permita la ajecución del proceso de busqueda documental
+05/12/2025 se colocan las paginas que hacen la validación documental
+12/12/2025 se pasa a pruebas y produccion</t>
   </si>
   <si>
     <t>OPT_32</t>
@@ -801,7 +803,11 @@
     <t>Crear página que realice el consumo para poder traernos las imágenes de PBS, y evitar que Colmédica las deje de manera manual en un repositorio</t>
   </si>
   <si>
-    <t>10/12/2025 Entrega de web service por parte de Colmedica url de pruebas y documentacion</t>
+    <t xml:space="preserve">10/12/2025 Entrega de web service por parte de Colmedica url de pruebas y documentacion
+12/12/2025 pruebas de consumo manualmente, el web service no da respuesta de imágenes
+15/12/2026 reunión contextualizacion incosistencia, y se evidencia que los id no son correctos para hacer los consumos, el proveedor debe hacer ajustes en el XML y el otro proveedor crear documentos de PBS
+17/12/2026 entregan el ajuste de los documentos, se hace nuevamente la prueba manual del consumo y ya se recibe el base64, sin embargo solo se pudieron consumir los documentos principales, ninguno de los adjuntos llega con id para el consumo, se reporta de nuevo al proveedor para que revisen
+</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -1194,10 +1200,10 @@
     <t>Internal Server Error</t>
   </si>
   <si>
-    <t>False</t>
+    <t>True</t>
   </si>
   <si>
-    <t>true</t>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -2550,8 +2556,8 @@
   <dimension ref="A1:AM940"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2696,7 +2702,7 @@
         <v>21</v>
       </c>
       <c r="Q2" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R2" s="27"/>
       <c r="S2" s="27"/>
@@ -2770,7 +2776,7 @@
         <v>24</v>
       </c>
       <c r="Q3" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R3" s="42"/>
       <c r="S3" s="42"/>
@@ -2844,7 +2850,7 @@
         <v>28</v>
       </c>
       <c r="Q4" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R4" s="27"/>
       <c r="S4" s="27"/>
@@ -2916,7 +2922,7 @@
         <v>32</v>
       </c>
       <c r="Q5" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R5" s="42"/>
       <c r="S5" s="42"/>
@@ -2990,7 +2996,7 @@
         <v>35</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="27"/>
@@ -3044,7 +3050,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32844</v>
+        <v>32848</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -3052,7 +3058,7 @@
         <v>40</v>
       </c>
       <c r="Q7" s="41" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="R7" s="42"/>
       <c r="S7" s="42"/>
@@ -3118,7 +3124,7 @@
         <v>43</v>
       </c>
       <c r="Q8" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="27"/>
@@ -3190,7 +3196,7 @@
         <v>46</v>
       </c>
       <c r="Q9" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R9" s="42"/>
       <c r="S9" s="42"/>
@@ -3262,7 +3268,7 @@
         <v>49</v>
       </c>
       <c r="Q10" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R10" s="27"/>
       <c r="S10" s="27"/>
@@ -3336,7 +3342,7 @@
         <v>53</v>
       </c>
       <c r="Q11" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R11" s="42"/>
       <c r="S11" s="42"/>
@@ -3394,7 +3400,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f ca="1">IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3404,7 +3410,7 @@
         <v>57</v>
       </c>
       <c r="Q12" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
@@ -3476,7 +3482,7 @@
         <v>61</v>
       </c>
       <c r="Q13" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R13" s="42"/>
       <c r="S13" s="42"/>
@@ -3548,7 +3554,7 @@
         <v>65</v>
       </c>
       <c r="Q14" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R14" s="27"/>
       <c r="S14" s="27"/>
@@ -3620,7 +3626,7 @@
         <v>69</v>
       </c>
       <c r="Q15" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R15" s="42"/>
       <c r="S15" s="42"/>
@@ -3672,7 +3678,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f ca="1">IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32844</v>
+        <v>32848</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -3680,7 +3686,7 @@
         <v>73</v>
       </c>
       <c r="Q16" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R16" s="27"/>
       <c r="S16" s="27"/>
@@ -3754,7 +3760,7 @@
         <v>76</v>
       </c>
       <c r="Q17" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R17" s="42"/>
       <c r="S17" s="42"/>
@@ -3828,7 +3834,7 @@
         <v>80</v>
       </c>
       <c r="Q18" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R18" s="27"/>
       <c r="S18" s="27"/>
@@ -3898,7 +3904,7 @@
         <v>83</v>
       </c>
       <c r="Q19" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R19" s="42"/>
       <c r="S19" s="42"/>
@@ -3970,7 +3976,7 @@
       </c>
       <c r="P20" s="25"/>
       <c r="Q20" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R20" s="27"/>
       <c r="S20" s="27"/>
@@ -4042,7 +4048,7 @@
         <v>89</v>
       </c>
       <c r="Q21" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R21" s="42"/>
       <c r="S21" s="42"/>
@@ -4098,7 +4104,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f ca="1">IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -4106,7 +4112,7 @@
         <v>94</v>
       </c>
       <c r="Q22" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R22" s="27"/>
       <c r="S22" s="27"/>
@@ -4180,7 +4186,7 @@
         <v>98</v>
       </c>
       <c r="Q23" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R23" s="42"/>
       <c r="S23" s="42"/>
@@ -4238,7 +4244,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f ca="1">IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4246,7 +4252,7 @@
         <v>102</v>
       </c>
       <c r="Q24" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R24" s="27"/>
       <c r="S24" s="27"/>
@@ -4320,7 +4326,7 @@
         <v>106</v>
       </c>
       <c r="Q25" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R25" s="42"/>
       <c r="S25" s="42"/>
@@ -4370,13 +4376,13 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f ca="1">IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32844</v>
+        <v>32848</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
       <c r="P26" s="25"/>
       <c r="Q26" s="26" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="R26" s="27"/>
       <c r="S26" s="27"/>
@@ -4448,7 +4454,7 @@
         <v>112</v>
       </c>
       <c r="Q27" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R27" s="42"/>
       <c r="S27" s="42"/>
@@ -4508,7 +4514,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f ca="1">IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
@@ -4516,7 +4522,7 @@
         <v>117</v>
       </c>
       <c r="Q28" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R28" s="27"/>
       <c r="S28" s="27"/>
@@ -4590,7 +4596,7 @@
         <v>120</v>
       </c>
       <c r="Q29" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R29" s="42"/>
       <c r="S29" s="42"/>
@@ -4664,7 +4670,7 @@
         <v>123</v>
       </c>
       <c r="Q30" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R30" s="27"/>
       <c r="S30" s="27"/>
@@ -4738,7 +4744,7 @@
         <v>127</v>
       </c>
       <c r="Q31" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R31" s="42"/>
       <c r="S31" s="42"/>
@@ -4812,7 +4818,7 @@
         <v>131</v>
       </c>
       <c r="Q32" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R32" s="27"/>
       <c r="S32" s="27"/>
@@ -4886,7 +4892,7 @@
         <v>135</v>
       </c>
       <c r="Q33" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R33" s="42"/>
       <c r="S33" s="42"/>
@@ -4946,7 +4952,7 @@
       <c r="L34" s="23"/>
       <c r="M34" s="24">
         <f ca="1">IF(ISBLANK(L34), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L34, Hoja2!$A$1:$A$18))</f>
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
@@ -4954,7 +4960,7 @@
         <v>138</v>
       </c>
       <c r="Q34" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R34" s="27"/>
       <c r="S34" s="27"/>
@@ -5012,7 +5018,7 @@
       <c r="L35" s="38"/>
       <c r="M35" s="39">
         <f ca="1">IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="N35" s="38">
         <v>45938</v>
@@ -5024,7 +5030,7 @@
         <v>142</v>
       </c>
       <c r="Q35" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R35" s="46"/>
       <c r="S35" s="46"/>
@@ -5082,7 +5088,7 @@
       <c r="L36" s="23"/>
       <c r="M36" s="24">
         <f ca="1">IF(ISBLANK(L36), NETWORKDAYS(J36, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J36, L36, Hoja2!$A$1:$A$18))</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
@@ -5090,7 +5096,7 @@
         <v>146</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R36" s="48"/>
       <c r="S36" s="48"/>
@@ -5148,7 +5154,7 @@
       <c r="L37" s="38"/>
       <c r="M37" s="39">
         <f ca="1">IF(ISBLANK(L37), NETWORKDAYS(J37, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J37, L37, Hoja2!$A$1:$A$18))</f>
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="N37" s="38">
         <v>45971</v>
@@ -5160,7 +5166,7 @@
         <v>150</v>
       </c>
       <c r="Q37" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R37" s="46"/>
       <c r="S37" s="46"/>
@@ -5216,7 +5222,7 @@
       <c r="L38" s="23"/>
       <c r="M38" s="24">
         <f ca="1">IF(ISBLANK(L38), NETWORKDAYS(J38, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J38, L38, Hoja2!$A$1:$A$18))</f>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="N38" s="23"/>
       <c r="O38" s="23"/>
@@ -5224,7 +5230,7 @@
         <v>154</v>
       </c>
       <c r="Q38" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R38" s="48"/>
       <c r="S38" s="48"/>
@@ -5278,12 +5284,15 @@
         <v>45979</v>
       </c>
       <c r="L39" s="38"/>
-      <c r="M39" s="39"/>
+      <c r="M39" s="39">
+        <f ca="1">IF(ISBLANK(L39), NETWORKDAYS(J39, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J39, L39, Hoja2!$A$1:$A$18))</f>
+        <v>32848</v>
+      </c>
       <c r="N39" s="38"/>
       <c r="O39" s="38"/>
       <c r="P39" s="40"/>
       <c r="Q39" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R39" s="46"/>
       <c r="S39" s="46"/>
@@ -5339,7 +5348,10 @@
         <v>45975</v>
       </c>
       <c r="L40" s="23"/>
-      <c r="M40" s="24"/>
+      <c r="M40" s="24">
+        <f ca="1">IF(ISBLANK(L40), NETWORKDAYS(J40, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J40, L40, Hoja2!$A$1:$A$18))</f>
+        <v>30</v>
+      </c>
       <c r="N40" s="23">
         <v>45981</v>
       </c>
@@ -5350,7 +5362,7 @@
         <v>161</v>
       </c>
       <c r="Q40" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R40" s="48"/>
       <c r="S40" s="48"/>
@@ -5406,7 +5418,10 @@
         <v>45975</v>
       </c>
       <c r="L41" s="38"/>
-      <c r="M41" s="39"/>
+      <c r="M41" s="39">
+        <f ca="1">IF(ISBLANK(L41), NETWORKDAYS(J41, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J41, L41, Hoja2!$A$1:$A$18))</f>
+        <v>30</v>
+      </c>
       <c r="N41" s="38">
         <v>45981</v>
       </c>
@@ -5417,7 +5432,7 @@
         <v>165</v>
       </c>
       <c r="Q41" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R41" s="46"/>
       <c r="S41" s="46"/>
@@ -5467,12 +5482,15 @@
       <c r="J42" s="22"/>
       <c r="K42" s="23"/>
       <c r="L42" s="23"/>
-      <c r="M42" s="24"/>
+      <c r="M42" s="24">
+        <f ca="1">IF(ISBLANK(L42), NETWORKDAYS(J42, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J42, L42, Hoja2!$A$1:$A$18))</f>
+        <v>32848</v>
+      </c>
       <c r="N42" s="23"/>
       <c r="O42" s="23"/>
       <c r="P42" s="25"/>
       <c r="Q42" s="26" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="R42" s="48"/>
       <c r="S42" s="48"/>
@@ -5528,7 +5546,10 @@
         <v>45981</v>
       </c>
       <c r="L43" s="38"/>
-      <c r="M43" s="39"/>
+      <c r="M43" s="39">
+        <f ca="1">IF(ISBLANK(L43), NETWORKDAYS(J43, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J43, L43, Hoja2!$A$1:$A$18))</f>
+        <v>21</v>
+      </c>
       <c r="N43" s="38">
         <v>45981</v>
       </c>
@@ -5539,7 +5560,7 @@
         <v>171</v>
       </c>
       <c r="Q43" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R43" s="46"/>
       <c r="S43" s="46"/>
@@ -5591,7 +5612,10 @@
       <c r="J44" s="22"/>
       <c r="K44" s="23"/>
       <c r="L44" s="23"/>
-      <c r="M44" s="24"/>
+      <c r="M44" s="24">
+        <f ca="1">IF(ISBLANK(L44), NETWORKDAYS(J44, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J44, L44, Hoja2!$A$1:$A$18))</f>
+        <v>32848</v>
+      </c>
       <c r="N44" s="21">
         <v>45973</v>
       </c>
@@ -5600,7 +5624,7 @@
       </c>
       <c r="P44" s="25"/>
       <c r="Q44" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R44" s="48"/>
       <c r="S44" s="48"/>
@@ -5652,7 +5676,10 @@
       <c r="J45" s="37"/>
       <c r="K45" s="38"/>
       <c r="L45" s="38"/>
-      <c r="M45" s="39"/>
+      <c r="M45" s="39">
+        <f ca="1">IF(ISBLANK(L45), NETWORKDAYS(J45, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J45, L45, Hoja2!$A$1:$A$18))</f>
+        <v>32848</v>
+      </c>
       <c r="N45" s="36">
         <v>45973</v>
       </c>
@@ -5661,7 +5688,7 @@
       </c>
       <c r="P45" s="40"/>
       <c r="Q45" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R45" s="46"/>
       <c r="S45" s="46"/>
@@ -5713,7 +5740,10 @@
       <c r="J46" s="22"/>
       <c r="K46" s="23"/>
       <c r="L46" s="23"/>
-      <c r="M46" s="24"/>
+      <c r="M46" s="24">
+        <f ca="1">IF(ISBLANK(L46), NETWORKDAYS(J46, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J46, L46, Hoja2!$A$1:$A$18))</f>
+        <v>32848</v>
+      </c>
       <c r="N46" s="23">
         <v>45979</v>
       </c>
@@ -5724,7 +5754,7 @@
         <v>181</v>
       </c>
       <c r="Q46" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R46" s="48"/>
       <c r="S46" s="48"/>
@@ -5776,12 +5806,15 @@
       <c r="J47" s="37"/>
       <c r="K47" s="38"/>
       <c r="L47" s="38"/>
-      <c r="M47" s="39"/>
+      <c r="M47" s="39">
+        <f ca="1">IF(ISBLANK(L47), NETWORKDAYS(J47, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J47, L47, Hoja2!$A$1:$A$18))</f>
+        <v>32848</v>
+      </c>
       <c r="N47" s="38"/>
       <c r="O47" s="38"/>
       <c r="P47" s="40"/>
       <c r="Q47" s="41" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="R47" s="46"/>
       <c r="S47" s="46"/>
@@ -5833,12 +5866,15 @@
       <c r="J48" s="22"/>
       <c r="K48" s="23"/>
       <c r="L48" s="23"/>
-      <c r="M48" s="24"/>
+      <c r="M48" s="24">
+        <f ca="1">IF(ISBLANK(L48), NETWORKDAYS(J48, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J48, L48, Hoja2!$A$1:$A$18))</f>
+        <v>32848</v>
+      </c>
       <c r="N48" s="23"/>
       <c r="O48" s="23"/>
       <c r="P48" s="25"/>
       <c r="Q48" s="26" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="R48" s="48"/>
       <c r="S48" s="48"/>
@@ -5888,11 +5924,16 @@
       <c r="J49" s="37"/>
       <c r="K49" s="38"/>
       <c r="L49" s="38"/>
-      <c r="M49" s="39"/>
+      <c r="M49" s="39">
+        <f ca="1">IF(ISBLANK(L49), NETWORKDAYS(J49, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J49, L49, Hoja2!$A$1:$A$18))</f>
+        <v>32848</v>
+      </c>
       <c r="N49" s="38"/>
       <c r="O49" s="38"/>
       <c r="P49" s="40"/>
-      <c r="Q49" s="41"/>
+      <c r="Q49" s="26" t="s">
+        <v>302</v>
+      </c>
       <c r="R49" s="46"/>
       <c r="S49" s="46"/>
       <c r="T49" s="46"/>
@@ -5931,7 +5972,7 @@
       </c>
       <c r="E50" s="17"/>
       <c r="F50" s="18" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="G50" s="19">
         <v>0</v>
@@ -5940,17 +5981,24 @@
       <c r="I50" s="21">
         <v>45988</v>
       </c>
-      <c r="J50" s="22"/>
-      <c r="K50" s="23"/>
+      <c r="J50" s="22">
+        <v>46009</v>
+      </c>
+      <c r="K50" s="23">
+        <v>46017</v>
+      </c>
       <c r="L50" s="23"/>
-      <c r="M50" s="24"/>
+      <c r="M50" s="24">
+        <f ca="1">IF(ISBLANK(L50), NETWORKDAYS(J50, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J50, L50, Hoja2!$A$1:$A$18))</f>
+        <v>1</v>
+      </c>
       <c r="N50" s="23"/>
       <c r="O50" s="23"/>
       <c r="P50" s="25" t="s">
         <v>193</v>
       </c>
       <c r="Q50" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R50" s="48"/>
       <c r="S50" s="48"/>
@@ -5990,26 +6038,39 @@
       </c>
       <c r="E51" s="32"/>
       <c r="F51" s="33" t="s">
-        <v>115</v>
+        <v>20</v>
       </c>
       <c r="G51" s="34">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="H51" s="35"/>
       <c r="I51" s="36">
         <v>45989</v>
       </c>
-      <c r="J51" s="37"/>
-      <c r="K51" s="38"/>
-      <c r="L51" s="38"/>
-      <c r="M51" s="39"/>
-      <c r="N51" s="38"/>
-      <c r="O51" s="38"/>
+      <c r="J51" s="37">
+        <v>45989</v>
+      </c>
+      <c r="K51" s="38">
+        <v>45996</v>
+      </c>
+      <c r="L51" s="38">
+        <v>45996</v>
+      </c>
+      <c r="M51" s="39">
+        <f ca="1">IF(ISBLANK(L51), NETWORKDAYS(J51, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J51, L51, Hoja2!$A$1:$A$18))</f>
+        <v>6</v>
+      </c>
+      <c r="N51" s="38">
+        <v>46003</v>
+      </c>
+      <c r="O51" s="38">
+        <v>46003</v>
+      </c>
       <c r="P51" s="40" t="s">
         <v>197</v>
       </c>
-      <c r="Q51" s="26" t="s">
-        <v>302</v>
+      <c r="Q51" s="41" t="s">
+        <v>301</v>
       </c>
       <c r="R51" s="46"/>
       <c r="S51" s="46"/>
@@ -6052,7 +6113,7 @@
         <v>115</v>
       </c>
       <c r="G52" s="19">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H52" s="20"/>
       <c r="I52" s="21">
@@ -6061,14 +6122,17 @@
       <c r="J52" s="22"/>
       <c r="K52" s="23"/>
       <c r="L52" s="23"/>
-      <c r="M52" s="24"/>
+      <c r="M52" s="24">
+        <f ca="1">IF(ISBLANK(L52), NETWORKDAYS(J52, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J52, L52, Hoja2!$A$1:$A$18))</f>
+        <v>32848</v>
+      </c>
       <c r="N52" s="23"/>
       <c r="O52" s="23"/>
       <c r="P52" s="25" t="s">
         <v>201</v>
       </c>
       <c r="Q52" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="R52" s="48"/>
       <c r="S52" s="48"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 23  Diciembre
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -803,11 +803,11 @@
     <t>Crear página que realice el consumo para poder traernos las imágenes de PBS, y evitar que Colmédica las deje de manera manual en un repositorio</t>
   </si>
   <si>
-    <t xml:space="preserve">10/12/2025 Entrega de web service por parte de Colmedica url de pruebas y documentacion
+    <t>10/12/2025 Entrega de web service por parte de Colmedica url de pruebas y documentacion
 12/12/2025 pruebas de consumo manualmente, el web service no da respuesta de imágenes
-15/12/2026 reunión contextualizacion incosistencia, y se evidencia que los id no son correctos para hacer los consumos, el proveedor debe hacer ajustes en el XML y el otro proveedor crear documentos de PBS
-17/12/2026 entregan el ajuste de los documentos, se hace nuevamente la prueba manual del consumo y ya se recibe el base64, sin embargo solo se pudieron consumir los documentos principales, ninguno de los adjuntos llega con id para el consumo, se reporta de nuevo al proveedor para que revisen
-</t>
+15/12/2025 reunión contextualizacion incosistencia, y se evidencia que los id no son correctos para hacer los consumos, el proveedor debe hacer ajustes en el XML y el otro proveedor crear documentos de PBS
+17/12/2025 entregan el ajuste de los documentos, se hace nuevamente la prueba manual del consumo y ya se recibe el base64, sin embargo solo se pudieron consumir los documentos principales, ninguno de los adjuntos llega con id para el consumo, se reporta de nuevo al proveedor para que revisen
+23/12/2025 Informa, que ya hicieron los ajustes en el XML para poder consumor los soportes adjuntos, se realizan las pruebas en Ambiente de pruebas, y se pudo hacer el consumo e los documentos.</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -1835,7 +1835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2326,6 +2326,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2555,9 +2558,9 @@
   </sheetPr>
   <dimension ref="A1:AM940"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R52" sqref="R52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -3050,7 +3053,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -3400,7 +3403,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f ca="1">IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3678,7 +3681,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f ca="1">IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -4104,7 +4107,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f ca="1">IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -4244,7 +4247,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f ca="1">IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4376,7 +4379,7 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f ca="1">IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
@@ -4514,7 +4517,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f ca="1">IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
@@ -4952,7 +4955,7 @@
       <c r="L34" s="23"/>
       <c r="M34" s="24">
         <f ca="1">IF(ISBLANK(L34), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L34, Hoja2!$A$1:$A$18))</f>
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
@@ -5018,7 +5021,7 @@
       <c r="L35" s="38"/>
       <c r="M35" s="39">
         <f ca="1">IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="N35" s="38">
         <v>45938</v>
@@ -5088,7 +5091,7 @@
       <c r="L36" s="23"/>
       <c r="M36" s="24">
         <f ca="1">IF(ISBLANK(L36), NETWORKDAYS(J36, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J36, L36, Hoja2!$A$1:$A$18))</f>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
@@ -5154,7 +5157,7 @@
       <c r="L37" s="38"/>
       <c r="M37" s="39">
         <f ca="1">IF(ISBLANK(L37), NETWORKDAYS(J37, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J37, L37, Hoja2!$A$1:$A$18))</f>
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="N37" s="38">
         <v>45971</v>
@@ -5222,7 +5225,7 @@
       <c r="L38" s="23"/>
       <c r="M38" s="24">
         <f ca="1">IF(ISBLANK(L38), NETWORKDAYS(J38, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J38, L38, Hoja2!$A$1:$A$18))</f>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="N38" s="23"/>
       <c r="O38" s="23"/>
@@ -5286,7 +5289,7 @@
       <c r="L39" s="38"/>
       <c r="M39" s="39">
         <f ca="1">IF(ISBLANK(L39), NETWORKDAYS(J39, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J39, L39, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N39" s="38"/>
       <c r="O39" s="38"/>
@@ -5350,7 +5353,7 @@
       <c r="L40" s="23"/>
       <c r="M40" s="24">
         <f ca="1">IF(ISBLANK(L40), NETWORKDAYS(J40, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J40, L40, Hoja2!$A$1:$A$18))</f>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N40" s="23">
         <v>45981</v>
@@ -5420,7 +5423,7 @@
       <c r="L41" s="38"/>
       <c r="M41" s="39">
         <f ca="1">IF(ISBLANK(L41), NETWORKDAYS(J41, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J41, L41, Hoja2!$A$1:$A$18))</f>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N41" s="38">
         <v>45981</v>
@@ -5484,7 +5487,7 @@
       <c r="L42" s="23"/>
       <c r="M42" s="24">
         <f ca="1">IF(ISBLANK(L42), NETWORKDAYS(J42, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J42, L42, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N42" s="23"/>
       <c r="O42" s="23"/>
@@ -5548,7 +5551,7 @@
       <c r="L43" s="38"/>
       <c r="M43" s="39">
         <f ca="1">IF(ISBLANK(L43), NETWORKDAYS(J43, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J43, L43, Hoja2!$A$1:$A$18))</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="N43" s="38">
         <v>45981</v>
@@ -5614,7 +5617,7 @@
       <c r="L44" s="23"/>
       <c r="M44" s="24">
         <f ca="1">IF(ISBLANK(L44), NETWORKDAYS(J44, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J44, L44, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N44" s="21">
         <v>45973</v>
@@ -5678,7 +5681,7 @@
       <c r="L45" s="38"/>
       <c r="M45" s="39">
         <f ca="1">IF(ISBLANK(L45), NETWORKDAYS(J45, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J45, L45, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N45" s="36">
         <v>45973</v>
@@ -5742,7 +5745,7 @@
       <c r="L46" s="23"/>
       <c r="M46" s="24">
         <f ca="1">IF(ISBLANK(L46), NETWORKDAYS(J46, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J46, L46, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N46" s="23">
         <v>45979</v>
@@ -5808,7 +5811,7 @@
       <c r="L47" s="38"/>
       <c r="M47" s="39">
         <f ca="1">IF(ISBLANK(L47), NETWORKDAYS(J47, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J47, L47, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N47" s="38"/>
       <c r="O47" s="38"/>
@@ -5868,7 +5871,7 @@
       <c r="L48" s="23"/>
       <c r="M48" s="24">
         <f ca="1">IF(ISBLANK(L48), NETWORKDAYS(J48, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J48, L48, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N48" s="23"/>
       <c r="O48" s="23"/>
@@ -5926,12 +5929,12 @@
       <c r="L49" s="38"/>
       <c r="M49" s="39">
         <f ca="1">IF(ISBLANK(L49), NETWORKDAYS(J49, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J49, L49, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N49" s="38"/>
       <c r="O49" s="38"/>
       <c r="P49" s="40"/>
-      <c r="Q49" s="26" t="s">
+      <c r="Q49" s="41" t="s">
         <v>302</v>
       </c>
       <c r="R49" s="46"/>
@@ -5990,7 +5993,7 @@
       <c r="L50" s="23"/>
       <c r="M50" s="24">
         <f ca="1">IF(ISBLANK(L50), NETWORKDAYS(J50, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J50, L50, Hoja2!$A$1:$A$18))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N50" s="23"/>
       <c r="O50" s="23"/>
@@ -6095,7 +6098,7 @@
       <c r="AL51" s="46"/>
       <c r="AM51" s="47"/>
     </row>
-    <row r="52" spans="1:39" ht="28.5">
+    <row r="52" spans="1:39" ht="267.75">
       <c r="A52" s="13" t="s">
         <v>36</v>
       </c>
@@ -6124,11 +6127,11 @@
       <c r="L52" s="23"/>
       <c r="M52" s="24">
         <f ca="1">IF(ISBLANK(L52), NETWORKDAYS(J52, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J52, L52, Hoja2!$A$1:$A$18))</f>
-        <v>32848</v>
+        <v>32851</v>
       </c>
       <c r="N52" s="23"/>
       <c r="O52" s="23"/>
-      <c r="P52" s="25" t="s">
+      <c r="P52" s="178" t="s">
         <v>201</v>
       </c>
       <c r="Q52" s="26" t="s">
@@ -42566,7 +42569,6 @@
       <c r="AM940" s="85"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q61"/>
   <conditionalFormatting sqref="B2:B61">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF(B$2:B$16,B2)&gt;1</formula>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 08 de enero 2026
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="306">
   <si>
     <t>Asignado a</t>
   </si>
@@ -813,6 +813,15 @@
 30/12/2025 ya se consumen en produccion las imágenes de las solicitudes y se crea la página que invocará el proceso de radicación, para que se vayan trayendo las imágenes a medida que se van radicando en el sistema
 5/01/2026 se hace hace la implementación en pruebas y consume sin problema las imágenes
 6/01/2026 se implementa en producción y se le hace seguimiento al proceso</t>
+  </si>
+  <si>
+    <t>Comercial - Modulo de Normalización</t>
+  </si>
+  <si>
+    <t>Mejoras al módulo para agilizar la auditoria y revisión de inconsistencias por parte de las Gestoras, ver inforción importante, eliminar datos innecesarios, mejorar ventana para visualización de información</t>
+  </si>
+  <si>
+    <t>7/01/2026 se hace reunión con el área comercial, para ver mejoras del módulode normalización, y mejorar la revisión de las solicitudes</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -3047,7 +3056,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f>IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32861</v>
+        <v>32863</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -3397,7 +3406,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f>IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3675,7 +3684,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f>IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32861</v>
+        <v>32863</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -4101,7 +4110,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f>IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -4241,7 +4250,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f>IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4375,7 +4384,7 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f>IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32861</v>
+        <v>32863</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
@@ -4513,7 +4522,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f>IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
@@ -4951,7 +4960,7 @@
       <c r="L34" s="23"/>
       <c r="M34" s="24">
         <f>IF(ISBLANK(L34), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L34, Hoja2!$A$1:$A$18))</f>
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
@@ -5017,7 +5026,7 @@
       <c r="L35" s="38"/>
       <c r="M35" s="39">
         <f>IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="N35" s="38">
         <v>45938.0</v>
@@ -5087,7 +5096,7 @@
       <c r="L36" s="23"/>
       <c r="M36" s="24">
         <f>IF(ISBLANK(L36), NETWORKDAYS(J36, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J36, L36, Hoja2!$A$1:$A$18))</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
@@ -5153,7 +5162,7 @@
       <c r="L37" s="38"/>
       <c r="M37" s="39">
         <f>IF(ISBLANK(L37), NETWORKDAYS(J37, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J37, L37, Hoja2!$A$1:$A$18))</f>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="N37" s="38">
         <v>45971.0</v>
@@ -5221,7 +5230,7 @@
       <c r="L38" s="23"/>
       <c r="M38" s="24">
         <f>IF(ISBLANK(L38), NETWORKDAYS(J38, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J38, L38, Hoja2!$A$1:$A$18))</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N38" s="23"/>
       <c r="O38" s="23"/>
@@ -5285,7 +5294,7 @@
       <c r="L39" s="38"/>
       <c r="M39" s="39">
         <f>IF(ISBLANK(L39), NETWORKDAYS(J39, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J39, L39, Hoja2!$A$1:$A$18))</f>
-        <v>32861</v>
+        <v>32863</v>
       </c>
       <c r="N39" s="38"/>
       <c r="O39" s="38"/>
@@ -5349,7 +5358,7 @@
       <c r="L40" s="23"/>
       <c r="M40" s="24">
         <f>IF(ISBLANK(L40), NETWORKDAYS(J40, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J40, L40, Hoja2!$A$1:$A$18))</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N40" s="23">
         <v>45981.0</v>
@@ -5419,7 +5428,7 @@
       <c r="L41" s="38"/>
       <c r="M41" s="39">
         <f>IF(ISBLANK(L41), NETWORKDAYS(J41, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J41, L41, Hoja2!$A$1:$A$18))</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N41" s="38">
         <v>45981.0</v>
@@ -5483,7 +5492,7 @@
       <c r="L42" s="23"/>
       <c r="M42" s="24">
         <f>IF(ISBLANK(L42), NETWORKDAYS(J42, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J42, L42, Hoja2!$A$1:$A$18))</f>
-        <v>32861</v>
+        <v>32863</v>
       </c>
       <c r="N42" s="23"/>
       <c r="O42" s="23"/>
@@ -5547,7 +5556,7 @@
       <c r="L43" s="38"/>
       <c r="M43" s="39">
         <f>IF(ISBLANK(L43), NETWORKDAYS(J43, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J43, L43, Hoja2!$A$1:$A$18))</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N43" s="38">
         <v>45981.0</v>
@@ -5613,7 +5622,7 @@
       <c r="L44" s="23"/>
       <c r="M44" s="24">
         <f>IF(ISBLANK(L44), NETWORKDAYS(J44, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J44, L44, Hoja2!$A$1:$A$18))</f>
-        <v>32861</v>
+        <v>32863</v>
       </c>
       <c r="N44" s="21">
         <v>45973.0</v>
@@ -5677,7 +5686,7 @@
       <c r="L45" s="38"/>
       <c r="M45" s="39">
         <f>IF(ISBLANK(L45), NETWORKDAYS(J45, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J45, L45, Hoja2!$A$1:$A$18))</f>
-        <v>32861</v>
+        <v>32863</v>
       </c>
       <c r="N45" s="36">
         <v>45973.0</v>
@@ -5741,7 +5750,7 @@
       <c r="L46" s="23"/>
       <c r="M46" s="24">
         <f>IF(ISBLANK(L46), NETWORKDAYS(J46, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J46, L46, Hoja2!$A$1:$A$18))</f>
-        <v>32861</v>
+        <v>32863</v>
       </c>
       <c r="N46" s="23">
         <v>45979.0</v>
@@ -5807,7 +5816,7 @@
       <c r="L47" s="38"/>
       <c r="M47" s="39">
         <f>IF(ISBLANK(L47), NETWORKDAYS(J47, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J47, L47, Hoja2!$A$1:$A$18))</f>
-        <v>32861</v>
+        <v>32863</v>
       </c>
       <c r="N47" s="38"/>
       <c r="O47" s="38"/>
@@ -5867,7 +5876,7 @@
       <c r="L48" s="23"/>
       <c r="M48" s="24">
         <f>IF(ISBLANK(L48), NETWORKDAYS(J48, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J48, L48, Hoja2!$A$1:$A$18))</f>
-        <v>32861</v>
+        <v>32863</v>
       </c>
       <c r="N48" s="23"/>
       <c r="O48" s="23"/>
@@ -5925,7 +5934,7 @@
       <c r="L49" s="38"/>
       <c r="M49" s="39">
         <f>IF(ISBLANK(L49), NETWORKDAYS(J49, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J49, L49, Hoja2!$A$1:$A$18))</f>
-        <v>32861</v>
+        <v>32863</v>
       </c>
       <c r="N49" s="38"/>
       <c r="O49" s="38"/>
@@ -6173,23 +6182,41 @@
       <c r="AM52" s="53"/>
     </row>
     <row r="53">
-      <c r="A53" s="28"/>
-      <c r="B53" s="29"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="31"/>
+      <c r="A53" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="D53" s="31" t="s">
+        <v>205</v>
+      </c>
       <c r="E53" s="32"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="34"/>
+      <c r="F53" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="G53" s="34">
+        <v>0.0</v>
+      </c>
       <c r="H53" s="35"/>
-      <c r="I53" s="36"/>
+      <c r="I53" s="36">
+        <v>46029.0</v>
+      </c>
       <c r="J53" s="37"/>
       <c r="K53" s="38"/>
       <c r="L53" s="38"/>
       <c r="M53" s="39"/>
       <c r="N53" s="38"/>
       <c r="O53" s="38"/>
-      <c r="P53" s="40"/>
-      <c r="Q53" s="41"/>
+      <c r="P53" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q53" s="43" t="s">
+        <v>44</v>
+      </c>
       <c r="R53" s="50"/>
       <c r="S53" s="50"/>
       <c r="T53" s="50"/>
@@ -42649,7 +42676,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="92" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B1" s="92" t="s">
         <v>2</v>
@@ -42676,13 +42703,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="95" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K1" s="92" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="L1" s="96" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="M1" s="97"/>
       <c r="N1" s="97"/>
@@ -42701,14 +42728,14 @@
     </row>
     <row r="2">
       <c r="A2" s="98" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C2" s="100"/>
       <c r="D2" s="101" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E2" s="102">
         <v>45526.0</v>
@@ -42722,7 +42749,7 @@
       <c r="J2" s="100"/>
       <c r="K2" s="100"/>
       <c r="L2" s="100" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="M2" s="103"/>
       <c r="N2" s="103"/>
@@ -42741,13 +42768,13 @@
     </row>
     <row r="3">
       <c r="A3" s="104" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C3" s="106" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D3" s="106" t="s">
         <v>20</v>
@@ -42771,7 +42798,7 @@
       </c>
       <c r="K3" s="108"/>
       <c r="L3" s="110" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="M3" s="97"/>
       <c r="N3" s="97"/>
@@ -42790,16 +42817,16 @@
     </row>
     <row r="4">
       <c r="A4" s="111" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B4" s="112" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C4" s="111" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D4" s="113" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E4" s="114">
         <v>45581.0</v>
@@ -42822,7 +42849,7 @@
       </c>
       <c r="K4" s="114"/>
       <c r="L4" s="111" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="M4" s="117"/>
       <c r="N4" s="117"/>
@@ -42841,16 +42868,16 @@
     </row>
     <row r="5">
       <c r="A5" s="96" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B5" s="112" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C5" s="106" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D5" s="118" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E5" s="107">
         <v>45572.0</v>
@@ -42871,7 +42898,7 @@
       </c>
       <c r="K5" s="107"/>
       <c r="L5" s="110" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="M5" s="97"/>
       <c r="N5" s="97"/>
@@ -42890,16 +42917,16 @@
     </row>
     <row r="6">
       <c r="A6" s="119" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B6" s="119" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C6" s="113" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D6" s="119" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E6" s="120">
         <v>45602.0</v>
@@ -42920,7 +42947,7 @@
         <v>45602.0</v>
       </c>
       <c r="L6" s="121" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="M6" s="122"/>
       <c r="N6" s="123"/>
@@ -42939,16 +42966,16 @@
     </row>
     <row r="7">
       <c r="A7" s="96" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C7" s="124" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D7" s="118" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E7" s="107">
         <v>45589.0</v>
@@ -42969,7 +42996,7 @@
       </c>
       <c r="K7" s="118"/>
       <c r="L7" s="126" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="M7" s="127"/>
       <c r="N7" s="127"/>
@@ -42988,14 +43015,14 @@
     </row>
     <row r="8">
       <c r="A8" s="128" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B8" s="129" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C8" s="130"/>
       <c r="D8" s="130" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E8" s="131">
         <v>45603.0</v>
@@ -43016,7 +43043,7 @@
       </c>
       <c r="K8" s="131"/>
       <c r="L8" s="133" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="M8" s="97"/>
       <c r="N8" s="97"/>
@@ -43035,16 +43062,16 @@
     </row>
     <row r="9">
       <c r="A9" s="134" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B9" s="135" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C9" s="136" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D9" s="137" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E9" s="138">
         <v>45671.0</v>
@@ -43053,7 +43080,7 @@
         <v>45673.0</v>
       </c>
       <c r="G9" s="136" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="H9" s="138">
         <v>45680.0</v>
@@ -43067,7 +43094,7 @@
       </c>
       <c r="K9" s="136"/>
       <c r="L9" s="140" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="M9" s="141"/>
       <c r="N9" s="141"/>
@@ -43086,14 +43113,14 @@
     </row>
     <row r="10">
       <c r="A10" s="134" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B10" s="142"/>
       <c r="C10" s="140" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" s="137" t="s">
         <v>240</v>
-      </c>
-      <c r="D10" s="137" t="s">
-        <v>237</v>
       </c>
       <c r="E10" s="138">
         <v>45671.0</v>
@@ -43112,7 +43139,7 @@
       <c r="J10" s="136"/>
       <c r="K10" s="136"/>
       <c r="L10" s="140" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="M10" s="141"/>
       <c r="N10" s="141"/>
@@ -43131,14 +43158,14 @@
     </row>
     <row r="11">
       <c r="A11" s="134" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B11" s="142"/>
       <c r="C11" s="140" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D11" s="137" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E11" s="138">
         <v>45671.0</v>
@@ -43157,7 +43184,7 @@
       <c r="J11" s="136"/>
       <c r="K11" s="136"/>
       <c r="L11" s="140" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="M11" s="141"/>
       <c r="N11" s="141"/>
@@ -43176,14 +43203,14 @@
     </row>
     <row r="12">
       <c r="A12" s="134" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B12" s="142"/>
       <c r="C12" s="140" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D12" s="137" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E12" s="138">
         <v>45671.0</v>
@@ -43202,7 +43229,7 @@
       <c r="J12" s="136"/>
       <c r="K12" s="136"/>
       <c r="L12" s="140" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="M12" s="141"/>
       <c r="N12" s="141"/>
@@ -43221,14 +43248,14 @@
     </row>
     <row r="13">
       <c r="A13" s="134" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B13" s="142"/>
       <c r="C13" s="140" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D13" s="137" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E13" s="138">
         <v>45671.0</v>
@@ -43247,7 +43274,7 @@
       <c r="J13" s="136"/>
       <c r="K13" s="136"/>
       <c r="L13" s="140" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="M13" s="141"/>
       <c r="N13" s="141"/>
@@ -43266,14 +43293,14 @@
     </row>
     <row r="14">
       <c r="A14" s="134" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B14" s="142"/>
       <c r="C14" s="140" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D14" s="137" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E14" s="138">
         <v>45671.0</v>
@@ -43292,7 +43319,7 @@
       <c r="J14" s="136"/>
       <c r="K14" s="136"/>
       <c r="L14" s="136" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="M14" s="141"/>
       <c r="N14" s="141"/>
@@ -43311,14 +43338,14 @@
     </row>
     <row r="15">
       <c r="A15" s="134" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B15" s="142"/>
       <c r="C15" s="140" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D15" s="137" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E15" s="138">
         <v>45671.0</v>
@@ -43337,7 +43364,7 @@
       <c r="J15" s="136"/>
       <c r="K15" s="136"/>
       <c r="L15" s="136" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="M15" s="141"/>
       <c r="N15" s="141"/>
@@ -43356,14 +43383,14 @@
     </row>
     <row r="16">
       <c r="A16" s="134" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B16" s="143"/>
       <c r="C16" s="144" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D16" s="137" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E16" s="138">
         <v>45681.0</v>
@@ -43382,7 +43409,7 @@
       <c r="J16" s="136"/>
       <c r="K16" s="136"/>
       <c r="L16" s="140" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="M16" s="141"/>
       <c r="N16" s="141"/>
@@ -49918,7 +49945,7 @@
         <v>45292.0</v>
       </c>
       <c r="B1" s="141" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
@@ -49926,7 +49953,7 @@
         <v>45299.0</v>
       </c>
       <c r="B2" s="141" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
@@ -49934,7 +49961,7 @@
         <v>45376.0</v>
       </c>
       <c r="B3" s="141" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1">
@@ -49942,7 +49969,7 @@
         <v>45379.0</v>
       </c>
       <c r="B4" s="141" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
@@ -49950,7 +49977,7 @@
         <v>45380.0</v>
       </c>
       <c r="B5" s="141" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
@@ -49958,7 +49985,7 @@
         <v>45413.0</v>
       </c>
       <c r="B6" s="141" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -49966,7 +49993,7 @@
         <v>45425.0</v>
       </c>
       <c r="B7" s="141" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1">
@@ -49974,7 +50001,7 @@
         <v>45446.0</v>
       </c>
       <c r="B8" s="141" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1">
@@ -49982,7 +50009,7 @@
         <v>45453.0</v>
       </c>
       <c r="B9" s="141" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
@@ -49990,7 +50017,7 @@
         <v>45474.0</v>
       </c>
       <c r="B10" s="141" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1">
@@ -49998,7 +50025,7 @@
         <v>45493.0</v>
       </c>
       <c r="B11" s="141" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1">
@@ -50006,7 +50033,7 @@
         <v>45511.0</v>
       </c>
       <c r="B12" s="141" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1">
@@ -50014,7 +50041,7 @@
         <v>45523.0</v>
       </c>
       <c r="B13" s="141" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1">
@@ -50022,7 +50049,7 @@
         <v>45579.0</v>
       </c>
       <c r="B14" s="141" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1">
@@ -50030,7 +50057,7 @@
         <v>45600.0</v>
       </c>
       <c r="B15" s="141" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1">
@@ -50038,7 +50065,7 @@
         <v>45607.0</v>
       </c>
       <c r="B16" s="141" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
@@ -50046,7 +50073,7 @@
         <v>45634.0</v>
       </c>
       <c r="B17" s="141" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1">
@@ -50054,7 +50081,7 @@
         <v>45651.0</v>
       </c>
       <c r="B18" s="141" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1"/>
@@ -51070,7 +51097,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="146" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B1" s="141"/>
       <c r="C1" s="141"/>
@@ -51128,7 +51155,7 @@
     </row>
     <row r="3" ht="32.25" customHeight="1">
       <c r="A3" s="147" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B3" s="148">
         <v>45596.0</v>
@@ -51421,261 +51448,261 @@
     </row>
     <row r="4" ht="30.75" customHeight="1">
       <c r="A4" s="151" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B4" s="152" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C4" s="153" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="J4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="K4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="L4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="M4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="N4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="O4" s="154" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="P4" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Q4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="R4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="S4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="T4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="U4" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="V4" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="V4" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="W4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="X4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Y4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Z4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AA4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AB4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AC4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AD4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AE4" s="156" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="AF4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AG4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AH4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AI4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AJ4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AK4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AL4" s="156" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="AM4" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AN4" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AO4" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="AN4" s="154" t="s">
+      <c r="AP4" s="156" t="s">
+        <v>279</v>
+      </c>
+      <c r="AQ4" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="AO4" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="AP4" s="156" t="s">
-        <v>276</v>
-      </c>
-      <c r="AQ4" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="AR4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AS4" s="156" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="AT4" s="157" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AU4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AV4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AW4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AX4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AY4" s="156" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="AZ4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BA4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BB4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BC4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BD4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BE4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BF4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BG4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BH4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BI4" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BJ4" s="156" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="BK4" s="155" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="BL4" s="155" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="BM4" s="155" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="BN4" s="155" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="BO4" s="155" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="BP4" s="155" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="BQ4" s="155" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="BR4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BS4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BT4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BU4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BV4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BW4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BX4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BY4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BZ4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CA4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CB4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CC4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CD4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CE4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CF4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CG4" s="154"/>
       <c r="CH4" s="154"/>
       <c r="CI4" s="156" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="CJ4" s="154"/>
       <c r="CK4" s="154"/>
@@ -51687,249 +51714,249 @@
       <c r="CQ4" s="154"/>
       <c r="CR4" s="154"/>
       <c r="CS4" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="151" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B5" s="152" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="J5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="K5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="L5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="M5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="N5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="O5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="P5" s="155" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="Q5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="R5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="S5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="T5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="U5" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="V5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="W5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="X5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Y5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Z5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AA5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AB5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AC5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AD5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AE5" s="158"/>
       <c r="AF5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AG5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AH5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AI5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AJ5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AK5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AL5" s="158"/>
       <c r="AM5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AN5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AO5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AP5" s="158"/>
       <c r="AQ5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="AR5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="AS5" s="158"/>
       <c r="AT5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="AU5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="AV5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="AW5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="AX5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="AY5" s="158"/>
       <c r="AZ5" s="154" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="BA5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BB5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BC5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BD5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BE5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BF5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BG5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BH5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BI5" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BJ5" s="158"/>
       <c r="BK5" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BL5" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BM5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BN5" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BO5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BP5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BQ5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BR5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BS5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BT5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BU5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BV5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BW5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BX5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BY5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BZ5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CA5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CB5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CC5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CD5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CE5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CF5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CG5" s="154"/>
       <c r="CH5" s="154"/>
@@ -51944,249 +51971,249 @@
       <c r="CQ5" s="154"/>
       <c r="CR5" s="154"/>
       <c r="CS5" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="151" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B6" s="152" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="J6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="K6" s="159" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="L6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="M6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="N6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="O6" s="154" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="P6" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Q6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="R6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="S6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="T6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="U6" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="V6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="W6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="X6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Y6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Z6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AA6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AB6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AC6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AD6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AE6" s="158"/>
       <c r="AF6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AG6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AH6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AI6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AJ6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AK6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AL6" s="158"/>
       <c r="AM6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AN6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AO6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AP6" s="158"/>
       <c r="AQ6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AR6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AS6" s="158"/>
       <c r="AT6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AU6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AV6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AW6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AX6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AY6" s="158"/>
       <c r="AZ6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BA6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BB6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BC6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BD6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BE6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BF6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BG6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BH6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BI6" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BJ6" s="158"/>
       <c r="BK6" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BL6" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BM6" s="154" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="BN6" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BO6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BP6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BQ6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BR6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BS6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BT6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BU6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BV6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BW6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BX6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BY6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BZ6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CA6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CB6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CC6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CD6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CE6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CF6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CG6" s="154"/>
       <c r="CH6" s="154"/>
@@ -52201,198 +52228,198 @@
       <c r="CQ6" s="154"/>
       <c r="CR6" s="154"/>
       <c r="CS6" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="151" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B7" s="152" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="J7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="K7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="L7" s="159" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="M7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="N7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="O7" s="154" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="P7" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Q7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="R7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="S7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="T7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="U7" s="155" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="V7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="W7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="X7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Y7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Z7" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AA7" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="AA7" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="AB7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AC7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AD7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AE7" s="158"/>
       <c r="AF7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AG7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AH7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AI7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AJ7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AK7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AL7" s="158"/>
       <c r="AM7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AN7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AO7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AP7" s="158"/>
       <c r="AQ7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AR7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AS7" s="158"/>
       <c r="AT7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AU7" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AV7" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="AV7" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="AW7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AX7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AY7" s="158"/>
       <c r="AZ7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BA7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BB7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BC7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BD7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BE7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BF7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BG7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BH7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BI7" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BJ7" s="158"/>
       <c r="BK7" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BL7" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BM7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BN7" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BO7" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BP7" s="154"/>
       <c r="BQ7" s="154"/>
@@ -52400,16 +52427,16 @@
       <c r="BS7" s="154"/>
       <c r="BT7" s="154"/>
       <c r="BU7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BV7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BW7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BX7" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BY7" s="154"/>
       <c r="BZ7" s="154"/>
@@ -52435,220 +52462,220 @@
     </row>
     <row r="8" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="151" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B8" s="152" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="J8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="K8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="L8" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="M8" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="M8" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="N8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="O8" s="154" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="P8" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Q8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="R8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="S8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="T8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="U8" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="V8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="W8" s="154" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="X8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Y8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Z8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AA8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AB8" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AC8" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="AC8" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="AD8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AE8" s="158"/>
       <c r="AF8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AG8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AH8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AI8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AJ8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AK8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AL8" s="158"/>
       <c r="AM8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AN8" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AO8" s="154" t="s">
         <v>273</v>
-      </c>
-      <c r="AO8" s="154" t="s">
-        <v>270</v>
       </c>
       <c r="AP8" s="158"/>
       <c r="AQ8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AR8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AS8" s="158"/>
       <c r="AT8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AU8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AV8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AW8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AX8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AY8" s="158"/>
       <c r="AZ8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BA8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BB8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BC8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BD8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BE8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BF8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BG8" s="154" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="BH8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BI8" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BJ8" s="158"/>
       <c r="BK8" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BL8" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BM8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BN8" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BO8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BP8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BQ8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BR8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BS8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BT8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BU8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BV8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BW8" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BX8" s="154" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="BY8" s="154"/>
       <c r="BZ8" s="154"/>
@@ -52674,244 +52701,244 @@
     </row>
     <row r="9">
       <c r="A9" s="151" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B9" s="152" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="J9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="K9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="L9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="M9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="N9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="O9" s="159" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="P9" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Q9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="R9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="S9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="T9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="U9" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="V9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="W9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="X9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Y9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Z9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AA9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AB9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AC9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AD9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AE9" s="158"/>
       <c r="AF9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AG9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AH9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AI9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AJ9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AK9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AL9" s="158"/>
       <c r="AM9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AN9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AO9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AP9" s="158"/>
       <c r="AQ9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AR9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AS9" s="158"/>
       <c r="AT9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AU9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AV9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AW9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AX9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AY9" s="158"/>
       <c r="AZ9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BA9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BB9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BC9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BD9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BE9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BF9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BG9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BH9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BI9" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BJ9" s="158"/>
       <c r="BK9" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BL9" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BM9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BN9" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BO9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BP9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BQ9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BR9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BS9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BT9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BU9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BV9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BW9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BX9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BY9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BZ9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CA9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CB9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CC9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CD9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CE9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CF9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CG9" s="154"/>
       <c r="CH9" s="154"/>
@@ -52926,249 +52953,249 @@
       <c r="CQ9" s="154"/>
       <c r="CR9" s="154"/>
       <c r="CS9" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="151" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B10" s="152" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I10" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="J10" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="J10" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="K10" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="L10" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="L10" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="M10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="N10" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="O10" s="154" t="s">
+        <v>275</v>
+      </c>
+      <c r="P10" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q10" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="R10" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="O10" s="154" t="s">
-        <v>272</v>
-      </c>
-      <c r="P10" s="155" t="s">
+      <c r="S10" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="Q10" s="154" t="s">
+      <c r="T10" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="R10" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="S10" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="T10" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="U10" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="V10" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="V10" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="W10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="X10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Y10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Z10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AA10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AB10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AC10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AD10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AE10" s="158"/>
       <c r="AF10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AG10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AH10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AI10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AJ10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AK10" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AL10" s="158"/>
       <c r="AM10" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AN10" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="AN10" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="AO10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AP10" s="158"/>
       <c r="AQ10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AR10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AS10" s="158"/>
       <c r="AT10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AU10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AV10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AW10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AX10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AY10" s="158"/>
       <c r="AZ10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BA10" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BB10" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BC10" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BD10" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BE10" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BF10" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BB10" s="154" t="s">
+      <c r="BG10" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BC10" s="154" t="s">
+      <c r="BH10" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BD10" s="154" t="s">
+      <c r="BI10" s="155" t="s">
         <v>273</v>
-      </c>
-      <c r="BE10" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BF10" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="BG10" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="BH10" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="BI10" s="155" t="s">
-        <v>270</v>
       </c>
       <c r="BJ10" s="158"/>
       <c r="BK10" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BL10" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BM10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BN10" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BO10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BP10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BQ10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BR10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BS10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BT10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BU10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BV10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BW10" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BX10" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BX10" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="BY10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BZ10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CA10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CB10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CC10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CD10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CE10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CF10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CG10" s="154"/>
       <c r="CH10" s="154"/>
@@ -53183,249 +53210,249 @@
       <c r="CQ10" s="154"/>
       <c r="CR10" s="154"/>
       <c r="CS10" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="151" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B11" s="152" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="J11" s="154" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="K11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="L11" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="L11" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="M11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="N11" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="N11" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="O11" s="154" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="P11" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Q11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="R11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="S11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="T11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="U11" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="V11" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="T11" s="154" t="s">
+      <c r="W11" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="U11" s="155" t="s">
+      <c r="X11" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="V11" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="W11" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="X11" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="Y11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Z11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AA11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AB11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AC11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AD11" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AE11" s="158"/>
       <c r="AF11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AG11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AH11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AI11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AJ11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AK11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AL11" s="158"/>
       <c r="AM11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AN11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AO11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AP11" s="158"/>
       <c r="AQ11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AR11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AS11" s="158"/>
       <c r="AT11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AU11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AV11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AW11" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="AV11" s="154" t="s">
+      <c r="AX11" s="154" t="s">
         <v>273</v>
-      </c>
-      <c r="AW11" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="AX11" s="154" t="s">
-        <v>270</v>
       </c>
       <c r="AY11" s="158"/>
       <c r="AZ11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BA11" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BA11" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="BB11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BC11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BD11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BE11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BF11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BG11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BH11" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BF11" s="154" t="s">
+      <c r="BI11" s="155" t="s">
         <v>273</v>
-      </c>
-      <c r="BG11" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BH11" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="BI11" s="155" t="s">
-        <v>270</v>
       </c>
       <c r="BJ11" s="158"/>
       <c r="BK11" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BL11" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BM11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BN11" s="155" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BO11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BP11" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BP11" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="BQ11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BR11" s="154" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="BS11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BT11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BU11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BV11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BW11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BX11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BY11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="BZ11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CA11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CB11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="CC11" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="CD11" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="CC11" s="154" t="s">
+      <c r="CE11" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="CD11" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="CE11" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="CF11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="CG11" s="154"/>
       <c r="CH11" s="154"/>
@@ -53440,249 +53467,249 @@
       <c r="CQ11" s="154"/>
       <c r="CR11" s="154"/>
       <c r="CS11" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="151" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B12" s="152" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="D12" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="E12" s="154" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="G12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="H12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="G12" s="154" t="s">
+      <c r="I12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="J12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="H12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="I12" s="154" t="s">
+      <c r="K12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="L12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="J12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="K12" s="154" t="s">
+      <c r="M12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="N12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="O12" s="154" t="s">
+        <v>275</v>
+      </c>
+      <c r="P12" s="155" t="s">
         <v>273</v>
       </c>
-      <c r="L12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="M12" s="154" t="s">
+      <c r="Q12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="R12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="S12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="T12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="U12" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="V12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="W12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="N12" s="154" t="s">
+      <c r="X12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="Y12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="Z12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="O12" s="154" t="s">
-        <v>272</v>
-      </c>
-      <c r="P12" s="155" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q12" s="154" t="s">
+      <c r="AA12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AB12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AC12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="R12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="S12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="T12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="U12" s="155" t="s">
-        <v>273</v>
-      </c>
-      <c r="V12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="W12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="X12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="Y12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="Z12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="AA12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="AB12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="AC12" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="AD12" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AE12" s="158"/>
       <c r="AF12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AH12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AI12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AJ12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="AG12" s="154" t="s">
+      <c r="AK12" s="154" t="s">
         <v>273</v>
-      </c>
-      <c r="AH12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="AI12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="AJ12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="AK12" s="154" t="s">
-        <v>270</v>
       </c>
       <c r="AL12" s="158"/>
       <c r="AM12" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AN12" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AO12" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AP12" s="158"/>
       <c r="AQ12" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AR12" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AS12" s="158"/>
       <c r="AT12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AU12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AV12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="AU12" s="154" t="s">
+      <c r="AW12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="AV12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="AW12" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="AX12" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AY12" s="158"/>
       <c r="AZ12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BA12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BB12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BC12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BA12" s="154" t="s">
+      <c r="BD12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BE12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BB12" s="154" t="s">
+      <c r="BF12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BG12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BH12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BC12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="BD12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BE12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="BF12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BG12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BH12" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="BI12" s="155" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BJ12" s="158"/>
       <c r="BK12" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="BL12" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="BM12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BL12" s="155" t="s">
+      <c r="BN12" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="BO12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BP12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BQ12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BR12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BM12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="BN12" s="155" t="s">
+      <c r="BS12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BT12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BU12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BO12" s="154" t="s">
+      <c r="BV12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BP12" s="154" t="s">
+      <c r="BW12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BX12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BY12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BQ12" s="154" t="s">
+      <c r="BZ12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="CA12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="CB12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BR12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="BS12" s="154" t="s">
+      <c r="CC12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="CD12" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="CE12" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BT12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BU12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="BV12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="BW12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BX12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BY12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="BZ12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="CA12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="CB12" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="CC12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="CD12" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="CE12" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="CF12" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="CG12" s="154"/>
       <c r="CH12" s="154"/>
@@ -53697,249 +53724,249 @@
       <c r="CQ12" s="154"/>
       <c r="CR12" s="154"/>
       <c r="CS12" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="151" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B13" s="152" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="E13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="F13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="G13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="H13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="I13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="J13" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="D13" s="154" t="s">
+      <c r="K13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="L13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="M13" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="E13" s="154" t="s">
+      <c r="N13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="O13" s="154" t="s">
+        <v>275</v>
+      </c>
+      <c r="P13" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="R13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="S13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="T13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="U13" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="V13" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="F13" s="154" t="s">
+      <c r="W13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="X13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="Y13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="Z13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AA13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AB13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AC13" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="G13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="H13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="I13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="J13" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="K13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="L13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="M13" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="N13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="O13" s="154" t="s">
-        <v>272</v>
-      </c>
-      <c r="P13" s="155" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="R13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="S13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="T13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="U13" s="155" t="s">
-        <v>273</v>
-      </c>
-      <c r="V13" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="W13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="X13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="Y13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="Z13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="AA13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="AB13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="AC13" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="AD13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AE13" s="160"/>
       <c r="AF13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AH13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="AI13" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="AG13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="AH13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="AI13" s="154" t="s">
-        <v>270</v>
-      </c>
       <c r="AJ13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AK13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AL13" s="160"/>
       <c r="AM13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AN13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AO13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AP13" s="160"/>
       <c r="AQ13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AR13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AS13" s="160"/>
       <c r="AT13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AU13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AV13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AW13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AX13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="AY13" s="160"/>
       <c r="AZ13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BA13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BB13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BC13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BD13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BE13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BF13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BG13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BH13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BI13" s="155" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="BJ13" s="160"/>
       <c r="BK13" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="BL13" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="BM13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BN13" s="155" t="s">
+        <v>276</v>
+      </c>
+      <c r="BO13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BP13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BQ13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BR13" s="154" t="s">
+        <v>294</v>
+      </c>
+      <c r="BS13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BT13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BU13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BV13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BW13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BX13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BY13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="BZ13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="CA13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="CB13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="CC13" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="CD13" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BL13" s="155" t="s">
+      <c r="CE13" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="BM13" s="154" t="s">
+      <c r="CF13" s="154" t="s">
         <v>273</v>
-      </c>
-      <c r="BN13" s="155" t="s">
-        <v>273</v>
-      </c>
-      <c r="BO13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BP13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BQ13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BR13" s="154" t="s">
-        <v>291</v>
-      </c>
-      <c r="BS13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BT13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BU13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BV13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BW13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BX13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BY13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BZ13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="CA13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="CB13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="CC13" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="CD13" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="CE13" s="154" t="s">
-        <v>270</v>
-      </c>
-      <c r="CF13" s="154" t="s">
-        <v>270</v>
       </c>
       <c r="CG13" s="154"/>
       <c r="CH13" s="154"/>
@@ -53954,7 +53981,7 @@
       <c r="CQ13" s="154"/>
       <c r="CR13" s="154"/>
       <c r="CS13" s="154" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -54980,7 +55007,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="161" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B1" s="161" t="s">
         <v>2</v>
@@ -55007,13 +55034,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="165" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="K1" s="166" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="L1" s="164" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="M1" s="167"/>
       <c r="N1" s="167"/>
@@ -55032,10 +55059,10 @@
     </row>
     <row r="2">
       <c r="A2" s="168" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B2" s="169" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C2" s="170"/>
       <c r="D2" s="170" t="s">
@@ -55062,7 +55089,7 @@
       </c>
       <c r="K2" s="173"/>
       <c r="L2" s="174" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="M2" s="167"/>
       <c r="N2" s="167"/>
@@ -55081,13 +55108,13 @@
     </row>
     <row r="3">
       <c r="A3" s="168" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B3" s="175" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C3" s="176" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="D3" s="170" t="s">
         <v>38</v>
@@ -55109,7 +55136,7 @@
       </c>
       <c r="K3" s="171"/>
       <c r="L3" s="174" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="M3" s="177"/>
       <c r="N3" s="167"/>
@@ -55128,11 +55155,11 @@
     </row>
     <row r="4">
       <c r="A4" s="168" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B4" s="158"/>
       <c r="C4" s="178" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="D4" s="170" t="s">
         <v>38</v>
@@ -55154,7 +55181,7 @@
       </c>
       <c r="K4" s="179"/>
       <c r="L4" s="182" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="M4" s="177"/>
       <c r="N4" s="167"/>
@@ -55173,13 +55200,13 @@
     </row>
     <row r="5">
       <c r="A5" s="168" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B5" s="164" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C5" s="170" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D5" s="170" t="s">
         <v>38</v>
@@ -55201,7 +55228,7 @@
       </c>
       <c r="K5" s="171"/>
       <c r="L5" s="174" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="M5" s="177"/>
       <c r="N5" s="167"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 16  de enero 2026
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="314">
   <si>
     <t>Asignado a</t>
   </si>
@@ -839,10 +839,22 @@
     <t>En la validación de los 7 campos importantes que se toman del soporte de identificación, si ya existe en la base de afiliados se completará la información con dicha data para que en la operación no la capturen pero si la validen</t>
   </si>
   <si>
-    <t>13/01/2026 en la opción de selección de lote que llena la tabla con la info del lote a validar con las identificaciones de titular y beneficiarios, se adiciona query para traer datos de la base de afiliados pre.</t>
+    <t>13/01/2026 en la opción de selección de lote que llena la tabla con la info del lote a validar con las identificaciones de titular y beneficiarios, se adiciona query para traer datos de la base de afiliados pre y si no está de afiliados pos</t>
   </si>
   <si>
     <t>Afiliaciones Pos - Validación 7 campos</t>
+  </si>
+  <si>
+    <t>14/01/2026 en la opción de selección de lote que llena la tabla con la info del lote a validar con las identificaciones de cotizante y beneficiarios, se adiciona query para traer datos de la base de afiliados pre y si no está de afiliados pos</t>
+  </si>
+  <si>
+    <t>Riesgo Médico - Informe General de Auditoria</t>
+  </si>
+  <si>
+    <t>Revisar la generación de la data de seguimiento de la revisión por parte del área médica, e identificar posibles errores en el query o impresión, dado que se evidenciaron registros duplicados</t>
+  </si>
+  <si>
+    <t>15/01/2026 revisar la generación actual del informe generla del módulo de Riesgo médico</t>
   </si>
   <si>
     <t>Asignado</t>
@@ -2591,8 +2603,8 @@
   <dimension ref="A1:AM940"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -3056,7 +3068,7 @@
       <c r="AL6" s="27"/>
       <c r="AM6" s="27"/>
     </row>
-    <row r="7" spans="1:39" ht="53.25" hidden="1" customHeight="1">
+    <row r="7" spans="1:39" ht="53.25" customHeight="1">
       <c r="A7" s="28" t="s">
         <v>35</v>
       </c>
@@ -3085,7 +3097,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="39">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
@@ -3435,7 +3447,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="24">
         <f ca="1">IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23">
@@ -3713,7 +3725,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="24">
         <f ca="1">IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -4139,7 +4151,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="24">
         <f ca="1">IF(ISBLANK(L22), NETWORKDAYS(J22, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J22, L22, Hoja2!$A$1:$A$18))</f>
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
@@ -4279,7 +4291,7 @@
       <c r="L24" s="23"/>
       <c r="M24" s="24">
         <f ca="1">IF(ISBLANK(L24), NETWORKDAYS(J24, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J24, L24, Hoja2!$A$1:$A$18))</f>
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="N24" s="23"/>
       <c r="O24" s="23"/>
@@ -4413,7 +4425,7 @@
       <c r="L26" s="23"/>
       <c r="M26" s="24">
         <f ca="1">IF(ISBLANK(L26), NETWORKDAYS(J26, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J26, L26, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
@@ -4551,7 +4563,7 @@
       <c r="L28" s="23"/>
       <c r="M28" s="24">
         <f ca="1">IF(ISBLANK(L28), NETWORKDAYS(J28, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J28, L28, Hoja2!$A$1:$A$18))</f>
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
@@ -4989,7 +5001,7 @@
       <c r="L34" s="23"/>
       <c r="M34" s="24">
         <f ca="1">IF(ISBLANK(L34), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L34, Hoja2!$A$1:$A$18))</f>
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
@@ -5055,7 +5067,7 @@
       <c r="L35" s="38"/>
       <c r="M35" s="39">
         <f ca="1">IF(ISBLANK(L35), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L35, Hoja2!$A$1:$A$18))</f>
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="N35" s="38">
         <v>45938</v>
@@ -5125,7 +5137,7 @@
       <c r="L36" s="23"/>
       <c r="M36" s="24">
         <f ca="1">IF(ISBLANK(L36), NETWORKDAYS(J36, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J36, L36, Hoja2!$A$1:$A$18))</f>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
@@ -5191,7 +5203,7 @@
       <c r="L37" s="38"/>
       <c r="M37" s="39">
         <f ca="1">IF(ISBLANK(L37), NETWORKDAYS(J37, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J37, L37, Hoja2!$A$1:$A$18))</f>
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N37" s="38">
         <v>45971</v>
@@ -5259,7 +5271,7 @@
       <c r="L38" s="23"/>
       <c r="M38" s="24">
         <f ca="1">IF(ISBLANK(L38), NETWORKDAYS(J38, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J38, L38, Hoja2!$A$1:$A$18))</f>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N38" s="23"/>
       <c r="O38" s="23"/>
@@ -5323,7 +5335,7 @@
       <c r="L39" s="38"/>
       <c r="M39" s="39">
         <f ca="1">IF(ISBLANK(L39), NETWORKDAYS(J39, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J39, L39, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N39" s="38"/>
       <c r="O39" s="38"/>
@@ -5387,7 +5399,7 @@
       <c r="L40" s="23"/>
       <c r="M40" s="24">
         <f ca="1">IF(ISBLANK(L40), NETWORKDAYS(J40, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J40, L40, Hoja2!$A$1:$A$18))</f>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N40" s="23">
         <v>45981</v>
@@ -5457,7 +5469,7 @@
       <c r="L41" s="38"/>
       <c r="M41" s="39">
         <f ca="1">IF(ISBLANK(L41), NETWORKDAYS(J41, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J41, L41, Hoja2!$A$1:$A$18))</f>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N41" s="38">
         <v>45981</v>
@@ -5494,7 +5506,7 @@
       <c r="AL41" s="50"/>
       <c r="AM41" s="51"/>
     </row>
-    <row r="42" spans="1:39" ht="42.75" hidden="1">
+    <row r="42" spans="1:39" ht="42.75">
       <c r="A42" s="13" t="s">
         <v>35</v>
       </c>
@@ -5521,7 +5533,7 @@
       <c r="L42" s="23"/>
       <c r="M42" s="24">
         <f ca="1">IF(ISBLANK(L42), NETWORKDAYS(J42, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J42, L42, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N42" s="23"/>
       <c r="O42" s="23"/>
@@ -5585,7 +5597,7 @@
       <c r="L43" s="38"/>
       <c r="M43" s="39">
         <f ca="1">IF(ISBLANK(L43), NETWORKDAYS(J43, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J43, L43, Hoja2!$A$1:$A$18))</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N43" s="38">
         <v>45981</v>
@@ -5651,7 +5663,7 @@
       <c r="L44" s="23"/>
       <c r="M44" s="24">
         <f ca="1">IF(ISBLANK(L44), NETWORKDAYS(J44, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J44, L44, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N44" s="21">
         <v>45973</v>
@@ -5715,7 +5727,7 @@
       <c r="L45" s="38"/>
       <c r="M45" s="39">
         <f ca="1">IF(ISBLANK(L45), NETWORKDAYS(J45, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J45, L45, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N45" s="36">
         <v>45973</v>
@@ -5779,7 +5791,7 @@
       <c r="L46" s="23"/>
       <c r="M46" s="24">
         <f ca="1">IF(ISBLANK(L46), NETWORKDAYS(J46, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J46, L46, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N46" s="23">
         <v>45979</v>
@@ -5816,7 +5828,7 @@
       <c r="AL46" s="52"/>
       <c r="AM46" s="53"/>
     </row>
-    <row r="47" spans="1:39" ht="71.25" hidden="1">
+    <row r="47" spans="1:39" ht="71.25">
       <c r="A47" s="28" t="s">
         <v>35</v>
       </c>
@@ -5845,7 +5857,7 @@
       <c r="L47" s="38"/>
       <c r="M47" s="39">
         <f ca="1">IF(ISBLANK(L47), NETWORKDAYS(J47, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J47, L47, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N47" s="38"/>
       <c r="O47" s="38"/>
@@ -5876,7 +5888,7 @@
       <c r="AL47" s="50"/>
       <c r="AM47" s="51"/>
     </row>
-    <row r="48" spans="1:39" ht="42.75" hidden="1">
+    <row r="48" spans="1:39" ht="42.75">
       <c r="A48" s="13" t="s">
         <v>35</v>
       </c>
@@ -5905,7 +5917,7 @@
       <c r="L48" s="23"/>
       <c r="M48" s="24">
         <f ca="1">IF(ISBLANK(L48), NETWORKDAYS(J48, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J48, L48, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N48" s="23"/>
       <c r="O48" s="23"/>
@@ -5936,7 +5948,7 @@
       <c r="AL48" s="52"/>
       <c r="AM48" s="53"/>
     </row>
-    <row r="49" spans="1:39" ht="57" hidden="1">
+    <row r="49" spans="1:39" ht="57">
       <c r="A49" s="28" t="s">
         <v>35</v>
       </c>
@@ -5963,7 +5975,7 @@
       <c r="L49" s="38"/>
       <c r="M49" s="39">
         <f ca="1">IF(ISBLANK(L49), NETWORKDAYS(J49, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J49, L49, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N49" s="38"/>
       <c r="O49" s="38"/>
@@ -6239,7 +6251,7 @@
       <c r="L53" s="38"/>
       <c r="M53" s="39">
         <f ca="1">IF(ISBLANK(L53), NETWORKDAYS(J53, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J53, L53, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N53" s="38"/>
       <c r="O53" s="38"/>
@@ -6305,7 +6317,7 @@
       <c r="L54" s="23"/>
       <c r="M54" s="24">
         <f ca="1">IF(ISBLANK(L54), NETWORKDAYS(J54, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J54, L54, Hoja2!$A$1:$A$18))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N54" s="23">
         <v>46035</v>
@@ -6357,10 +6369,10 @@
       </c>
       <c r="E55" s="32"/>
       <c r="F55" s="33" t="s">
-        <v>117</v>
+        <v>20</v>
       </c>
       <c r="G55" s="34">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H55" s="35"/>
       <c r="I55" s="36">
@@ -6375,11 +6387,17 @@
       <c r="L55" s="38"/>
       <c r="M55" s="39">
         <f ca="1">IF(ISBLANK(L55), NETWORKDAYS(J55, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J55, L55, Hoja2!$A$1:$A$18))</f>
-        <v>1</v>
-      </c>
-      <c r="N55" s="38"/>
-      <c r="O55" s="38"/>
-      <c r="P55" s="40"/>
+        <v>3</v>
+      </c>
+      <c r="N55" s="38">
+        <v>46036</v>
+      </c>
+      <c r="O55" s="38">
+        <v>46036</v>
+      </c>
+      <c r="P55" s="40" t="s">
+        <v>211</v>
+      </c>
       <c r="Q55" s="43" t="s">
         <v>44</v>
       </c>
@@ -6406,27 +6424,45 @@
       <c r="AL55" s="50"/>
       <c r="AM55" s="51"/>
     </row>
-    <row r="56" spans="1:39">
-      <c r="A56" s="13"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="16"/>
+    <row r="56" spans="1:39" ht="38.25">
+      <c r="A56" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>213</v>
+      </c>
       <c r="E56" s="17"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="19"/>
+      <c r="F56" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="G56" s="19">
+        <v>0</v>
+      </c>
       <c r="H56" s="20"/>
-      <c r="I56" s="21"/>
+      <c r="I56" s="21">
+        <v>46037</v>
+      </c>
       <c r="J56" s="22"/>
       <c r="K56" s="23"/>
       <c r="L56" s="23"/>
       <c r="M56" s="24">
         <f ca="1">IF(ISBLANK(L56), NETWORKDAYS(J56, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J56, L56, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N56" s="23"/>
       <c r="O56" s="23"/>
-      <c r="P56" s="25"/>
-      <c r="Q56" s="26"/>
+      <c r="P56" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q56" s="43" t="s">
+        <v>44</v>
+      </c>
       <c r="R56" s="52"/>
       <c r="S56" s="52"/>
       <c r="T56" s="52"/>
@@ -6465,7 +6501,7 @@
       <c r="L57" s="38"/>
       <c r="M57" s="39">
         <f ca="1">IF(ISBLANK(L57), NETWORKDAYS(J57, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J57, L57, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N57" s="38"/>
       <c r="O57" s="38"/>
@@ -6509,7 +6545,7 @@
       <c r="L58" s="23"/>
       <c r="M58" s="24">
         <f ca="1">IF(ISBLANK(L58), NETWORKDAYS(J58, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J58, L58, Hoja2!$A$1:$A$18))</f>
-        <v>32867</v>
+        <v>32869</v>
       </c>
       <c r="N58" s="23"/>
       <c r="O58" s="23"/>
@@ -42705,11 +42741,6 @@
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="JENNIFER"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="16">
-      <filters blank="1">
-        <filter val="TRUE"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -42759,7 +42790,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30">
       <c r="A1" s="92" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B1" s="92" t="s">
         <v>2</v>
@@ -42786,13 +42817,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="95" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="K1" s="92" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="L1" s="96" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="M1" s="97"/>
       <c r="N1" s="97"/>
@@ -42811,14 +42842,14 @@
     </row>
     <row r="2" spans="1:26" ht="30">
       <c r="A2" s="98" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C2" s="100"/>
       <c r="D2" s="101" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E2" s="102">
         <v>45526</v>
@@ -42832,7 +42863,7 @@
       <c r="J2" s="100"/>
       <c r="K2" s="100"/>
       <c r="L2" s="100" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="M2" s="103"/>
       <c r="N2" s="103"/>
@@ -42851,13 +42882,13 @@
     </row>
     <row r="3" spans="1:26" ht="28.5">
       <c r="A3" s="104" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C3" s="106" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D3" s="106" t="s">
         <v>20</v>
@@ -42881,7 +42912,7 @@
       </c>
       <c r="K3" s="108"/>
       <c r="L3" s="110" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="M3" s="97"/>
       <c r="N3" s="97"/>
@@ -42900,16 +42931,16 @@
     </row>
     <row r="4" spans="1:26" ht="186">
       <c r="A4" s="111" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B4" s="112" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C4" s="111" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D4" s="113" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="E4" s="114">
         <v>45581</v>
@@ -42932,7 +42963,7 @@
       </c>
       <c r="K4" s="114"/>
       <c r="L4" s="111" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="M4" s="117"/>
       <c r="N4" s="117"/>
@@ -42951,16 +42982,16 @@
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" s="96" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B5" s="112" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C5" s="106" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D5" s="118" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E5" s="107">
         <v>45572</v>
@@ -42981,7 +43012,7 @@
       </c>
       <c r="K5" s="107"/>
       <c r="L5" s="110" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="M5" s="97"/>
       <c r="N5" s="97"/>
@@ -43000,16 +43031,16 @@
     </row>
     <row r="6" spans="1:26" ht="117">
       <c r="A6" s="119" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B6" s="119" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C6" s="113" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D6" s="119" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E6" s="120">
         <v>45602</v>
@@ -43030,7 +43061,7 @@
         <v>45602</v>
       </c>
       <c r="L6" s="121" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="M6" s="122"/>
       <c r="N6" s="123"/>
@@ -43049,16 +43080,16 @@
     </row>
     <row r="7" spans="1:26" ht="99.75">
       <c r="A7" s="96" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C7" s="124" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="D7" s="118" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E7" s="107">
         <v>45589</v>
@@ -43079,7 +43110,7 @@
       </c>
       <c r="K7" s="118"/>
       <c r="L7" s="126" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="M7" s="127"/>
       <c r="N7" s="127"/>
@@ -43098,14 +43129,14 @@
     </row>
     <row r="8" spans="1:26" ht="71.25">
       <c r="A8" s="128" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B8" s="129" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C8" s="130"/>
       <c r="D8" s="130" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E8" s="131">
         <v>45603</v>
@@ -43126,7 +43157,7 @@
       </c>
       <c r="K8" s="131"/>
       <c r="L8" s="133" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="M8" s="97"/>
       <c r="N8" s="97"/>
@@ -43145,16 +43176,16 @@
     </row>
     <row r="9" spans="1:26" ht="42.75">
       <c r="A9" s="134" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B9" s="135" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C9" s="136" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D9" s="137" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E9" s="138">
         <v>45671</v>
@@ -43163,7 +43194,7 @@
         <v>45673</v>
       </c>
       <c r="G9" s="136" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="H9" s="138">
         <v>45680</v>
@@ -43177,7 +43208,7 @@
       </c>
       <c r="K9" s="136"/>
       <c r="L9" s="140" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="M9" s="141"/>
       <c r="N9" s="141"/>
@@ -43196,14 +43227,14 @@
     </row>
     <row r="10" spans="1:26" ht="57">
       <c r="A10" s="134" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B10" s="142"/>
       <c r="C10" s="140" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D10" s="137" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E10" s="138">
         <v>45671</v>
@@ -43222,7 +43253,7 @@
       <c r="J10" s="136"/>
       <c r="K10" s="136"/>
       <c r="L10" s="140" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="M10" s="141"/>
       <c r="N10" s="141"/>
@@ -43241,14 +43272,14 @@
     </row>
     <row r="11" spans="1:26" ht="42.75">
       <c r="A11" s="134" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B11" s="142"/>
       <c r="C11" s="140" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D11" s="137" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E11" s="138">
         <v>45671</v>
@@ -43267,7 +43298,7 @@
       <c r="J11" s="136"/>
       <c r="K11" s="136"/>
       <c r="L11" s="140" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="M11" s="141"/>
       <c r="N11" s="141"/>
@@ -43286,14 +43317,14 @@
     </row>
     <row r="12" spans="1:26" ht="42.75">
       <c r="A12" s="134" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B12" s="142"/>
       <c r="C12" s="140" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D12" s="137" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E12" s="138">
         <v>45671</v>
@@ -43312,7 +43343,7 @@
       <c r="J12" s="136"/>
       <c r="K12" s="136"/>
       <c r="L12" s="140" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="M12" s="141"/>
       <c r="N12" s="141"/>
@@ -43331,14 +43362,14 @@
     </row>
     <row r="13" spans="1:26" ht="42.75">
       <c r="A13" s="134" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B13" s="142"/>
       <c r="C13" s="140" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D13" s="137" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E13" s="138">
         <v>45671</v>
@@ -43357,7 +43388,7 @@
       <c r="J13" s="136"/>
       <c r="K13" s="136"/>
       <c r="L13" s="140" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="M13" s="141"/>
       <c r="N13" s="141"/>
@@ -43376,14 +43407,14 @@
     </row>
     <row r="14" spans="1:26" ht="42.75">
       <c r="A14" s="134" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B14" s="142"/>
       <c r="C14" s="140" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D14" s="137" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E14" s="138">
         <v>45671</v>
@@ -43402,7 +43433,7 @@
       <c r="J14" s="136"/>
       <c r="K14" s="136"/>
       <c r="L14" s="136" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="M14" s="141"/>
       <c r="N14" s="141"/>
@@ -43421,14 +43452,14 @@
     </row>
     <row r="15" spans="1:26" ht="42.75">
       <c r="A15" s="134" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B15" s="142"/>
       <c r="C15" s="140" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D15" s="137" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E15" s="138">
         <v>45671</v>
@@ -43447,7 +43478,7 @@
       <c r="J15" s="136"/>
       <c r="K15" s="136"/>
       <c r="L15" s="136" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="M15" s="141"/>
       <c r="N15" s="141"/>
@@ -43466,14 +43497,14 @@
     </row>
     <row r="16" spans="1:26" ht="71.25">
       <c r="A16" s="134" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B16" s="143"/>
       <c r="C16" s="144" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D16" s="137" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E16" s="138">
         <v>45681</v>
@@ -43492,7 +43523,7 @@
       <c r="J16" s="136"/>
       <c r="K16" s="136"/>
       <c r="L16" s="140" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="M16" s="141"/>
       <c r="N16" s="141"/>
@@ -50024,7 +50055,7 @@
         <v>45292</v>
       </c>
       <c r="B1" s="141" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
@@ -50032,7 +50063,7 @@
         <v>45299</v>
       </c>
       <c r="B2" s="141" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
@@ -50040,7 +50071,7 @@
         <v>45376</v>
       </c>
       <c r="B3" s="141" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
@@ -50048,7 +50079,7 @@
         <v>45379</v>
       </c>
       <c r="B4" s="141" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
@@ -50056,7 +50087,7 @@
         <v>45380</v>
       </c>
       <c r="B5" s="141" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1">
@@ -50064,7 +50095,7 @@
         <v>45413</v>
       </c>
       <c r="B6" s="141" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
@@ -50072,7 +50103,7 @@
         <v>45425</v>
       </c>
       <c r="B7" s="141" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
@@ -50080,7 +50111,7 @@
         <v>45446</v>
       </c>
       <c r="B8" s="141" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1">
@@ -50088,7 +50119,7 @@
         <v>45453</v>
       </c>
       <c r="B9" s="141" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1">
@@ -50096,7 +50127,7 @@
         <v>45474</v>
       </c>
       <c r="B10" s="141" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1">
@@ -50104,7 +50135,7 @@
         <v>45493</v>
       </c>
       <c r="B11" s="141" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" customHeight="1">
@@ -50112,7 +50143,7 @@
         <v>45511</v>
       </c>
       <c r="B12" s="141" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1">
@@ -50120,7 +50151,7 @@
         <v>45523</v>
       </c>
       <c r="B13" s="141" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" customHeight="1">
@@ -50128,7 +50159,7 @@
         <v>45579</v>
       </c>
       <c r="B14" s="141" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" customHeight="1">
@@ -50136,7 +50167,7 @@
         <v>45600</v>
       </c>
       <c r="B15" s="141" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1">
@@ -50144,7 +50175,7 @@
         <v>45607</v>
       </c>
       <c r="B16" s="141" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
@@ -50152,7 +50183,7 @@
         <v>45634</v>
       </c>
       <c r="B17" s="141" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1">
@@ -50160,7 +50191,7 @@
         <v>45651</v>
       </c>
       <c r="B18" s="141" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1"/>
@@ -51172,7 +51203,7 @@
   <sheetData>
     <row r="1" spans="1:97" ht="15.75">
       <c r="A1" s="146" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B1" s="141"/>
       <c r="C1" s="141"/>
@@ -51230,7 +51261,7 @@
     </row>
     <row r="3" spans="1:97" ht="32.25" customHeight="1">
       <c r="A3" s="147" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B3" s="148">
         <v>45596</v>
@@ -51523,261 +51554,261 @@
     </row>
     <row r="4" spans="1:97" ht="30.75" customHeight="1">
       <c r="A4" s="151" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B4" s="152" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C4" s="153" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="J4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="L4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="M4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="N4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="O4" s="154" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="P4" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="R4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="S4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="T4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="U4" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="V4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="W4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="X4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Y4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Z4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AA4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AB4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AC4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AD4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AE4" s="180" t="s">
+        <v>285</v>
+      </c>
+      <c r="AF4" s="154" t="s">
         <v>281</v>
       </c>
-      <c r="AF4" s="154" t="s">
-        <v>277</v>
-      </c>
       <c r="AG4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AH4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AI4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AJ4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AK4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AL4" s="180" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="AM4" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AN4" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AO4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AP4" s="180" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="AQ4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AR4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AS4" s="180" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="AT4" s="156" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AU4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AV4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AW4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AX4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AY4" s="180" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="AZ4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BA4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BB4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BC4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BD4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BE4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BF4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BG4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BH4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BI4" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BJ4" s="180" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="BK4" s="155" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="BL4" s="155" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="BM4" s="155" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="BN4" s="155" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="BO4" s="155" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="BP4" s="155" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="BQ4" s="155" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="BR4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BS4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BT4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BU4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BV4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BW4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BX4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BY4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BZ4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CA4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CB4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CC4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CD4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CE4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CF4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CG4" s="154"/>
       <c r="CH4" s="154"/>
       <c r="CI4" s="180" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="CJ4" s="154"/>
       <c r="CK4" s="154"/>
@@ -51789,249 +51820,249 @@
       <c r="CQ4" s="154"/>
       <c r="CR4" s="154"/>
       <c r="CS4" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:97" ht="15.75" customHeight="1">
       <c r="A5" s="151" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B5" s="152" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="J5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="L5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="M5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="N5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="O5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="P5" s="155" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="Q5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="R5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="S5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="T5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="U5" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="V5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="W5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="X5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Y5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Z5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AA5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AB5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AC5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AD5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AE5" s="181"/>
       <c r="AF5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AG5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AH5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AI5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AJ5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AK5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AL5" s="181"/>
       <c r="AM5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AN5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AO5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AP5" s="181"/>
       <c r="AQ5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="AR5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="AS5" s="181"/>
       <c r="AT5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="AU5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="AV5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="AW5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="AX5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="AY5" s="181"/>
       <c r="AZ5" s="154" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="BA5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BB5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BC5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BD5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BE5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BF5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BG5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BH5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BI5" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BJ5" s="181"/>
       <c r="BK5" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BL5" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BM5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BN5" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BO5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BP5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BQ5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BR5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BS5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BT5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BU5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BV5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BW5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BX5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BY5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BZ5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CA5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CB5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CC5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CD5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CE5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CF5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CG5" s="154"/>
       <c r="CH5" s="154"/>
@@ -52046,249 +52077,249 @@
       <c r="CQ5" s="154"/>
       <c r="CR5" s="154"/>
       <c r="CS5" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:97" ht="15.75">
       <c r="A6" s="151" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B6" s="152" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="J6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K6" s="157" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="L6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="M6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="N6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="O6" s="154" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="P6" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="R6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="S6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="T6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="U6" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="V6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="W6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="X6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Y6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Z6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AA6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AB6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AC6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AD6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AE6" s="181"/>
       <c r="AF6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AG6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AH6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AI6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AJ6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AK6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AL6" s="181"/>
       <c r="AM6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AN6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AO6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AP6" s="181"/>
       <c r="AQ6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AR6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AS6" s="181"/>
       <c r="AT6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AU6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AV6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AW6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AX6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AY6" s="181"/>
       <c r="AZ6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BA6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BB6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BC6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BD6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BE6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BF6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BG6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BH6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BI6" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BJ6" s="181"/>
       <c r="BK6" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BL6" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BM6" s="154" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="BN6" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BO6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BP6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BQ6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BR6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BS6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BT6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BU6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BV6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BW6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BX6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BY6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BZ6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CA6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CB6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CC6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CD6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CE6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CF6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CG6" s="154"/>
       <c r="CH6" s="154"/>
@@ -52303,198 +52334,198 @@
       <c r="CQ6" s="154"/>
       <c r="CR6" s="154"/>
       <c r="CS6" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="151" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B7" s="152" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="J7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="L7" s="157" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="M7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="N7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="O7" s="154" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="P7" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="R7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="S7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="T7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="U7" s="155" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="V7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="W7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="X7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Y7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Z7" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AA7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AB7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AC7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AD7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AE7" s="181"/>
       <c r="AF7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AG7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AH7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AI7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AJ7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AK7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AL7" s="181"/>
       <c r="AM7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AN7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AO7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AP7" s="181"/>
       <c r="AQ7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AR7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AS7" s="181"/>
       <c r="AT7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AU7" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AV7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AW7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AX7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AY7" s="181"/>
       <c r="AZ7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BA7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BB7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BC7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BD7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BE7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BF7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BG7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BH7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BI7" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BJ7" s="181"/>
       <c r="BK7" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BL7" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BM7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BN7" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BO7" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BP7" s="154"/>
       <c r="BQ7" s="154"/>
@@ -52502,16 +52533,16 @@
       <c r="BS7" s="154"/>
       <c r="BT7" s="154"/>
       <c r="BU7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BV7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BW7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BX7" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BY7" s="154"/>
       <c r="BZ7" s="154"/>
@@ -52537,220 +52568,220 @@
     </row>
     <row r="8" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="151" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B8" s="152" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="J8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="L8" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="M8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="N8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="O8" s="154" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="P8" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="R8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="S8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="T8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="U8" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="V8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="W8" s="154" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="X8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Y8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Z8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AA8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AB8" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AC8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AD8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AE8" s="181"/>
       <c r="AF8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AG8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AH8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AI8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AJ8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AK8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AL8" s="181"/>
       <c r="AM8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AN8" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AO8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AP8" s="181"/>
       <c r="AQ8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AR8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AS8" s="181"/>
       <c r="AT8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AU8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AV8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AW8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AX8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AY8" s="181"/>
       <c r="AZ8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BA8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BB8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BC8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BD8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BE8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BF8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BG8" s="154" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="BH8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BI8" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BJ8" s="181"/>
       <c r="BK8" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BL8" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BM8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BN8" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BO8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BP8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BQ8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BR8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BS8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BT8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BU8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BV8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BW8" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BX8" s="154" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="BY8" s="154"/>
       <c r="BZ8" s="154"/>
@@ -52776,244 +52807,244 @@
     </row>
     <row r="9" spans="1:97" ht="15.75">
       <c r="A9" s="151" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B9" s="152" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="J9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="L9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="M9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="N9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="O9" s="157" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="P9" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="R9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="S9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="T9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="U9" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="V9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="W9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="X9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Y9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Z9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AA9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AB9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AC9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AD9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AE9" s="181"/>
       <c r="AF9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AG9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AH9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AI9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AJ9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AK9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AL9" s="181"/>
       <c r="AM9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AN9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AO9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AP9" s="181"/>
       <c r="AQ9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AR9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AS9" s="181"/>
       <c r="AT9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AU9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AV9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AW9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AX9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AY9" s="181"/>
       <c r="AZ9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BA9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BB9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BC9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BD9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BE9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BF9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BG9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BH9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BI9" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BJ9" s="181"/>
       <c r="BK9" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BL9" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BM9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BN9" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BO9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BP9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BQ9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BR9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BS9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BT9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BU9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BV9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BW9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BX9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BY9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BZ9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CA9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CB9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CC9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CD9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CE9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CF9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CG9" s="154"/>
       <c r="CH9" s="154"/>
@@ -53028,249 +53059,249 @@
       <c r="CQ9" s="154"/>
       <c r="CR9" s="154"/>
       <c r="CS9" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:97" ht="15.75">
       <c r="A10" s="151" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B10" s="152" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="J10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="L10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="M10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="N10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="O10" s="154" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="P10" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="Q10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="R10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="S10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="T10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="U10" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="V10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="W10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="X10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Y10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Z10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AA10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AB10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AC10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AD10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AE10" s="181"/>
       <c r="AF10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AG10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AH10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AI10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AJ10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AK10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AL10" s="181"/>
       <c r="AM10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AN10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AO10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AP10" s="181"/>
       <c r="AQ10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AR10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AS10" s="181"/>
       <c r="AT10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AU10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AV10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AW10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AX10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AY10" s="181"/>
       <c r="AZ10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BA10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BB10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BC10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BD10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BE10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BF10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BG10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BH10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BI10" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BJ10" s="181"/>
       <c r="BK10" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BL10" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BM10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BN10" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BO10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BP10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BQ10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BR10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BS10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BT10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BU10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BV10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BW10" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BX10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BY10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BZ10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CA10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CB10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CC10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CD10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CE10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CF10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CG10" s="154"/>
       <c r="CH10" s="154"/>
@@ -53285,249 +53316,249 @@
       <c r="CQ10" s="154"/>
       <c r="CR10" s="154"/>
       <c r="CS10" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:97" ht="15.75">
       <c r="A11" s="151" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B11" s="152" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="J11" s="154" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="K11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="L11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="M11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="N11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="O11" s="154" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="P11" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="R11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="S11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="T11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="U11" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="V11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="W11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="X11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Y11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Z11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AA11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AB11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AC11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AD11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AE11" s="181"/>
       <c r="AF11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AG11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AH11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AI11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AJ11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AK11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AL11" s="181"/>
       <c r="AM11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AN11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AO11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AP11" s="181"/>
       <c r="AQ11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AR11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AS11" s="181"/>
       <c r="AT11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AU11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AV11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AW11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AX11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AY11" s="181"/>
       <c r="AZ11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BA11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BB11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BC11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BD11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BE11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BF11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BG11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BH11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BI11" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BJ11" s="181"/>
       <c r="BK11" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BL11" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BM11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BN11" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BO11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BP11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BQ11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BR11" s="154" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="BS11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BT11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BU11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BV11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BW11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BX11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BY11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BZ11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CA11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CB11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="CC11" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="CD11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CE11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CF11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CG11" s="154"/>
       <c r="CH11" s="154"/>
@@ -53542,249 +53573,249 @@
       <c r="CQ11" s="154"/>
       <c r="CR11" s="154"/>
       <c r="CS11" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:97" ht="15.75">
       <c r="A12" s="151" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B12" s="152" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="G12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="H12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="J12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="L12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="M12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="N12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="O12" s="154" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="P12" s="155" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="R12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="S12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="T12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="U12" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="V12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="W12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="X12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="Y12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="Z12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AA12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AB12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AC12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AD12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AE12" s="181"/>
       <c r="AF12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AG12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AH12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AI12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AJ12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AK12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AL12" s="181"/>
       <c r="AM12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AN12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AO12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AP12" s="181"/>
       <c r="AQ12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AR12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AS12" s="181"/>
       <c r="AT12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AU12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AV12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AW12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AX12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AY12" s="181"/>
       <c r="AZ12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BA12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BB12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BC12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BD12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BE12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BF12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BG12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BH12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BI12" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BJ12" s="181"/>
       <c r="BK12" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BL12" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BM12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BN12" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BO12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BP12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BQ12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BR12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BS12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BT12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BU12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BV12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BW12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BX12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BY12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BZ12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="CA12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="CB12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CC12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="CD12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="CE12" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CF12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="CG12" s="154"/>
       <c r="CH12" s="154"/>
@@ -53799,249 +53830,249 @@
       <c r="CQ12" s="154"/>
       <c r="CR12" s="154"/>
       <c r="CS12" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:97" ht="15.75">
       <c r="A13" s="151" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B13" s="152" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="F13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="G13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="H13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="I13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="J13" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="K13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="L13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="M13" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="N13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="O13" s="154" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="P13" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="Q13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="R13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="S13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="T13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="U13" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="V13" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="W13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="X13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="Y13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="Z13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AA13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AB13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AC13" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AD13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AE13" s="182"/>
       <c r="AF13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AG13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AH13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AI13" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AJ13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AK13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AL13" s="182"/>
       <c r="AM13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AN13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AO13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AP13" s="182"/>
       <c r="AQ13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AR13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AS13" s="182"/>
       <c r="AT13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AU13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AV13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AW13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AX13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AY13" s="182"/>
       <c r="AZ13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BA13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BB13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BC13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BD13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BE13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BF13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BG13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BH13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BI13" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BJ13" s="182"/>
       <c r="BK13" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BL13" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BM13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BN13" s="155" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BO13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BP13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BQ13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BR13" s="154" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="BS13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BT13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BU13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BV13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BW13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BX13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BY13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BZ13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="CA13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="CB13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="CC13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="CD13" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CE13" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CF13" s="154" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CG13" s="154"/>
       <c r="CH13" s="154"/>
@@ -54056,7 +54087,7 @@
       <c r="CQ13" s="154"/>
       <c r="CR13" s="154"/>
       <c r="CS13" s="154" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -55078,7 +55109,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="25.5">
       <c r="A1" s="158" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B1" s="158" t="s">
         <v>2</v>
@@ -55105,13 +55136,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="162" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="K1" s="163" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="L1" s="161" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="M1" s="164"/>
       <c r="N1" s="164"/>
@@ -55130,10 +55161,10 @@
     </row>
     <row r="2" spans="1:26" ht="38.25">
       <c r="A2" s="165" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B2" s="166" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C2" s="167"/>
       <c r="D2" s="167" t="s">
@@ -55160,7 +55191,7 @@
       </c>
       <c r="K2" s="170"/>
       <c r="L2" s="171" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="M2" s="164"/>
       <c r="N2" s="164"/>
@@ -55179,13 +55210,13 @@
     </row>
     <row r="3" spans="1:26" ht="51">
       <c r="A3" s="165" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B3" s="183" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C3" s="172" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="D3" s="167" t="s">
         <v>38</v>
@@ -55207,7 +55238,7 @@
       </c>
       <c r="K3" s="168"/>
       <c r="L3" s="171" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="M3" s="173"/>
       <c r="N3" s="164"/>
@@ -55226,11 +55257,11 @@
     </row>
     <row r="4" spans="1:26" ht="51">
       <c r="A4" s="165" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B4" s="181"/>
       <c r="C4" s="174" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D4" s="167" t="s">
         <v>38</v>
@@ -55252,7 +55283,7 @@
       </c>
       <c r="K4" s="175"/>
       <c r="L4" s="178" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="M4" s="173"/>
       <c r="N4" s="164"/>
@@ -55271,13 +55302,13 @@
     </row>
     <row r="5" spans="1:26" ht="51">
       <c r="A5" s="165" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B5" s="161" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C5" s="167" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D5" s="167" t="s">
         <v>38</v>
@@ -55299,7 +55330,7 @@
       </c>
       <c r="K5" s="168"/>
       <c r="L5" s="171" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="M5" s="173"/>
       <c r="N5" s="164"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 11 de febrero 2026
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -831,7 +831,9 @@
     <t>Mejoras al módulo para agilizar la auditoria y revisión de inconsistencias por parte de las Gestoras, ver inforción importante, eliminar datos innecesarios, mejorar ventana para visualización de información</t>
   </si>
   <si>
-    <t>7/01/2026 se hace reunión con el área comercial, para ver mejoras del módulode normalización, y mejorar la revisión de las solicitudes</t>
+    <t>7/01/2026 se hace reunión con el área comercial, para ver mejoras del módulode normalización, y mejorar la revisión de las solicitudes
+5/02/2025 Se revisa documento enviado por el área comercial, para validar los ajustes solicitados para la plataforma de Normalización de Afiliaciones, Se renombfran columnas y eliminan las soliictadas
+6/02/2025 se inicia con la adición de columnas y la modificación en query para obtener l dato</t>
   </si>
   <si>
     <t>Afiliaciones Pre - Validación 7 campos</t>
@@ -855,7 +857,7 @@
     <t>Revisar la generación de la data de seguimiento de la revisión por parte del área médica, e identificar posibles errores en el query o impresión, dado que se evidenciaron registros duplicados</t>
   </si>
   <si>
-    <t>15/01/2026 revisar la generación actual del informe generla del módulo de Riesgo médico</t>
+    <t>11/02/2026 revisar la generación actual del informe generla del módulo de Riesgo médico, y revisar resultado e identificar posible inconsistencia de duplicados</t>
   </si>
   <si>
     <t>Convenios Medicos - Cargue Masivo de Planes a Nits</t>
@@ -1619,7 +1621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1895,6 +1897,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2125,8 +2128,8 @@
   <dimension ref="A1:AN60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2660,7 +2663,7 @@
       <c r="L7" s="43"/>
       <c r="M7" s="50">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32882</v>
+        <v>32887</v>
       </c>
       <c r="N7" s="43"/>
       <c r="O7" s="43"/>
@@ -3047,7 +3050,7 @@
       NETWORKDAYS(J12,L12,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="N12" s="28"/>
       <c r="O12" s="28"/>
@@ -3835,7 +3838,7 @@
       NETWORKDAYS(J22,L22,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="N22" s="28"/>
       <c r="O22" s="28"/>
@@ -3989,7 +3992,7 @@
       NETWORKDAYS(J24,L24,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="N24" s="28"/>
       <c r="O24" s="28"/>
@@ -4293,7 +4296,7 @@
       NETWORKDAYS(J28,L28,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="N28" s="28"/>
       <c r="O28" s="28"/>
@@ -4747,7 +4750,7 @@
       </c>
       <c r="E34" s="21"/>
       <c r="F34" s="22" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="G34" s="23">
         <v>30</v>
@@ -4773,7 +4776,7 @@
       NETWORKDAYS(J34,L34,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="N34" s="28"/>
       <c r="O34" s="28"/>
@@ -4848,7 +4851,7 @@
       NETWORKDAYS(J35,L35,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="N35" s="43"/>
       <c r="O35" s="43">
@@ -4927,7 +4930,7 @@
       NETWORKDAYS(J36,L36,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="N36" s="28"/>
       <c r="O36" s="28"/>
@@ -5002,7 +5005,7 @@
       NETWORKDAYS(J37,L37,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="N37" s="43"/>
       <c r="O37" s="43">
@@ -5079,7 +5082,7 @@
       NETWORKDAYS(J38,L38,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="N38" s="28"/>
       <c r="O38" s="28"/>
@@ -5225,7 +5228,7 @@
       NETWORKDAYS(J40,L40,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="N40" s="28"/>
       <c r="O40" s="28">
@@ -5304,7 +5307,7 @@
       NETWORKDAYS(J41,L41,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="N41" s="43"/>
       <c r="O41" s="43">
@@ -5369,7 +5372,7 @@
       <c r="L42" s="28"/>
       <c r="M42" s="64">
         <f ca="1">IF(ISBLANK(L42), NETWORKDAYS(J42, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J42, L42, Hoja2!$A$1:$A$18))</f>
-        <v>32882</v>
+        <v>32887</v>
       </c>
       <c r="N42" s="28"/>
       <c r="O42" s="28"/>
@@ -5442,7 +5445,7 @@
       NETWORKDAYS(J43,L43,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="N43" s="43"/>
       <c r="O43" s="43">
@@ -5730,7 +5733,7 @@
       <c r="L47" s="43"/>
       <c r="M47" s="50">
         <f ca="1">IF(ISBLANK(L47), NETWORKDAYS(J47, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J47, L47, Hoja2!$A$1:$A$18))</f>
-        <v>32882</v>
+        <v>32887</v>
       </c>
       <c r="N47" s="43"/>
       <c r="O47" s="43"/>
@@ -5791,7 +5794,7 @@
       <c r="L48" s="28"/>
       <c r="M48" s="64">
         <f ca="1">IF(ISBLANK(L48), NETWORKDAYS(J48, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J48, L48, Hoja2!$A$1:$A$18))</f>
-        <v>32882</v>
+        <v>32887</v>
       </c>
       <c r="N48" s="28"/>
       <c r="O48" s="28"/>
@@ -5850,7 +5853,7 @@
       <c r="L49" s="43"/>
       <c r="M49" s="50">
         <f ca="1">IF(ISBLANK(L49), NETWORKDAYS(J49, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J49, L49, Hoja2!$A$1:$A$18))</f>
-        <v>32882</v>
+        <v>32887</v>
       </c>
       <c r="N49" s="43"/>
       <c r="O49" s="43"/>
@@ -6140,20 +6143,24 @@
       </c>
       <c r="E53" s="36"/>
       <c r="F53" s="37" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="G53" s="38">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H53" s="39">
         <f>IF(OR(J53="",K53="",K53&lt;J53),0,NETWORKDAYS(J53,K53,Hoja2!$A$2:$A$53))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I53" s="40">
         <v>46029</v>
       </c>
-      <c r="J53" s="40"/>
-      <c r="K53" s="41"/>
+      <c r="J53" s="40">
+        <v>46058</v>
+      </c>
+      <c r="K53" s="41">
+        <v>46066</v>
+      </c>
       <c r="L53" s="41"/>
       <c r="M53" s="42">
         <f ca="1">IF(OR(J53="",AND(L53="",TODAY()&lt;J53),AND(L53&lt;&gt;"",L53&lt;J53)),0,
@@ -6162,7 +6169,7 @@
       NETWORKDAYS(J53,L53,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N53" s="43"/>
       <c r="O53" s="43"/>
@@ -6237,7 +6244,7 @@
       NETWORKDAYS(J54,L54,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="N54" s="28"/>
       <c r="O54" s="28">
@@ -6316,7 +6323,7 @@
       NETWORKDAYS(J55,L55,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N55" s="43"/>
       <c r="O55" s="43">
@@ -6381,7 +6388,9 @@
       <c r="I56" s="25">
         <v>46037</v>
       </c>
-      <c r="J56" s="25"/>
+      <c r="J56" s="25">
+        <v>46064</v>
+      </c>
       <c r="K56" s="26"/>
       <c r="L56" s="26"/>
       <c r="M56" s="27">
@@ -6391,7 +6400,7 @@
       NETWORKDAYS(J56,L56,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N56" s="28"/>
       <c r="O56" s="28"/>
@@ -6462,8 +6471,8 @@
       <c r="O57" s="43"/>
       <c r="P57" s="43"/>
       <c r="Q57" s="44"/>
-      <c r="R57" s="45" t="s">
-        <v>45</v>
+      <c r="R57" s="109" t="s">
+        <v>41</v>
       </c>
       <c r="S57" s="57"/>
       <c r="T57" s="57"/>
@@ -6525,8 +6534,8 @@
       <c r="O58" s="28"/>
       <c r="P58" s="28"/>
       <c r="Q58" s="29"/>
-      <c r="R58" s="30" t="s">
-        <v>45</v>
+      <c r="R58" s="109" t="s">
+        <v>41</v>
       </c>
       <c r="S58" s="59"/>
       <c r="T58" s="59"/>
@@ -6588,8 +6597,8 @@
       <c r="O59" s="43"/>
       <c r="P59" s="43"/>
       <c r="Q59" s="44"/>
-      <c r="R59" s="45" t="s">
-        <v>45</v>
+      <c r="R59" s="109" t="s">
+        <v>41</v>
       </c>
       <c r="S59" s="57"/>
       <c r="T59" s="57"/>
@@ -6651,8 +6660,8 @@
       <c r="O60" s="28"/>
       <c r="P60" s="28"/>
       <c r="Q60" s="29"/>
-      <c r="R60" s="30" t="s">
-        <v>45</v>
+      <c r="R60" s="109" t="s">
+        <v>41</v>
       </c>
       <c r="S60" s="59"/>
       <c r="T60" s="59"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 17 de febrero 2026
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="319">
   <si>
     <t>Asignado a</t>
   </si>
@@ -905,10 +905,22 @@
     <t>OPT_39</t>
   </si>
   <si>
+    <t>Afiliaciones PRE - Modificar opción de devoluciones por escalas encontradas en la consulta SARLAFT</t>
+  </si>
+  <si>
+    <t>Modificar opción de devoluciones por escalas encontradas en la consulta SARLAFT, solo se deben devolver y reportar por correo las solicitude que en su consulta reporten las escalas se reportaran las escalas 1, 2, 5 y 6</t>
+  </si>
+  <si>
+    <t>17/02/2026 revisar la pagina donde se cargan los soportes de infolat, y se identifican las escalas, para que se pregunte por las escalas 1, 2, 5 y 6, solo para estas se deben generar las devoluciones</t>
+  </si>
+  <si>
+    <t>OPT_40</t>
+  </si>
+  <si>
     <t>Afiliaciones POS - Completar descarga de cartas Derechos y Deberes</t>
   </si>
   <si>
-    <t>OPT_40</t>
+    <t>OPT_41</t>
   </si>
   <si>
     <t>Afiliaciones POS - Consumo Puntual de las afiliaciones</t>
@@ -1176,6 +1188,9 @@
   </si>
   <si>
     <t>Internal Server Error</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -1663,7 +1678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1939,6 +1954,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2166,11 +2182,11 @@
   <sheetPr>
     <tabColor rgb="FF93C47D"/>
   </sheetPr>
-  <dimension ref="A1:AN61"/>
+  <dimension ref="A1:AN62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2702,14 +2718,9 @@
       <c r="J7" s="49"/>
       <c r="K7" s="43"/>
       <c r="L7" s="43"/>
-      <c r="M7" s="27">
-        <f ca="1">IF(OR(J7="",AND(L7="",TODAY()&lt;J7),AND(L7&lt;&gt;"",L7&lt;J7)),0,
-   IF(L7="",
-      NETWORKDAYS(J7,TODAY(),Hoja2!$A$2:$A$53),
-      NETWORKDAYS(J7,L7,Hoja2!$A$2:$A$53)
-   )
-)</f>
-        <v>0</v>
+      <c r="M7" s="50">
+        <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
+        <v>32891</v>
       </c>
       <c r="N7" s="43"/>
       <c r="O7" s="43"/>
@@ -3096,7 +3107,7 @@
       NETWORKDAYS(J12,L12,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="N12" s="28"/>
       <c r="O12" s="28"/>
@@ -3884,7 +3895,7 @@
       NETWORKDAYS(J22,L22,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="N22" s="28"/>
       <c r="O22" s="28"/>
@@ -4038,7 +4049,7 @@
       NETWORKDAYS(J24,L24,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="N24" s="28"/>
       <c r="O24" s="28"/>
@@ -4342,7 +4353,7 @@
       NETWORKDAYS(J28,L28,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N28" s="28"/>
       <c r="O28" s="28"/>
@@ -4822,7 +4833,7 @@
       NETWORKDAYS(J34,L34,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="N34" s="28"/>
       <c r="O34" s="28"/>
@@ -4897,7 +4908,7 @@
       NETWORKDAYS(J35,L35,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N35" s="43"/>
       <c r="O35" s="43">
@@ -4950,10 +4961,10 @@
       </c>
       <c r="E36" s="21"/>
       <c r="F36" s="22" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="G36" s="23">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="H36" s="24">
         <f>IF(OR(J36="",K36="",K36&lt;J36),0,NETWORKDAYS(J36,K36,Hoja2!$A$2:$A$53))</f>
@@ -4976,11 +4987,15 @@
       NETWORKDAYS(J36,L36,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N36" s="28"/>
-      <c r="O36" s="28"/>
-      <c r="P36" s="28"/>
+      <c r="O36" s="28">
+        <v>45975</v>
+      </c>
+      <c r="P36" s="28">
+        <v>45975</v>
+      </c>
       <c r="Q36" s="29" t="s">
         <v>150</v>
       </c>
@@ -5051,7 +5066,7 @@
       NETWORKDAYS(J37,L37,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="N37" s="43"/>
       <c r="O37" s="43">
@@ -5128,7 +5143,7 @@
       NETWORKDAYS(J38,L38,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N38" s="28"/>
       <c r="O38" s="28"/>
@@ -5208,7 +5223,7 @@
       <c r="P39" s="43"/>
       <c r="Q39" s="44"/>
       <c r="R39" s="51" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="S39" s="57"/>
       <c r="T39" s="57"/>
@@ -5274,7 +5289,7 @@
       NETWORKDAYS(J40,L40,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N40" s="28"/>
       <c r="O40" s="28">
@@ -5353,7 +5368,7 @@
       NETWORKDAYS(J41,L41,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N41" s="43"/>
       <c r="O41" s="43">
@@ -5418,7 +5433,7 @@
       <c r="L42" s="28"/>
       <c r="M42" s="64">
         <f ca="1">IF(ISBLANK(L42), NETWORKDAYS(J42, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J42, L42, Hoja2!$A$1:$A$18))</f>
-        <v>32889</v>
+        <v>32891</v>
       </c>
       <c r="N42" s="28"/>
       <c r="O42" s="28"/>
@@ -5491,7 +5506,7 @@
       NETWORKDAYS(J43,L43,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N43" s="43"/>
       <c r="O43" s="43">
@@ -5779,7 +5794,7 @@
       <c r="L47" s="43"/>
       <c r="M47" s="50">
         <f ca="1">IF(ISBLANK(L47), NETWORKDAYS(J47, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J47, L47, Hoja2!$A$1:$A$18))</f>
-        <v>32889</v>
+        <v>32891</v>
       </c>
       <c r="N47" s="43"/>
       <c r="O47" s="43"/>
@@ -5840,7 +5855,7 @@
       <c r="L48" s="28"/>
       <c r="M48" s="64">
         <f ca="1">IF(ISBLANK(L48), NETWORKDAYS(J48, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J48, L48, Hoja2!$A$1:$A$18))</f>
-        <v>32889</v>
+        <v>32891</v>
       </c>
       <c r="N48" s="28"/>
       <c r="O48" s="28"/>
@@ -5899,7 +5914,7 @@
       <c r="L49" s="43"/>
       <c r="M49" s="50">
         <f ca="1">IF(ISBLANK(L49), NETWORKDAYS(J49, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J49, L49, Hoja2!$A$1:$A$18))</f>
-        <v>32889</v>
+        <v>32891</v>
       </c>
       <c r="N49" s="43"/>
       <c r="O49" s="43"/>
@@ -6215,7 +6230,7 @@
       NETWORKDAYS(J53,L53,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N53" s="43"/>
       <c r="O53" s="43"/>
@@ -6290,7 +6305,7 @@
       NETWORKDAYS(J54,L54,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N54" s="28"/>
       <c r="O54" s="28">
@@ -6369,7 +6384,7 @@
       NETWORKDAYS(J55,L55,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N55" s="43"/>
       <c r="O55" s="43">
@@ -6446,7 +6461,7 @@
       NETWORKDAYS(J56,L56,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N56" s="28"/>
       <c r="O56" s="28"/>
@@ -6560,10 +6575,10 @@
       </c>
       <c r="E58" s="21"/>
       <c r="F58" s="22" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="G58" s="23">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="H58" s="24">
         <f>IF(OR(J58="",K58="",K58&lt;J58),0,NETWORKDAYS(J58,K58,Hoja2!$A$2:$A$53))</f>
@@ -6584,7 +6599,7 @@
       NETWORKDAYS(J58,L58,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N58" s="28"/>
       <c r="O58" s="28">
@@ -6687,7 +6702,7 @@
       <c r="AM59" s="57"/>
       <c r="AN59" s="58"/>
     </row>
-    <row r="60" spans="1:40" ht="57">
+    <row r="60" spans="1:40" ht="71.25">
       <c r="A60" s="17" t="s">
         <v>36</v>
       </c>
@@ -6697,19 +6712,29 @@
       <c r="C60" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="D60" s="20"/>
+      <c r="D60" s="20" t="s">
+        <v>232</v>
+      </c>
       <c r="E60" s="21"/>
       <c r="F60" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G60" s="23"/>
+        <v>119</v>
+      </c>
+      <c r="G60" s="23">
+        <v>35</v>
+      </c>
       <c r="H60" s="24">
         <f>IF(OR(J60="",K60="",K60&lt;J60),0,NETWORKDAYS(J60,K60,Hoja2!$A$2:$A$53))</f>
-        <v>0</v>
-      </c>
-      <c r="I60" s="25"/>
-      <c r="J60" s="25"/>
-      <c r="K60" s="26"/>
+        <v>2</v>
+      </c>
+      <c r="I60" s="25">
+        <v>46069</v>
+      </c>
+      <c r="J60" s="25">
+        <v>46070</v>
+      </c>
+      <c r="K60" s="26">
+        <v>46071</v>
+      </c>
       <c r="L60" s="26"/>
       <c r="M60" s="27">
         <f ca="1">IF(OR(J60="",AND(L60="",TODAY()&lt;J60),AND(L60&lt;&gt;"",L60&lt;J60)),0,
@@ -6718,14 +6743,16 @@
       NETWORKDAYS(J60,L60,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N60" s="28"/>
       <c r="O60" s="28"/>
       <c r="P60" s="28"/>
-      <c r="Q60" s="29"/>
+      <c r="Q60" s="29" t="s">
+        <v>233</v>
+      </c>
       <c r="R60" s="30" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="S60" s="59"/>
       <c r="T60" s="59"/>
@@ -6750,15 +6777,15 @@
       <c r="AM60" s="59"/>
       <c r="AN60" s="60"/>
     </row>
-    <row r="61" spans="1:40" ht="42.75">
+    <row r="61" spans="1:40" ht="57">
       <c r="A61" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B61" s="33" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C61" s="34" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D61" s="35"/>
       <c r="E61" s="36"/>
@@ -6785,8 +6812,8 @@
       <c r="O61" s="43"/>
       <c r="P61" s="43"/>
       <c r="Q61" s="44"/>
-      <c r="R61" s="30" t="s">
-        <v>41</v>
+      <c r="R61" s="109" t="s">
+        <v>318</v>
       </c>
       <c r="S61" s="57"/>
       <c r="T61" s="57"/>
@@ -6811,18 +6838,79 @@
       <c r="AM61" s="57"/>
       <c r="AN61" s="58"/>
     </row>
+    <row r="62" spans="1:40" ht="42.75">
+      <c r="A62" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="D62" s="20"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="24">
+        <f>IF(OR(J62="",K62="",K62&lt;J62),0,NETWORKDAYS(J62,K62,Hoja2!$A$2:$A$53))</f>
+        <v>0</v>
+      </c>
+      <c r="I62" s="25"/>
+      <c r="J62" s="25"/>
+      <c r="K62" s="26"/>
+      <c r="L62" s="26"/>
+      <c r="M62" s="27">
+        <f ca="1">IF(OR(J62="",AND(L62="",TODAY()&lt;J62),AND(L62&lt;&gt;"",L62&lt;J62)),0,
+   IF(L62="",
+      NETWORKDAYS(J62,TODAY(),Hoja2!$A$2:$A$53),
+      NETWORKDAYS(J62,L62,Hoja2!$A$2:$A$53)
+   )
+)</f>
+        <v>0</v>
+      </c>
+      <c r="N62" s="28"/>
+      <c r="O62" s="28"/>
+      <c r="P62" s="28"/>
+      <c r="Q62" s="29"/>
+      <c r="R62" s="109" t="s">
+        <v>318</v>
+      </c>
+      <c r="S62" s="59"/>
+      <c r="T62" s="59"/>
+      <c r="U62" s="59"/>
+      <c r="V62" s="59"/>
+      <c r="W62" s="59"/>
+      <c r="X62" s="59"/>
+      <c r="Y62" s="59"/>
+      <c r="Z62" s="59"/>
+      <c r="AA62" s="59"/>
+      <c r="AB62" s="59"/>
+      <c r="AC62" s="59"/>
+      <c r="AD62" s="59"/>
+      <c r="AE62" s="59"/>
+      <c r="AF62" s="59"/>
+      <c r="AG62" s="59"/>
+      <c r="AH62" s="59"/>
+      <c r="AI62" s="59"/>
+      <c r="AJ62" s="59"/>
+      <c r="AK62" s="59"/>
+      <c r="AL62" s="59"/>
+      <c r="AM62" s="59"/>
+      <c r="AN62" s="60"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:R61"/>
-  <conditionalFormatting sqref="B8:B61">
+  <conditionalFormatting sqref="B8:B62">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>COUNTIF(B8:B61, B8)&gt;1</formula>
+      <formula>COUNTIF(B8:B62, B8)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="F2:F61">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F62">
       <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS CLIENTE,PRUEBAS IMAGINE,PASO A PRODUCCION"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L26 N2:P26 I27 I28:L61 N28:P61">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L26 N2:P26 I27 I28:L62 N28:P62">
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
     </dataValidation>
   </dataValidations>
@@ -6847,7 +6935,7 @@
         <v>45292</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
@@ -6855,7 +6943,7 @@
         <v>45299</v>
       </c>
       <c r="B2" s="68" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
@@ -6863,7 +6951,7 @@
         <v>45376</v>
       </c>
       <c r="B3" s="68" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
@@ -6871,7 +6959,7 @@
         <v>45379</v>
       </c>
       <c r="B4" s="68" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
@@ -6879,7 +6967,7 @@
         <v>45380</v>
       </c>
       <c r="B5" s="68" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1">
@@ -6887,7 +6975,7 @@
         <v>45413</v>
       </c>
       <c r="B6" s="68" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
@@ -6895,7 +6983,7 @@
         <v>45425</v>
       </c>
       <c r="B7" s="68" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
@@ -6903,7 +6991,7 @@
         <v>45446</v>
       </c>
       <c r="B8" s="68" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1">
@@ -6911,7 +6999,7 @@
         <v>45453</v>
       </c>
       <c r="B9" s="68" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1">
@@ -6919,7 +7007,7 @@
         <v>45474</v>
       </c>
       <c r="B10" s="68" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1">
@@ -6927,7 +7015,7 @@
         <v>45493</v>
       </c>
       <c r="B11" s="68" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" customHeight="1">
@@ -6935,7 +7023,7 @@
         <v>45511</v>
       </c>
       <c r="B12" s="68" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1">
@@ -6943,7 +7031,7 @@
         <v>45523</v>
       </c>
       <c r="B13" s="68" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" customHeight="1">
@@ -6951,7 +7039,7 @@
         <v>45579</v>
       </c>
       <c r="B14" s="68" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" customHeight="1">
@@ -6959,7 +7047,7 @@
         <v>45600</v>
       </c>
       <c r="B15" s="68" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1">
@@ -6967,7 +7055,7 @@
         <v>45607</v>
       </c>
       <c r="B16" s="68" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
@@ -6975,7 +7063,7 @@
         <v>45634</v>
       </c>
       <c r="B17" s="68" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1">
@@ -6983,7 +7071,7 @@
         <v>45651</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1">
@@ -6991,7 +7079,7 @@
         <v>45658</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" customHeight="1">
@@ -6999,7 +7087,7 @@
         <v>45663</v>
       </c>
       <c r="B20" s="69" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" customHeight="1">
@@ -7007,7 +7095,7 @@
         <v>45740</v>
       </c>
       <c r="B21" s="69" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" customHeight="1">
@@ -7015,7 +7103,7 @@
         <v>45764</v>
       </c>
       <c r="B22" s="69" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.25" customHeight="1">
@@ -7023,7 +7111,7 @@
         <v>45765</v>
       </c>
       <c r="B23" s="69" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" customHeight="1">
@@ -7031,7 +7119,7 @@
         <v>45778</v>
       </c>
       <c r="B24" s="69" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="17.25" customHeight="1">
@@ -7039,7 +7127,7 @@
         <v>45810</v>
       </c>
       <c r="B25" s="69" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="17.25" customHeight="1">
@@ -7047,7 +7135,7 @@
         <v>45831</v>
       </c>
       <c r="B26" s="69" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17.25" customHeight="1">
@@ -7055,7 +7143,7 @@
         <v>45838</v>
       </c>
       <c r="B27" s="69" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="17.25" customHeight="1">
@@ -7063,7 +7151,7 @@
         <v>45858</v>
       </c>
       <c r="B28" s="69" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17.25" customHeight="1">
@@ -7071,7 +7159,7 @@
         <v>45876</v>
       </c>
       <c r="B29" s="69" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17.25" customHeight="1">
@@ -7079,7 +7167,7 @@
         <v>45887</v>
       </c>
       <c r="B30" s="69" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17.25" customHeight="1">
@@ -7087,7 +7175,7 @@
         <v>45943</v>
       </c>
       <c r="B31" s="69" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17.25" customHeight="1">
@@ -7095,7 +7183,7 @@
         <v>45964</v>
       </c>
       <c r="B32" s="69" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="17.25" customHeight="1">
@@ -7103,7 +7191,7 @@
         <v>45978</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17.25" customHeight="1">
@@ -7111,7 +7199,7 @@
         <v>45999</v>
       </c>
       <c r="B34" s="69" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17.25" customHeight="1">
@@ -7119,7 +7207,7 @@
         <v>46016</v>
       </c>
       <c r="B35" s="69" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17.25" customHeight="1">
@@ -7127,7 +7215,7 @@
         <v>46023</v>
       </c>
       <c r="B36" s="69" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17.25" customHeight="1">
@@ -7135,7 +7223,7 @@
         <v>46034</v>
       </c>
       <c r="B37" s="69" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="17.25" customHeight="1">
@@ -7143,7 +7231,7 @@
         <v>46104</v>
       </c>
       <c r="B38" s="69" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="17.25" customHeight="1">
@@ -7151,7 +7239,7 @@
         <v>46114</v>
       </c>
       <c r="B39" s="69" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="17.25" customHeight="1">
@@ -7159,7 +7247,7 @@
         <v>46115</v>
       </c>
       <c r="B40" s="69" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="17.25" customHeight="1">
@@ -7167,7 +7255,7 @@
         <v>46143</v>
       </c>
       <c r="B41" s="69" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17.25" customHeight="1">
@@ -7175,7 +7263,7 @@
         <v>46160</v>
       </c>
       <c r="B42" s="69" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="17.25" customHeight="1">
@@ -7183,7 +7271,7 @@
         <v>46181</v>
       </c>
       <c r="B43" s="69" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17.25" customHeight="1">
@@ -7191,7 +7279,7 @@
         <v>46188</v>
       </c>
       <c r="B44" s="69" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="17.25" customHeight="1">
@@ -7199,7 +7287,7 @@
         <v>46202</v>
       </c>
       <c r="B45" s="69" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17.25" customHeight="1">
@@ -7207,7 +7295,7 @@
         <v>46223</v>
       </c>
       <c r="B46" s="69" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17.25" customHeight="1">
@@ -7215,7 +7303,7 @@
         <v>46241</v>
       </c>
       <c r="B47" s="69" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17.25" customHeight="1">
@@ -7223,7 +7311,7 @@
         <v>46251</v>
       </c>
       <c r="B48" s="69" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="17.25" customHeight="1">
@@ -7231,7 +7319,7 @@
         <v>46307</v>
       </c>
       <c r="B49" s="69" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="17.25" customHeight="1">
@@ -7239,7 +7327,7 @@
         <v>46328</v>
       </c>
       <c r="B50" s="69" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="17.25" customHeight="1">
@@ -7247,7 +7335,7 @@
         <v>46342</v>
       </c>
       <c r="B51" s="69" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="17.25" customHeight="1">
@@ -7255,7 +7343,7 @@
         <v>46364</v>
       </c>
       <c r="B52" s="69" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="17.25" customHeight="1">
@@ -7263,7 +7351,7 @@
         <v>46381</v>
       </c>
       <c r="B53" s="69" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="17.25" customHeight="1"/>
@@ -8240,7 +8328,7 @@
   <sheetData>
     <row r="1" spans="1:97" ht="15.75">
       <c r="A1" s="70" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B1" s="71"/>
       <c r="C1" s="71"/>
@@ -8298,7 +8386,7 @@
     </row>
     <row r="3" spans="1:97" ht="32.25" customHeight="1">
       <c r="A3" s="72" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B3" s="73">
         <v>45596</v>
@@ -8591,261 +8679,261 @@
     </row>
     <row r="4" spans="1:97" ht="30.75" customHeight="1">
       <c r="A4" s="76" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B4" s="77" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C4" s="78" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="J4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="L4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="M4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="N4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="O4" s="79" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="P4" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Q4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="R4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="S4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="T4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U4" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="V4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="W4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="X4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Y4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Z4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AA4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AB4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AD4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AE4" s="105" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="AF4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AG4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AH4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AI4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AJ4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AK4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AL4" s="105" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="AM4" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AN4" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AO4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AP4" s="105" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AQ4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AR4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AS4" s="105" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AT4" s="81" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AU4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AV4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AW4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AX4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AY4" s="105" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="AZ4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BA4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BB4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BC4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BD4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BE4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BF4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BG4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BH4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BI4" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BJ4" s="105" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="BK4" s="80" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="BL4" s="80" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="BM4" s="80" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="BN4" s="80" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="BO4" s="80" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="BP4" s="80" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="BQ4" s="80" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="BR4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BS4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BT4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BU4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BV4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BW4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BX4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BY4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BZ4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CA4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CB4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CC4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CD4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CE4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CF4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CG4" s="79"/>
       <c r="CH4" s="79"/>
       <c r="CI4" s="105" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="CJ4" s="79"/>
       <c r="CK4" s="79"/>
@@ -8857,249 +8945,249 @@
       <c r="CQ4" s="79"/>
       <c r="CR4" s="79"/>
       <c r="CS4" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:97" ht="15.75" customHeight="1">
       <c r="A5" s="76" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="B5" s="77" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="J5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="L5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="M5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="N5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="O5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="P5" s="80" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="Q5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="R5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="S5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="T5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U5" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="V5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="W5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="X5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Y5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Z5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AA5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AB5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AD5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AE5" s="106"/>
       <c r="AF5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AG5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AH5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AI5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AJ5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AK5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AL5" s="106"/>
       <c r="AM5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AN5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AO5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AP5" s="106"/>
       <c r="AQ5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="AR5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="AS5" s="106"/>
       <c r="AT5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="AU5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="AV5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="AW5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="AX5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="AY5" s="106"/>
       <c r="AZ5" s="79" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="BA5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BB5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BC5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BD5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BE5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BF5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BG5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BH5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BI5" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BJ5" s="106"/>
       <c r="BK5" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BL5" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BM5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BN5" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BO5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BP5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BQ5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BR5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BS5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BT5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BU5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BV5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BW5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BX5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BY5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BZ5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CA5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CB5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CC5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CD5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CE5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CF5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CG5" s="79"/>
       <c r="CH5" s="79"/>
@@ -9114,249 +9202,249 @@
       <c r="CQ5" s="79"/>
       <c r="CR5" s="79"/>
       <c r="CS5" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:97" ht="15.75">
       <c r="A6" s="76" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B6" s="77" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="J6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K6" s="82" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="L6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="M6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="N6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="O6" s="79" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="P6" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Q6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="R6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="S6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="T6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U6" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="V6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="W6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="X6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Y6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Z6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AA6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AB6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AD6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AE6" s="106"/>
       <c r="AF6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AG6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AH6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AI6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AJ6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AK6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AL6" s="106"/>
       <c r="AM6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AN6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AO6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AP6" s="106"/>
       <c r="AQ6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AR6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AS6" s="106"/>
       <c r="AT6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AU6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AV6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AW6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AX6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AY6" s="106"/>
       <c r="AZ6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BA6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BB6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BC6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BD6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BE6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BF6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BG6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BH6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BI6" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BJ6" s="106"/>
       <c r="BK6" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BL6" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BM6" s="79" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="BN6" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BO6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BP6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BQ6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BR6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BS6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BT6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BU6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BV6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BW6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BX6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BY6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BZ6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CA6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CB6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CC6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CD6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CE6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CF6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CG6" s="79"/>
       <c r="CH6" s="79"/>
@@ -9371,198 +9459,198 @@
       <c r="CQ6" s="79"/>
       <c r="CR6" s="79"/>
       <c r="CS6" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A7" s="76" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B7" s="77" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="J7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="L7" s="82" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="M7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="N7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="O7" s="79" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="P7" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Q7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="R7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="S7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="T7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U7" s="80" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="V7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="W7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="X7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Y7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Z7" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AA7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AB7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AD7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AE7" s="106"/>
       <c r="AF7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AG7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AH7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AI7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AJ7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AK7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AL7" s="106"/>
       <c r="AM7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AN7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AO7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AP7" s="106"/>
       <c r="AQ7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AR7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AS7" s="106"/>
       <c r="AT7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AU7" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AV7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AW7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AX7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AY7" s="106"/>
       <c r="AZ7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BA7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BB7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BC7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BD7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BE7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BF7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BG7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BH7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BI7" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BJ7" s="106"/>
       <c r="BK7" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BL7" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BM7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BN7" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BO7" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BP7" s="79"/>
       <c r="BQ7" s="79"/>
@@ -9570,16 +9658,16 @@
       <c r="BS7" s="79"/>
       <c r="BT7" s="79"/>
       <c r="BU7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BV7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BW7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BX7" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BY7" s="79"/>
       <c r="BZ7" s="79"/>
@@ -9605,220 +9693,220 @@
     </row>
     <row r="8" spans="1:97" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="76" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B8" s="77" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="J8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="L8" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="M8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="N8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="O8" s="79" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="P8" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Q8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="R8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="S8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="T8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U8" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="V8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="W8" s="79" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="X8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Y8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Z8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AA8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AB8" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AC8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AD8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AE8" s="106"/>
       <c r="AF8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AG8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AH8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AI8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AJ8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AK8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AL8" s="106"/>
       <c r="AM8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AN8" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AO8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AP8" s="106"/>
       <c r="AQ8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AR8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AS8" s="106"/>
       <c r="AT8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AU8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AV8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AW8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AX8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AY8" s="106"/>
       <c r="AZ8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BA8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BB8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BC8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BD8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BE8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BF8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BG8" s="79" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="BH8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BI8" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BJ8" s="106"/>
       <c r="BK8" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BL8" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BM8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BN8" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BO8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BP8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BQ8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BR8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BS8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BT8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BU8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BV8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BW8" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BX8" s="79" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="BY8" s="79"/>
       <c r="BZ8" s="79"/>
@@ -9844,244 +9932,244 @@
     </row>
     <row r="9" spans="1:97" ht="15.75">
       <c r="A9" s="76" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B9" s="77" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="J9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="L9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="M9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="N9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="O9" s="82" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="P9" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Q9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="R9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="S9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="T9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U9" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="V9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="W9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="X9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Y9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Z9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AA9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AB9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AD9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AE9" s="106"/>
       <c r="AF9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AG9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AH9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AI9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AJ9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AK9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AL9" s="106"/>
       <c r="AM9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AN9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AO9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AP9" s="106"/>
       <c r="AQ9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AR9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AS9" s="106"/>
       <c r="AT9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AU9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AV9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AW9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AX9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AY9" s="106"/>
       <c r="AZ9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BA9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BB9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BC9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BD9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BE9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BF9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BG9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BH9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BI9" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BJ9" s="106"/>
       <c r="BK9" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BL9" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BM9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BN9" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BO9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BP9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BQ9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BR9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BS9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BT9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BU9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BV9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BW9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BX9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BY9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BZ9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CA9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CB9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CC9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CD9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CE9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CF9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CG9" s="79"/>
       <c r="CH9" s="79"/>
@@ -10096,249 +10184,249 @@
       <c r="CQ9" s="79"/>
       <c r="CR9" s="79"/>
       <c r="CS9" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:97" ht="15.75">
       <c r="A10" s="76" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B10" s="77" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="J10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="L10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="M10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="N10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="O10" s="79" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="P10" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="R10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="S10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="T10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="U10" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="V10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="W10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="X10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Y10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Z10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AA10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AB10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AD10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AE10" s="106"/>
       <c r="AF10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AG10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AH10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AI10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AJ10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AK10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AL10" s="106"/>
       <c r="AM10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AN10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AO10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AP10" s="106"/>
       <c r="AQ10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AR10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AS10" s="106"/>
       <c r="AT10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AU10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AV10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AW10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AX10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AY10" s="106"/>
       <c r="AZ10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BA10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BB10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BC10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BD10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BE10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BF10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BG10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BH10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BI10" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BJ10" s="106"/>
       <c r="BK10" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BL10" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BM10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BN10" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BO10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BP10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BQ10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BR10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BS10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BT10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BU10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BV10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BW10" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BX10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BY10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BZ10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CA10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CB10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CC10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CD10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CE10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CF10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CG10" s="79"/>
       <c r="CH10" s="79"/>
@@ -10353,249 +10441,249 @@
       <c r="CQ10" s="79"/>
       <c r="CR10" s="79"/>
       <c r="CS10" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:97" ht="15.75">
       <c r="A11" s="76" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B11" s="77" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="J11" s="79" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="K11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="L11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="M11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="N11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="O11" s="79" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="P11" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Q11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="R11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="S11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="T11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="U11" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="V11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="W11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="X11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Y11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Z11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AA11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AB11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AC11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AD11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AE11" s="106"/>
       <c r="AF11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AG11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AH11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AI11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AJ11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AK11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AL11" s="106"/>
       <c r="AM11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AN11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AO11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AP11" s="106"/>
       <c r="AQ11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AR11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AS11" s="106"/>
       <c r="AT11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AU11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AV11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AW11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AX11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AY11" s="106"/>
       <c r="AZ11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BA11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BB11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BC11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BD11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BE11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BF11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BG11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BH11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BI11" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BJ11" s="106"/>
       <c r="BK11" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BL11" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BM11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BN11" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BO11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BP11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BQ11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BR11" s="79" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="BS11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BT11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BU11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BV11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BW11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BX11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BY11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BZ11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CA11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CB11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CC11" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CD11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CE11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CF11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CG11" s="79"/>
       <c r="CH11" s="79"/>
@@ -10610,249 +10698,249 @@
       <c r="CQ11" s="79"/>
       <c r="CR11" s="79"/>
       <c r="CS11" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:97" ht="15.75">
       <c r="A12" s="76" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B12" s="77" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="F12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="J12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="L12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="M12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="N12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="O12" s="79" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="P12" s="80" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Q12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="R12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="S12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="T12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="U12" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="V12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="W12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="X12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Y12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Z12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AA12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AB12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AC12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AD12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AE12" s="106"/>
       <c r="AF12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AG12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AH12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AI12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AJ12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AK12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AL12" s="106"/>
       <c r="AM12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AN12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AO12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AP12" s="106"/>
       <c r="AQ12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AR12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AS12" s="106"/>
       <c r="AT12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AU12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AV12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AW12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AX12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AY12" s="106"/>
       <c r="AZ12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BA12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BB12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BC12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BD12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BE12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BF12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BG12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BH12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BI12" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BJ12" s="106"/>
       <c r="BK12" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BL12" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BM12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BN12" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BO12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BP12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BQ12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BR12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BS12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BT12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BU12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BV12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BW12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BX12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BY12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="BZ12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CA12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CB12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CC12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CD12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CE12" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CF12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CG12" s="79"/>
       <c r="CH12" s="79"/>
@@ -10867,249 +10955,249 @@
       <c r="CQ12" s="79"/>
       <c r="CR12" s="79"/>
       <c r="CS12" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:97" ht="15.75">
       <c r="A13" s="76" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B13" s="77" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="C13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="G13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="I13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="J13" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="K13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="L13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="M13" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="N13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="O13" s="79" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="P13" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Q13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="R13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="S13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="T13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="U13" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="V13" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="W13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="X13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Y13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="Z13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AA13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AB13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AC13" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AD13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AE13" s="107"/>
       <c r="AF13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AG13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AH13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AI13" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="AJ13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AK13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AL13" s="107"/>
       <c r="AM13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AN13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AO13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AP13" s="107"/>
       <c r="AQ13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AR13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AS13" s="107"/>
       <c r="AT13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AU13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AV13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AW13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AX13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="AY13" s="107"/>
       <c r="AZ13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BA13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BB13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BC13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BD13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BE13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BF13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BG13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BH13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BI13" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BJ13" s="107"/>
       <c r="BK13" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BL13" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BM13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BN13" s="80" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BO13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BP13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BQ13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BR13" s="79" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="BS13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BT13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BU13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BV13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BW13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BX13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BY13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="BZ13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CA13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CB13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CC13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="CD13" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CE13" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CF13" s="79" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="CG13" s="79"/>
       <c r="CH13" s="79"/>
@@ -11124,7 +11212,7 @@
       <c r="CQ13" s="79"/>
       <c r="CR13" s="79"/>
       <c r="CS13" s="79" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -12146,7 +12234,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="25.5">
       <c r="A1" s="83" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B1" s="83" t="s">
         <v>2</v>
@@ -12173,13 +12261,13 @@
         <v>12</v>
       </c>
       <c r="J1" s="87" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="K1" s="88" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="L1" s="86" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="M1" s="89"/>
       <c r="N1" s="89"/>
@@ -12198,10 +12286,10 @@
     </row>
     <row r="2" spans="1:26" ht="38.25">
       <c r="A2" s="90" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B2" s="91" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C2" s="92"/>
       <c r="D2" s="92" t="s">
@@ -12228,7 +12316,7 @@
       </c>
       <c r="K2" s="95"/>
       <c r="L2" s="96" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="M2" s="89"/>
       <c r="N2" s="89"/>
@@ -12247,13 +12335,13 @@
     </row>
     <row r="3" spans="1:26" ht="51">
       <c r="A3" s="90" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B3" s="108" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C3" s="97" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D3" s="92" t="s">
         <v>39</v>
@@ -12275,7 +12363,7 @@
       </c>
       <c r="K3" s="93"/>
       <c r="L3" s="96" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="M3" s="98"/>
       <c r="N3" s="89"/>
@@ -12294,11 +12382,11 @@
     </row>
     <row r="4" spans="1:26" ht="51">
       <c r="A4" s="90" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B4" s="106"/>
       <c r="C4" s="99" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D4" s="92" t="s">
         <v>39</v>
@@ -12320,7 +12408,7 @@
       </c>
       <c r="K4" s="100"/>
       <c r="L4" s="103" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="M4" s="98"/>
       <c r="N4" s="89"/>
@@ -12339,13 +12427,13 @@
     </row>
     <row r="5" spans="1:26" ht="51">
       <c r="A5" s="90" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B5" s="86" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C5" s="92" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="D5" s="92" t="s">
         <v>39</v>
@@ -12367,7 +12455,7 @@
       </c>
       <c r="K5" s="93"/>
       <c r="L5" s="96" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="M5" s="98"/>
       <c r="N5" s="89"/>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 23 de febrero 2026
</commit_message>
<xml_diff>
--- a/Colmedica.xlsx
+++ b/Colmedica.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="318">
   <si>
     <t>Asignado a</t>
   </si>
@@ -839,7 +839,7 @@
   <si>
     <t>7/01/2026 se hace reunión con el área comercial, para ver mejoras del módulode normalización, y mejorar la revisión de las solicitudes
 5/02/2025 Se revisa documento enviado por el área comercial, para validar los ajustes solicitados para la plataforma de Normalización de Afiliaciones, Se renombfran columnas y eliminan las soliictadas
-6/02/2025 se inicia con la adición de columnas y la modificación en query para obtener l dato</t>
+6/02/2025 se inicia con la adición de columnas y la modificación en query para obtener el dato</t>
   </si>
   <si>
     <t>Afiliaciones Pre - Validación 7 campos</t>
@@ -911,19 +911,20 @@
     <t>Modificar opción de devoluciones por escalas encontradas en la consulta SARLAFT, solo se deben devolver y reportar por correo las solicitude que en su consulta reporten las escalas se reportaran las escalas 1, 2, 5 y 6</t>
   </si>
   <si>
-    <t>17/02/2026 revisar la pagina donde se cargan los soportes de infolat, y se identifican las escalas, para que se pregunte por las escalas 1, 2, 5 y 6, solo para estas se deben generar las devoluciones</t>
+    <t xml:space="preserve">17/02/2026 revisar la pagina donde se cargan los soportes de infolat, y se identifican las escalas, para que se pregunte por las escalas 1, 2, 5 y 6, solo para estas se deben generar las devoluciones
+</t>
   </si>
   <si>
     <t>OPT_40</t>
   </si>
   <si>
-    <t>Afiliaciones POS - Completar descarga de cartas Derechos y Deberes</t>
-  </si>
-  <si>
-    <t>OPT_41</t>
-  </si>
-  <si>
-    <t>Afiliaciones POS - Consumo Puntual de las afiliaciones</t>
+    <t>Afiliaciones PRE - Proceso de anuladas</t>
+  </si>
+  <si>
+    <t>el correo que se envia cada 15 días, ahora se debe ajustar para envío diario de Lunes a viernes, y eliminar la macrcación que se hacia para enviarla los miercoles cada 15 días</t>
+  </si>
+  <si>
+    <t>18/02/2026 Se ajusta la tarea programada, para enviar el correo todos los días de lunes a viernes. y dentro del codigo se elimina la marca que se hacia para identificar que miercoles si se enviaba y que miercoles no</t>
   </si>
   <si>
     <t xml:space="preserve"> Año Nuevo</t>
@@ -1188,9 +1189,6 @@
   </si>
   <si>
     <t>Internal Server Error</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
 </sst>
 </file>
@@ -1678,7 +1676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1954,7 +1952,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2182,11 +2179,11 @@
   <sheetPr>
     <tabColor rgb="FF93C47D"/>
   </sheetPr>
-  <dimension ref="A1:AN62"/>
+  <dimension ref="A1:AN61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2720,7 +2717,7 @@
       <c r="L7" s="43"/>
       <c r="M7" s="50">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>32891</v>
+        <v>32894</v>
       </c>
       <c r="N7" s="43"/>
       <c r="O7" s="43"/>
@@ -3107,7 +3104,7 @@
       NETWORKDAYS(J12,L12,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="N12" s="28"/>
       <c r="O12" s="28"/>
@@ -3895,7 +3892,7 @@
       NETWORKDAYS(J22,L22,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="N22" s="28"/>
       <c r="O22" s="28"/>
@@ -4049,7 +4046,7 @@
       NETWORKDAYS(J24,L24,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="N24" s="28"/>
       <c r="O24" s="28"/>
@@ -4353,7 +4350,7 @@
       NETWORKDAYS(J28,L28,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="N28" s="28"/>
       <c r="O28" s="28"/>
@@ -4833,7 +4830,7 @@
       NETWORKDAYS(J34,L34,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="N34" s="28"/>
       <c r="O34" s="28"/>
@@ -4908,7 +4905,7 @@
       NETWORKDAYS(J35,L35,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="N35" s="43"/>
       <c r="O35" s="43">
@@ -4987,7 +4984,7 @@
       NETWORKDAYS(J36,L36,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="N36" s="28"/>
       <c r="O36" s="28">
@@ -5066,7 +5063,7 @@
       NETWORKDAYS(J37,L37,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N37" s="43"/>
       <c r="O37" s="43">
@@ -5143,7 +5140,7 @@
       NETWORKDAYS(J38,L38,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="N38" s="28"/>
       <c r="O38" s="28"/>
@@ -5289,7 +5286,7 @@
       NETWORKDAYS(J40,L40,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="N40" s="28"/>
       <c r="O40" s="28">
@@ -5368,7 +5365,7 @@
       NETWORKDAYS(J41,L41,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="N41" s="43"/>
       <c r="O41" s="43">
@@ -5433,7 +5430,7 @@
       <c r="L42" s="28"/>
       <c r="M42" s="64">
         <f ca="1">IF(ISBLANK(L42), NETWORKDAYS(J42, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J42, L42, Hoja2!$A$1:$A$18))</f>
-        <v>32891</v>
+        <v>32894</v>
       </c>
       <c r="N42" s="28"/>
       <c r="O42" s="28"/>
@@ -5506,7 +5503,7 @@
       NETWORKDAYS(J43,L43,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="N43" s="43"/>
       <c r="O43" s="43">
@@ -5794,7 +5791,7 @@
       <c r="L47" s="43"/>
       <c r="M47" s="50">
         <f ca="1">IF(ISBLANK(L47), NETWORKDAYS(J47, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J47, L47, Hoja2!$A$1:$A$18))</f>
-        <v>32891</v>
+        <v>32894</v>
       </c>
       <c r="N47" s="43"/>
       <c r="O47" s="43"/>
@@ -5855,7 +5852,7 @@
       <c r="L48" s="28"/>
       <c r="M48" s="64">
         <f ca="1">IF(ISBLANK(L48), NETWORKDAYS(J48, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J48, L48, Hoja2!$A$1:$A$18))</f>
-        <v>32891</v>
+        <v>32894</v>
       </c>
       <c r="N48" s="28"/>
       <c r="O48" s="28"/>
@@ -5914,7 +5911,7 @@
       <c r="L49" s="43"/>
       <c r="M49" s="50">
         <f ca="1">IF(ISBLANK(L49), NETWORKDAYS(J49, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J49, L49, Hoja2!$A$1:$A$18))</f>
-        <v>32891</v>
+        <v>32894</v>
       </c>
       <c r="N49" s="43"/>
       <c r="O49" s="43"/>
@@ -6207,11 +6204,11 @@
         <v>119</v>
       </c>
       <c r="G53" s="38">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="H53" s="39">
         <f>IF(OR(J53="",K53="",K53&lt;J53),0,NETWORKDAYS(J53,K53,Hoja2!$A$2:$A$53))</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I53" s="40">
         <v>46029</v>
@@ -6220,7 +6217,7 @@
         <v>46058</v>
       </c>
       <c r="K53" s="41">
-        <v>46066</v>
+        <v>46073</v>
       </c>
       <c r="L53" s="41"/>
       <c r="M53" s="42">
@@ -6230,7 +6227,7 @@
       NETWORKDAYS(J53,L53,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="N53" s="43"/>
       <c r="O53" s="43"/>
@@ -6305,7 +6302,7 @@
       NETWORKDAYS(J54,L54,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="N54" s="28"/>
       <c r="O54" s="28">
@@ -6384,7 +6381,7 @@
       NETWORKDAYS(J55,L55,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="N55" s="43"/>
       <c r="O55" s="43">
@@ -6461,7 +6458,7 @@
       NETWORKDAYS(J56,L56,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="N56" s="28"/>
       <c r="O56" s="28"/>
@@ -6599,7 +6596,7 @@
       NETWORKDAYS(J58,L58,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N58" s="28"/>
       <c r="O58" s="28">
@@ -6717,10 +6714,10 @@
       </c>
       <c r="E60" s="21"/>
       <c r="F60" s="22" t="s">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="G60" s="23">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="H60" s="24">
         <f>IF(OR(J60="",K60="",K60&lt;J60),0,NETWORKDAYS(J60,K60,Hoja2!$A$2:$A$53))</f>
@@ -6743,11 +6740,15 @@
       NETWORKDAYS(J60,L60,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N60" s="28"/>
-      <c r="O60" s="28"/>
-      <c r="P60" s="28"/>
+      <c r="O60" s="28">
+        <v>46071</v>
+      </c>
+      <c r="P60" s="28">
+        <v>46071</v>
+      </c>
       <c r="Q60" s="29" t="s">
         <v>233</v>
       </c>
@@ -6777,7 +6778,7 @@
       <c r="AM60" s="59"/>
       <c r="AN60" s="60"/>
     </row>
-    <row r="61" spans="1:40" ht="57">
+    <row r="61" spans="1:40" ht="28.5">
       <c r="A61" s="32" t="s">
         <v>36</v>
       </c>
@@ -6787,17 +6788,29 @@
       <c r="C61" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="D61" s="35"/>
+      <c r="D61" s="35" t="s">
+        <v>236</v>
+      </c>
       <c r="E61" s="36"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="38"/>
+      <c r="F61" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="G61" s="38">
+        <v>100</v>
+      </c>
       <c r="H61" s="39">
         <f>IF(OR(J61="",K61="",K61&lt;J61),0,NETWORKDAYS(J61,K61,Hoja2!$A$2:$A$53))</f>
-        <v>0</v>
-      </c>
-      <c r="I61" s="40"/>
-      <c r="J61" s="40"/>
-      <c r="K61" s="41"/>
+        <v>1</v>
+      </c>
+      <c r="I61" s="40">
+        <v>46071</v>
+      </c>
+      <c r="J61" s="40">
+        <v>46071</v>
+      </c>
+      <c r="K61" s="41">
+        <v>46071</v>
+      </c>
       <c r="L61" s="41"/>
       <c r="M61" s="42">
         <f ca="1">IF(OR(J61="",AND(L61="",TODAY()&lt;J61),AND(L61&lt;&gt;"",L61&lt;J61)),0,
@@ -6806,14 +6819,20 @@
       NETWORKDAYS(J61,L61,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N61" s="43"/>
-      <c r="O61" s="43"/>
-      <c r="P61" s="43"/>
-      <c r="Q61" s="44"/>
-      <c r="R61" s="109" t="s">
-        <v>318</v>
+      <c r="O61" s="43">
+        <v>46071</v>
+      </c>
+      <c r="P61" s="43">
+        <v>46071</v>
+      </c>
+      <c r="Q61" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="R61" s="45" t="s">
+        <v>45</v>
       </c>
       <c r="S61" s="57"/>
       <c r="T61" s="57"/>
@@ -6838,79 +6857,18 @@
       <c r="AM61" s="57"/>
       <c r="AN61" s="58"/>
     </row>
-    <row r="62" spans="1:40" ht="42.75">
-      <c r="A62" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="22"/>
-      <c r="G62" s="23"/>
-      <c r="H62" s="24">
-        <f>IF(OR(J62="",K62="",K62&lt;J62),0,NETWORKDAYS(J62,K62,Hoja2!$A$2:$A$53))</f>
-        <v>0</v>
-      </c>
-      <c r="I62" s="25"/>
-      <c r="J62" s="25"/>
-      <c r="K62" s="26"/>
-      <c r="L62" s="26"/>
-      <c r="M62" s="27">
-        <f ca="1">IF(OR(J62="",AND(L62="",TODAY()&lt;J62),AND(L62&lt;&gt;"",L62&lt;J62)),0,
-   IF(L62="",
-      NETWORKDAYS(J62,TODAY(),Hoja2!$A$2:$A$53),
-      NETWORKDAYS(J62,L62,Hoja2!$A$2:$A$53)
-   )
-)</f>
-        <v>0</v>
-      </c>
-      <c r="N62" s="28"/>
-      <c r="O62" s="28"/>
-      <c r="P62" s="28"/>
-      <c r="Q62" s="29"/>
-      <c r="R62" s="109" t="s">
-        <v>318</v>
-      </c>
-      <c r="S62" s="59"/>
-      <c r="T62" s="59"/>
-      <c r="U62" s="59"/>
-      <c r="V62" s="59"/>
-      <c r="W62" s="59"/>
-      <c r="X62" s="59"/>
-      <c r="Y62" s="59"/>
-      <c r="Z62" s="59"/>
-      <c r="AA62" s="59"/>
-      <c r="AB62" s="59"/>
-      <c r="AC62" s="59"/>
-      <c r="AD62" s="59"/>
-      <c r="AE62" s="59"/>
-      <c r="AF62" s="59"/>
-      <c r="AG62" s="59"/>
-      <c r="AH62" s="59"/>
-      <c r="AI62" s="59"/>
-      <c r="AJ62" s="59"/>
-      <c r="AK62" s="59"/>
-      <c r="AL62" s="59"/>
-      <c r="AM62" s="59"/>
-      <c r="AN62" s="60"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:R61"/>
-  <conditionalFormatting sqref="B8:B62">
+  <conditionalFormatting sqref="B8:B61">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>COUNTIF(B8:B62, B8)&gt;1</formula>
+      <formula>COUNTIF(B8:B61, B8)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="F2:F62">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F61">
       <formula1>"FINALIZADO,EN PROCESO,PAUSADO,EN TEST,PENDIENTE,PRUEBAS CLIENTE,PRUEBAS IMAGINE,PASO A PRODUCCION"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L26 N2:P26 I27 I28:L62 N28:P62">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="I2:L26 N2:P26 I27 I28:L61 N28:P61">
       <formula1>OR(NOT(ISERROR(DATEVALUE(I2))), AND(ISNUMBER(I2), LEFT(CELL("format", I2))="D"))</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>